<commit_message>
Update spanish export templates
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/courselist-enhanced.xlsx
+++ b/src/spz/templates/export/courselist-enhanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Tims\Code\Workspace\SPZ\git\src\spz\spz\templates\export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiasdierich/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E14B9AF-C940-4937-A6A2-D8664047F9C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F353F99A-3958-8B4E-B73A-8A9270567995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="11" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="Paricipantlist" sheetId="12" r:id="rId5"/>
     <sheet name="Teilnehmer" sheetId="13" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="kursname">Notenliste!$A$52:$A$60</definedName>
+    <definedName name="semester">Notenliste!$D$52:$D$62</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -256,6 +260,9 @@
   </si>
   <si>
     <t>Arabisch 1</t>
+  </si>
+  <si>
+    <t>Alaa Khalil</t>
   </si>
   <si>
     <t>A1</t>
@@ -792,10 +799,40 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="19">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -808,7 +845,7 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -837,36 +874,6 @@
     <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -888,7 +895,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1138,47 +1145,47 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{90DB29BF-3DDC-4EF7-A672-2F2A72667EA5}" name="DATA" displayName="DATA" ref="B1:G2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="B1:G2" xr:uid="{97F12B18-54F3-4E51-933A-952CCD914FD4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB3762C0-B84C-7842-884D-F1AF8DEB89A7}" name="DATA" displayName="DATA" ref="B1:G2" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="B1:G2" xr:uid="{CC3A94DF-ED58-BC4D-81B4-531D123D1578}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{2E80D315-055A-465C-9B05-7462CA515BD8}" name="Nachname" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{725B7483-B755-4DB1-A356-072DE17BFCB0}" name="Vorname" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{DB668D32-F5A3-4D25-90AB-A757726B27B7}" name="Hochschule" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{509ABD6A-9BBF-420E-B1D2-5C10E5281587}" name="Matrikelnummer" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{D36E8D60-8FD8-4EDD-8941-F0E2AA90F88D}" name="E-Mail" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{BB962A67-0999-48D8-9885-DAC3DC5AC302}" name="Telefon" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{0C760751-8195-ED40-BAD1-1742CEDD2F2A}" name="Nachname" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{D514A574-7540-8D48-AA1C-519DDA696DBD}" name="Vorname" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{9DDCA179-D1CF-BD4C-A77C-AADB4AE9A4AE}" name="Hochschule" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{3FDFBCBF-BABE-7240-8A25-C665ECC07111}" name="Matrikelnummer" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1844E8D5-5CA1-8448-8686-148586CBBBFC}" name="E-Mail" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{E23CCDE5-D5A2-6149-A990-1E8F99CDA73B}" name="Telefon" dataDxfId="2"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Teilnehmerliste" displayName="Teilnehmerliste" ref="A1:H36" totalsRowShown="0" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:H36" totalsRowShown="0" dataDxfId="18">
   <autoFilter ref="A1:H36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Matrikelnummer" dataDxfId="9" totalsRowDxfId="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Matrikelnummer" dataDxfId="17" totalsRowDxfId="16">
       <calculatedColumnFormula>IF(Notenliste!D2=0," ",Notenliste!D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Status" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="LP" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Status" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="LP" dataDxfId="14">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$43," ")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Note" dataDxfId="5" totalsRowDxfId="4">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Note" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",Notenliste!F2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Datum" dataDxfId="3">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Datum" dataDxfId="11">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$48," ")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Individueller Titel deutsch" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Individueller Titel englisch" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Anmerkungen" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Individueller Titel deutsch" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Individueller Titel englisch" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Anmerkungen" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1500,25 +1507,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.68359375" style="44" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.41796875" style="44" customWidth="1"/>
-    <col min="3" max="3" width="26.15625" style="44" customWidth="1"/>
-    <col min="4" max="4" width="13.15625" style="44" customWidth="1"/>
-    <col min="5" max="5" width="17.83984375" style="45" customWidth="1"/>
-    <col min="6" max="6" width="31.83984375" style="44" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.83984375" style="44" customWidth="1"/>
-    <col min="8" max="8" width="45.15625" style="44" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.41796875" style="44" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.41796875" hidden="1"/>
+    <col min="1" max="1" width="3.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5" style="44" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" style="44" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="44" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="45" customWidth="1"/>
+    <col min="6" max="6" width="31.83203125" style="44" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.83203125" style="44" customWidth="1"/>
+    <col min="8" max="8" width="45.1640625" style="44" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="44" hidden="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="42" t="s">
         <v>26</v>
       </c>
@@ -1547,33 +1554,33 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="21">
         <v>1</v>
       </c>
       <c r="B2" s="44" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D2" s="44" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E2" s="44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" s="44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G2" s="44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H2" s="44" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="21">
         <v>2</v>
       </c>
@@ -1582,7 +1589,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="21">
         <v>3</v>
       </c>
@@ -1591,7 +1598,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>4</v>
       </c>
@@ -1600,7 +1607,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="21">
         <v>5</v>
       </c>
@@ -1609,7 +1616,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="21">
         <v>6</v>
       </c>
@@ -1618,7 +1625,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="21">
         <v>7</v>
       </c>
@@ -1627,7 +1634,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="21">
         <v>8</v>
       </c>
@@ -1636,7 +1643,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="21">
         <v>9</v>
       </c>
@@ -1645,7 +1652,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="21">
         <v>10</v>
       </c>
@@ -1654,7 +1661,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="21">
         <v>11</v>
       </c>
@@ -1663,7 +1670,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="21">
         <v>12</v>
       </c>
@@ -1672,7 +1679,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="21">
         <v>13</v>
       </c>
@@ -1681,7 +1688,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
         <v>14</v>
       </c>
@@ -1690,7 +1697,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="21">
         <v>15</v>
       </c>
@@ -1699,7 +1706,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="21">
         <v>16</v>
       </c>
@@ -1708,7 +1715,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="21">
         <v>17</v>
       </c>
@@ -1717,7 +1724,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="21">
         <v>18</v>
       </c>
@@ -1726,7 +1733,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="21">
         <v>19</v>
       </c>
@@ -1735,7 +1742,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
         <v>20</v>
       </c>
@@ -1744,7 +1751,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>21</v>
       </c>
@@ -1753,7 +1760,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="21">
         <v>22</v>
       </c>
@@ -1762,7 +1769,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="21">
         <v>23</v>
       </c>
@@ -1771,68 +1778,68 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="21">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="21">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="21">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="21">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="21">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" s="21">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" s="21">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" s="21">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" s="21">
         <v>35</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" formatColumns="0" selectLockedCells="1"/>
+  <sheetProtection formatColumns="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1847,549 +1854,549 @@
   </sheetPr>
   <dimension ref="A1:WVW71"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="12.3" zeroHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="13" zeroHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23.68359375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" style="3" customWidth="1"/>
     <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.26171875" style="12" customWidth="1"/>
-    <col min="6" max="6" width="16.83984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.68359375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="5.68359375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.68359375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.68359375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="2.68359375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="2.6640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="3" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.41796875" style="1" hidden="1"/>
-    <col min="14" max="14" width="5.15625" style="1" hidden="1"/>
-    <col min="15" max="15" width="6.83984375" style="2" hidden="1"/>
-    <col min="16" max="16" width="17.68359375" style="1" hidden="1"/>
+    <col min="13" max="13" width="6.5" style="1" hidden="1"/>
+    <col min="14" max="14" width="5.1640625" style="1" hidden="1"/>
+    <col min="15" max="15" width="6.83203125" style="2" hidden="1"/>
+    <col min="16" max="16" width="17.6640625" style="1" hidden="1"/>
     <col min="17" max="17" width="16" style="1" hidden="1"/>
-    <col min="18" max="18" width="17.68359375" style="1" hidden="1"/>
-    <col min="19" max="243" width="11.41796875" style="1" hidden="1"/>
-    <col min="244" max="244" width="15.41796875" style="1" hidden="1"/>
-    <col min="245" max="245" width="11.41796875" style="1" hidden="1"/>
-    <col min="246" max="246" width="15.68359375" style="1" hidden="1"/>
-    <col min="247" max="247" width="21.83984375" style="1" hidden="1"/>
-    <col min="248" max="250" width="11.41796875" style="1" hidden="1"/>
+    <col min="18" max="18" width="17.6640625" style="1" hidden="1"/>
+    <col min="19" max="243" width="11.5" style="1" hidden="1"/>
+    <col min="244" max="244" width="15.5" style="1" hidden="1"/>
+    <col min="245" max="245" width="11.5" style="1" hidden="1"/>
+    <col min="246" max="246" width="15.6640625" style="1" hidden="1"/>
+    <col min="247" max="247" width="21.83203125" style="1" hidden="1"/>
+    <col min="248" max="250" width="11.5" style="1" hidden="1"/>
     <col min="251" max="251" width="16" style="1" hidden="1"/>
-    <col min="252" max="252" width="20.41796875" style="1" hidden="1"/>
-    <col min="253" max="499" width="11.41796875" style="1" hidden="1"/>
-    <col min="500" max="500" width="15.41796875" style="1" hidden="1"/>
-    <col min="501" max="501" width="11.41796875" style="1" hidden="1"/>
-    <col min="502" max="502" width="15.68359375" style="1" hidden="1"/>
-    <col min="503" max="503" width="21.83984375" style="1" hidden="1"/>
-    <col min="504" max="506" width="11.41796875" style="1" hidden="1"/>
+    <col min="252" max="252" width="20.5" style="1" hidden="1"/>
+    <col min="253" max="499" width="11.5" style="1" hidden="1"/>
+    <col min="500" max="500" width="15.5" style="1" hidden="1"/>
+    <col min="501" max="501" width="11.5" style="1" hidden="1"/>
+    <col min="502" max="502" width="15.6640625" style="1" hidden="1"/>
+    <col min="503" max="503" width="21.83203125" style="1" hidden="1"/>
+    <col min="504" max="506" width="11.5" style="1" hidden="1"/>
     <col min="507" max="507" width="16" style="1" hidden="1"/>
-    <col min="508" max="508" width="20.41796875" style="1" hidden="1"/>
-    <col min="509" max="755" width="11.41796875" style="1" hidden="1"/>
-    <col min="756" max="756" width="15.41796875" style="1" hidden="1"/>
-    <col min="757" max="757" width="11.41796875" style="1" hidden="1"/>
-    <col min="758" max="758" width="15.68359375" style="1" hidden="1"/>
-    <col min="759" max="759" width="21.83984375" style="1" hidden="1"/>
-    <col min="760" max="762" width="11.41796875" style="1" hidden="1"/>
+    <col min="508" max="508" width="20.5" style="1" hidden="1"/>
+    <col min="509" max="755" width="11.5" style="1" hidden="1"/>
+    <col min="756" max="756" width="15.5" style="1" hidden="1"/>
+    <col min="757" max="757" width="11.5" style="1" hidden="1"/>
+    <col min="758" max="758" width="15.6640625" style="1" hidden="1"/>
+    <col min="759" max="759" width="21.83203125" style="1" hidden="1"/>
+    <col min="760" max="762" width="11.5" style="1" hidden="1"/>
     <col min="763" max="763" width="16" style="1" hidden="1"/>
-    <col min="764" max="764" width="20.41796875" style="1" hidden="1"/>
-    <col min="765" max="1011" width="11.41796875" style="1" hidden="1"/>
-    <col min="1012" max="1012" width="15.41796875" style="1" hidden="1"/>
-    <col min="1013" max="1013" width="11.41796875" style="1" hidden="1"/>
-    <col min="1014" max="1014" width="15.68359375" style="1" hidden="1"/>
-    <col min="1015" max="1015" width="21.83984375" style="1" hidden="1"/>
-    <col min="1016" max="1018" width="11.41796875" style="1" hidden="1"/>
+    <col min="764" max="764" width="20.5" style="1" hidden="1"/>
+    <col min="765" max="1011" width="11.5" style="1" hidden="1"/>
+    <col min="1012" max="1012" width="15.5" style="1" hidden="1"/>
+    <col min="1013" max="1013" width="11.5" style="1" hidden="1"/>
+    <col min="1014" max="1014" width="15.6640625" style="1" hidden="1"/>
+    <col min="1015" max="1015" width="21.83203125" style="1" hidden="1"/>
+    <col min="1016" max="1018" width="11.5" style="1" hidden="1"/>
     <col min="1019" max="1019" width="16" style="1" hidden="1"/>
-    <col min="1020" max="1020" width="20.41796875" style="1" hidden="1"/>
-    <col min="1021" max="1267" width="11.41796875" style="1" hidden="1"/>
-    <col min="1268" max="1268" width="15.41796875" style="1" hidden="1"/>
-    <col min="1269" max="1269" width="11.41796875" style="1" hidden="1"/>
-    <col min="1270" max="1270" width="15.68359375" style="1" hidden="1"/>
-    <col min="1271" max="1271" width="21.83984375" style="1" hidden="1"/>
-    <col min="1272" max="1274" width="11.41796875" style="1" hidden="1"/>
+    <col min="1020" max="1020" width="20.5" style="1" hidden="1"/>
+    <col min="1021" max="1267" width="11.5" style="1" hidden="1"/>
+    <col min="1268" max="1268" width="15.5" style="1" hidden="1"/>
+    <col min="1269" max="1269" width="11.5" style="1" hidden="1"/>
+    <col min="1270" max="1270" width="15.6640625" style="1" hidden="1"/>
+    <col min="1271" max="1271" width="21.83203125" style="1" hidden="1"/>
+    <col min="1272" max="1274" width="11.5" style="1" hidden="1"/>
     <col min="1275" max="1275" width="16" style="1" hidden="1"/>
-    <col min="1276" max="1276" width="20.41796875" style="1" hidden="1"/>
-    <col min="1277" max="1523" width="11.41796875" style="1" hidden="1"/>
-    <col min="1524" max="1524" width="15.41796875" style="1" hidden="1"/>
-    <col min="1525" max="1525" width="11.41796875" style="1" hidden="1"/>
-    <col min="1526" max="1526" width="15.68359375" style="1" hidden="1"/>
-    <col min="1527" max="1527" width="21.83984375" style="1" hidden="1"/>
-    <col min="1528" max="1530" width="11.41796875" style="1" hidden="1"/>
+    <col min="1276" max="1276" width="20.5" style="1" hidden="1"/>
+    <col min="1277" max="1523" width="11.5" style="1" hidden="1"/>
+    <col min="1524" max="1524" width="15.5" style="1" hidden="1"/>
+    <col min="1525" max="1525" width="11.5" style="1" hidden="1"/>
+    <col min="1526" max="1526" width="15.6640625" style="1" hidden="1"/>
+    <col min="1527" max="1527" width="21.83203125" style="1" hidden="1"/>
+    <col min="1528" max="1530" width="11.5" style="1" hidden="1"/>
     <col min="1531" max="1531" width="16" style="1" hidden="1"/>
-    <col min="1532" max="1532" width="20.41796875" style="1" hidden="1"/>
-    <col min="1533" max="1779" width="11.41796875" style="1" hidden="1"/>
-    <col min="1780" max="1780" width="15.41796875" style="1" hidden="1"/>
-    <col min="1781" max="1781" width="11.41796875" style="1" hidden="1"/>
-    <col min="1782" max="1782" width="15.68359375" style="1" hidden="1"/>
-    <col min="1783" max="1783" width="21.83984375" style="1" hidden="1"/>
-    <col min="1784" max="1786" width="11.41796875" style="1" hidden="1"/>
+    <col min="1532" max="1532" width="20.5" style="1" hidden="1"/>
+    <col min="1533" max="1779" width="11.5" style="1" hidden="1"/>
+    <col min="1780" max="1780" width="15.5" style="1" hidden="1"/>
+    <col min="1781" max="1781" width="11.5" style="1" hidden="1"/>
+    <col min="1782" max="1782" width="15.6640625" style="1" hidden="1"/>
+    <col min="1783" max="1783" width="21.83203125" style="1" hidden="1"/>
+    <col min="1784" max="1786" width="11.5" style="1" hidden="1"/>
     <col min="1787" max="1787" width="16" style="1" hidden="1"/>
-    <col min="1788" max="1788" width="20.41796875" style="1" hidden="1"/>
-    <col min="1789" max="2035" width="11.41796875" style="1" hidden="1"/>
-    <col min="2036" max="2036" width="15.41796875" style="1" hidden="1"/>
-    <col min="2037" max="2037" width="11.41796875" style="1" hidden="1"/>
-    <col min="2038" max="2038" width="15.68359375" style="1" hidden="1"/>
-    <col min="2039" max="2039" width="21.83984375" style="1" hidden="1"/>
-    <col min="2040" max="2042" width="11.41796875" style="1" hidden="1"/>
+    <col min="1788" max="1788" width="20.5" style="1" hidden="1"/>
+    <col min="1789" max="2035" width="11.5" style="1" hidden="1"/>
+    <col min="2036" max="2036" width="15.5" style="1" hidden="1"/>
+    <col min="2037" max="2037" width="11.5" style="1" hidden="1"/>
+    <col min="2038" max="2038" width="15.6640625" style="1" hidden="1"/>
+    <col min="2039" max="2039" width="21.83203125" style="1" hidden="1"/>
+    <col min="2040" max="2042" width="11.5" style="1" hidden="1"/>
     <col min="2043" max="2043" width="16" style="1" hidden="1"/>
-    <col min="2044" max="2044" width="20.41796875" style="1" hidden="1"/>
-    <col min="2045" max="2291" width="11.41796875" style="1" hidden="1"/>
-    <col min="2292" max="2292" width="15.41796875" style="1" hidden="1"/>
-    <col min="2293" max="2293" width="11.41796875" style="1" hidden="1"/>
-    <col min="2294" max="2294" width="15.68359375" style="1" hidden="1"/>
-    <col min="2295" max="2295" width="21.83984375" style="1" hidden="1"/>
-    <col min="2296" max="2298" width="11.41796875" style="1" hidden="1"/>
+    <col min="2044" max="2044" width="20.5" style="1" hidden="1"/>
+    <col min="2045" max="2291" width="11.5" style="1" hidden="1"/>
+    <col min="2292" max="2292" width="15.5" style="1" hidden="1"/>
+    <col min="2293" max="2293" width="11.5" style="1" hidden="1"/>
+    <col min="2294" max="2294" width="15.6640625" style="1" hidden="1"/>
+    <col min="2295" max="2295" width="21.83203125" style="1" hidden="1"/>
+    <col min="2296" max="2298" width="11.5" style="1" hidden="1"/>
     <col min="2299" max="2299" width="16" style="1" hidden="1"/>
-    <col min="2300" max="2300" width="20.41796875" style="1" hidden="1"/>
-    <col min="2301" max="2547" width="11.41796875" style="1" hidden="1"/>
-    <col min="2548" max="2548" width="15.41796875" style="1" hidden="1"/>
-    <col min="2549" max="2549" width="11.41796875" style="1" hidden="1"/>
-    <col min="2550" max="2550" width="15.68359375" style="1" hidden="1"/>
-    <col min="2551" max="2551" width="21.83984375" style="1" hidden="1"/>
-    <col min="2552" max="2554" width="11.41796875" style="1" hidden="1"/>
+    <col min="2300" max="2300" width="20.5" style="1" hidden="1"/>
+    <col min="2301" max="2547" width="11.5" style="1" hidden="1"/>
+    <col min="2548" max="2548" width="15.5" style="1" hidden="1"/>
+    <col min="2549" max="2549" width="11.5" style="1" hidden="1"/>
+    <col min="2550" max="2550" width="15.6640625" style="1" hidden="1"/>
+    <col min="2551" max="2551" width="21.83203125" style="1" hidden="1"/>
+    <col min="2552" max="2554" width="11.5" style="1" hidden="1"/>
     <col min="2555" max="2555" width="16" style="1" hidden="1"/>
-    <col min="2556" max="2556" width="20.41796875" style="1" hidden="1"/>
-    <col min="2557" max="2803" width="11.41796875" style="1" hidden="1"/>
-    <col min="2804" max="2804" width="15.41796875" style="1" hidden="1"/>
-    <col min="2805" max="2805" width="11.41796875" style="1" hidden="1"/>
-    <col min="2806" max="2806" width="15.68359375" style="1" hidden="1"/>
-    <col min="2807" max="2807" width="21.83984375" style="1" hidden="1"/>
-    <col min="2808" max="2810" width="11.41796875" style="1" hidden="1"/>
+    <col min="2556" max="2556" width="20.5" style="1" hidden="1"/>
+    <col min="2557" max="2803" width="11.5" style="1" hidden="1"/>
+    <col min="2804" max="2804" width="15.5" style="1" hidden="1"/>
+    <col min="2805" max="2805" width="11.5" style="1" hidden="1"/>
+    <col min="2806" max="2806" width="15.6640625" style="1" hidden="1"/>
+    <col min="2807" max="2807" width="21.83203125" style="1" hidden="1"/>
+    <col min="2808" max="2810" width="11.5" style="1" hidden="1"/>
     <col min="2811" max="2811" width="16" style="1" hidden="1"/>
-    <col min="2812" max="2812" width="20.41796875" style="1" hidden="1"/>
-    <col min="2813" max="3059" width="11.41796875" style="1" hidden="1"/>
-    <col min="3060" max="3060" width="15.41796875" style="1" hidden="1"/>
-    <col min="3061" max="3061" width="11.41796875" style="1" hidden="1"/>
-    <col min="3062" max="3062" width="15.68359375" style="1" hidden="1"/>
-    <col min="3063" max="3063" width="21.83984375" style="1" hidden="1"/>
-    <col min="3064" max="3066" width="11.41796875" style="1" hidden="1"/>
+    <col min="2812" max="2812" width="20.5" style="1" hidden="1"/>
+    <col min="2813" max="3059" width="11.5" style="1" hidden="1"/>
+    <col min="3060" max="3060" width="15.5" style="1" hidden="1"/>
+    <col min="3061" max="3061" width="11.5" style="1" hidden="1"/>
+    <col min="3062" max="3062" width="15.6640625" style="1" hidden="1"/>
+    <col min="3063" max="3063" width="21.83203125" style="1" hidden="1"/>
+    <col min="3064" max="3066" width="11.5" style="1" hidden="1"/>
     <col min="3067" max="3067" width="16" style="1" hidden="1"/>
-    <col min="3068" max="3068" width="20.41796875" style="1" hidden="1"/>
-    <col min="3069" max="3315" width="11.41796875" style="1" hidden="1"/>
-    <col min="3316" max="3316" width="15.41796875" style="1" hidden="1"/>
-    <col min="3317" max="3317" width="11.41796875" style="1" hidden="1"/>
-    <col min="3318" max="3318" width="15.68359375" style="1" hidden="1"/>
-    <col min="3319" max="3319" width="21.83984375" style="1" hidden="1"/>
-    <col min="3320" max="3322" width="11.41796875" style="1" hidden="1"/>
+    <col min="3068" max="3068" width="20.5" style="1" hidden="1"/>
+    <col min="3069" max="3315" width="11.5" style="1" hidden="1"/>
+    <col min="3316" max="3316" width="15.5" style="1" hidden="1"/>
+    <col min="3317" max="3317" width="11.5" style="1" hidden="1"/>
+    <col min="3318" max="3318" width="15.6640625" style="1" hidden="1"/>
+    <col min="3319" max="3319" width="21.83203125" style="1" hidden="1"/>
+    <col min="3320" max="3322" width="11.5" style="1" hidden="1"/>
     <col min="3323" max="3323" width="16" style="1" hidden="1"/>
-    <col min="3324" max="3324" width="20.41796875" style="1" hidden="1"/>
-    <col min="3325" max="3571" width="11.41796875" style="1" hidden="1"/>
-    <col min="3572" max="3572" width="15.41796875" style="1" hidden="1"/>
-    <col min="3573" max="3573" width="11.41796875" style="1" hidden="1"/>
-    <col min="3574" max="3574" width="15.68359375" style="1" hidden="1"/>
-    <col min="3575" max="3575" width="21.83984375" style="1" hidden="1"/>
-    <col min="3576" max="3578" width="11.41796875" style="1" hidden="1"/>
+    <col min="3324" max="3324" width="20.5" style="1" hidden="1"/>
+    <col min="3325" max="3571" width="11.5" style="1" hidden="1"/>
+    <col min="3572" max="3572" width="15.5" style="1" hidden="1"/>
+    <col min="3573" max="3573" width="11.5" style="1" hidden="1"/>
+    <col min="3574" max="3574" width="15.6640625" style="1" hidden="1"/>
+    <col min="3575" max="3575" width="21.83203125" style="1" hidden="1"/>
+    <col min="3576" max="3578" width="11.5" style="1" hidden="1"/>
     <col min="3579" max="3579" width="16" style="1" hidden="1"/>
-    <col min="3580" max="3580" width="20.41796875" style="1" hidden="1"/>
-    <col min="3581" max="3827" width="11.41796875" style="1" hidden="1"/>
-    <col min="3828" max="3828" width="15.41796875" style="1" hidden="1"/>
-    <col min="3829" max="3829" width="11.41796875" style="1" hidden="1"/>
-    <col min="3830" max="3830" width="15.68359375" style="1" hidden="1"/>
-    <col min="3831" max="3831" width="21.83984375" style="1" hidden="1"/>
-    <col min="3832" max="3834" width="11.41796875" style="1" hidden="1"/>
+    <col min="3580" max="3580" width="20.5" style="1" hidden="1"/>
+    <col min="3581" max="3827" width="11.5" style="1" hidden="1"/>
+    <col min="3828" max="3828" width="15.5" style="1" hidden="1"/>
+    <col min="3829" max="3829" width="11.5" style="1" hidden="1"/>
+    <col min="3830" max="3830" width="15.6640625" style="1" hidden="1"/>
+    <col min="3831" max="3831" width="21.83203125" style="1" hidden="1"/>
+    <col min="3832" max="3834" width="11.5" style="1" hidden="1"/>
     <col min="3835" max="3835" width="16" style="1" hidden="1"/>
-    <col min="3836" max="3836" width="20.41796875" style="1" hidden="1"/>
-    <col min="3837" max="4083" width="11.41796875" style="1" hidden="1"/>
-    <col min="4084" max="4084" width="15.41796875" style="1" hidden="1"/>
-    <col min="4085" max="4085" width="11.41796875" style="1" hidden="1"/>
-    <col min="4086" max="4086" width="15.68359375" style="1" hidden="1"/>
-    <col min="4087" max="4087" width="21.83984375" style="1" hidden="1"/>
-    <col min="4088" max="4090" width="11.41796875" style="1" hidden="1"/>
+    <col min="3836" max="3836" width="20.5" style="1" hidden="1"/>
+    <col min="3837" max="4083" width="11.5" style="1" hidden="1"/>
+    <col min="4084" max="4084" width="15.5" style="1" hidden="1"/>
+    <col min="4085" max="4085" width="11.5" style="1" hidden="1"/>
+    <col min="4086" max="4086" width="15.6640625" style="1" hidden="1"/>
+    <col min="4087" max="4087" width="21.83203125" style="1" hidden="1"/>
+    <col min="4088" max="4090" width="11.5" style="1" hidden="1"/>
     <col min="4091" max="4091" width="16" style="1" hidden="1"/>
-    <col min="4092" max="4092" width="20.41796875" style="1" hidden="1"/>
-    <col min="4093" max="4339" width="11.41796875" style="1" hidden="1"/>
-    <col min="4340" max="4340" width="15.41796875" style="1" hidden="1"/>
-    <col min="4341" max="4341" width="11.41796875" style="1" hidden="1"/>
-    <col min="4342" max="4342" width="15.68359375" style="1" hidden="1"/>
-    <col min="4343" max="4343" width="21.83984375" style="1" hidden="1"/>
-    <col min="4344" max="4346" width="11.41796875" style="1" hidden="1"/>
+    <col min="4092" max="4092" width="20.5" style="1" hidden="1"/>
+    <col min="4093" max="4339" width="11.5" style="1" hidden="1"/>
+    <col min="4340" max="4340" width="15.5" style="1" hidden="1"/>
+    <col min="4341" max="4341" width="11.5" style="1" hidden="1"/>
+    <col min="4342" max="4342" width="15.6640625" style="1" hidden="1"/>
+    <col min="4343" max="4343" width="21.83203125" style="1" hidden="1"/>
+    <col min="4344" max="4346" width="11.5" style="1" hidden="1"/>
     <col min="4347" max="4347" width="16" style="1" hidden="1"/>
-    <col min="4348" max="4348" width="20.41796875" style="1" hidden="1"/>
-    <col min="4349" max="4595" width="11.41796875" style="1" hidden="1"/>
-    <col min="4596" max="4596" width="15.41796875" style="1" hidden="1"/>
-    <col min="4597" max="4597" width="11.41796875" style="1" hidden="1"/>
-    <col min="4598" max="4598" width="15.68359375" style="1" hidden="1"/>
-    <col min="4599" max="4599" width="21.83984375" style="1" hidden="1"/>
-    <col min="4600" max="4602" width="11.41796875" style="1" hidden="1"/>
+    <col min="4348" max="4348" width="20.5" style="1" hidden="1"/>
+    <col min="4349" max="4595" width="11.5" style="1" hidden="1"/>
+    <col min="4596" max="4596" width="15.5" style="1" hidden="1"/>
+    <col min="4597" max="4597" width="11.5" style="1" hidden="1"/>
+    <col min="4598" max="4598" width="15.6640625" style="1" hidden="1"/>
+    <col min="4599" max="4599" width="21.83203125" style="1" hidden="1"/>
+    <col min="4600" max="4602" width="11.5" style="1" hidden="1"/>
     <col min="4603" max="4603" width="16" style="1" hidden="1"/>
-    <col min="4604" max="4604" width="20.41796875" style="1" hidden="1"/>
-    <col min="4605" max="4851" width="11.41796875" style="1" hidden="1"/>
-    <col min="4852" max="4852" width="15.41796875" style="1" hidden="1"/>
-    <col min="4853" max="4853" width="11.41796875" style="1" hidden="1"/>
-    <col min="4854" max="4854" width="15.68359375" style="1" hidden="1"/>
-    <col min="4855" max="4855" width="21.83984375" style="1" hidden="1"/>
-    <col min="4856" max="4858" width="11.41796875" style="1" hidden="1"/>
+    <col min="4604" max="4604" width="20.5" style="1" hidden="1"/>
+    <col min="4605" max="4851" width="11.5" style="1" hidden="1"/>
+    <col min="4852" max="4852" width="15.5" style="1" hidden="1"/>
+    <col min="4853" max="4853" width="11.5" style="1" hidden="1"/>
+    <col min="4854" max="4854" width="15.6640625" style="1" hidden="1"/>
+    <col min="4855" max="4855" width="21.83203125" style="1" hidden="1"/>
+    <col min="4856" max="4858" width="11.5" style="1" hidden="1"/>
     <col min="4859" max="4859" width="16" style="1" hidden="1"/>
-    <col min="4860" max="4860" width="20.41796875" style="1" hidden="1"/>
-    <col min="4861" max="5107" width="11.41796875" style="1" hidden="1"/>
-    <col min="5108" max="5108" width="15.41796875" style="1" hidden="1"/>
-    <col min="5109" max="5109" width="11.41796875" style="1" hidden="1"/>
-    <col min="5110" max="5110" width="15.68359375" style="1" hidden="1"/>
-    <col min="5111" max="5111" width="21.83984375" style="1" hidden="1"/>
-    <col min="5112" max="5114" width="11.41796875" style="1" hidden="1"/>
+    <col min="4860" max="4860" width="20.5" style="1" hidden="1"/>
+    <col min="4861" max="5107" width="11.5" style="1" hidden="1"/>
+    <col min="5108" max="5108" width="15.5" style="1" hidden="1"/>
+    <col min="5109" max="5109" width="11.5" style="1" hidden="1"/>
+    <col min="5110" max="5110" width="15.6640625" style="1" hidden="1"/>
+    <col min="5111" max="5111" width="21.83203125" style="1" hidden="1"/>
+    <col min="5112" max="5114" width="11.5" style="1" hidden="1"/>
     <col min="5115" max="5115" width="16" style="1" hidden="1"/>
-    <col min="5116" max="5116" width="20.41796875" style="1" hidden="1"/>
-    <col min="5117" max="5363" width="11.41796875" style="1" hidden="1"/>
-    <col min="5364" max="5364" width="15.41796875" style="1" hidden="1"/>
-    <col min="5365" max="5365" width="11.41796875" style="1" hidden="1"/>
-    <col min="5366" max="5366" width="15.68359375" style="1" hidden="1"/>
-    <col min="5367" max="5367" width="21.83984375" style="1" hidden="1"/>
-    <col min="5368" max="5370" width="11.41796875" style="1" hidden="1"/>
+    <col min="5116" max="5116" width="20.5" style="1" hidden="1"/>
+    <col min="5117" max="5363" width="11.5" style="1" hidden="1"/>
+    <col min="5364" max="5364" width="15.5" style="1" hidden="1"/>
+    <col min="5365" max="5365" width="11.5" style="1" hidden="1"/>
+    <col min="5366" max="5366" width="15.6640625" style="1" hidden="1"/>
+    <col min="5367" max="5367" width="21.83203125" style="1" hidden="1"/>
+    <col min="5368" max="5370" width="11.5" style="1" hidden="1"/>
     <col min="5371" max="5371" width="16" style="1" hidden="1"/>
-    <col min="5372" max="5372" width="20.41796875" style="1" hidden="1"/>
-    <col min="5373" max="5619" width="11.41796875" style="1" hidden="1"/>
-    <col min="5620" max="5620" width="15.41796875" style="1" hidden="1"/>
-    <col min="5621" max="5621" width="11.41796875" style="1" hidden="1"/>
-    <col min="5622" max="5622" width="15.68359375" style="1" hidden="1"/>
-    <col min="5623" max="5623" width="21.83984375" style="1" hidden="1"/>
-    <col min="5624" max="5626" width="11.41796875" style="1" hidden="1"/>
+    <col min="5372" max="5372" width="20.5" style="1" hidden="1"/>
+    <col min="5373" max="5619" width="11.5" style="1" hidden="1"/>
+    <col min="5620" max="5620" width="15.5" style="1" hidden="1"/>
+    <col min="5621" max="5621" width="11.5" style="1" hidden="1"/>
+    <col min="5622" max="5622" width="15.6640625" style="1" hidden="1"/>
+    <col min="5623" max="5623" width="21.83203125" style="1" hidden="1"/>
+    <col min="5624" max="5626" width="11.5" style="1" hidden="1"/>
     <col min="5627" max="5627" width="16" style="1" hidden="1"/>
-    <col min="5628" max="5628" width="20.41796875" style="1" hidden="1"/>
-    <col min="5629" max="5875" width="11.41796875" style="1" hidden="1"/>
-    <col min="5876" max="5876" width="15.41796875" style="1" hidden="1"/>
-    <col min="5877" max="5877" width="11.41796875" style="1" hidden="1"/>
-    <col min="5878" max="5878" width="15.68359375" style="1" hidden="1"/>
-    <col min="5879" max="5879" width="21.83984375" style="1" hidden="1"/>
-    <col min="5880" max="5882" width="11.41796875" style="1" hidden="1"/>
+    <col min="5628" max="5628" width="20.5" style="1" hidden="1"/>
+    <col min="5629" max="5875" width="11.5" style="1" hidden="1"/>
+    <col min="5876" max="5876" width="15.5" style="1" hidden="1"/>
+    <col min="5877" max="5877" width="11.5" style="1" hidden="1"/>
+    <col min="5878" max="5878" width="15.6640625" style="1" hidden="1"/>
+    <col min="5879" max="5879" width="21.83203125" style="1" hidden="1"/>
+    <col min="5880" max="5882" width="11.5" style="1" hidden="1"/>
     <col min="5883" max="5883" width="16" style="1" hidden="1"/>
-    <col min="5884" max="5884" width="20.41796875" style="1" hidden="1"/>
-    <col min="5885" max="6131" width="11.41796875" style="1" hidden="1"/>
-    <col min="6132" max="6132" width="15.41796875" style="1" hidden="1"/>
-    <col min="6133" max="6133" width="11.41796875" style="1" hidden="1"/>
-    <col min="6134" max="6134" width="15.68359375" style="1" hidden="1"/>
-    <col min="6135" max="6135" width="21.83984375" style="1" hidden="1"/>
-    <col min="6136" max="6138" width="11.41796875" style="1" hidden="1"/>
+    <col min="5884" max="5884" width="20.5" style="1" hidden="1"/>
+    <col min="5885" max="6131" width="11.5" style="1" hidden="1"/>
+    <col min="6132" max="6132" width="15.5" style="1" hidden="1"/>
+    <col min="6133" max="6133" width="11.5" style="1" hidden="1"/>
+    <col min="6134" max="6134" width="15.6640625" style="1" hidden="1"/>
+    <col min="6135" max="6135" width="21.83203125" style="1" hidden="1"/>
+    <col min="6136" max="6138" width="11.5" style="1" hidden="1"/>
     <col min="6139" max="6139" width="16" style="1" hidden="1"/>
-    <col min="6140" max="6140" width="20.41796875" style="1" hidden="1"/>
-    <col min="6141" max="6387" width="11.41796875" style="1" hidden="1"/>
-    <col min="6388" max="6388" width="15.41796875" style="1" hidden="1"/>
-    <col min="6389" max="6389" width="11.41796875" style="1" hidden="1"/>
-    <col min="6390" max="6390" width="15.68359375" style="1" hidden="1"/>
-    <col min="6391" max="6391" width="21.83984375" style="1" hidden="1"/>
-    <col min="6392" max="6394" width="11.41796875" style="1" hidden="1"/>
+    <col min="6140" max="6140" width="20.5" style="1" hidden="1"/>
+    <col min="6141" max="6387" width="11.5" style="1" hidden="1"/>
+    <col min="6388" max="6388" width="15.5" style="1" hidden="1"/>
+    <col min="6389" max="6389" width="11.5" style="1" hidden="1"/>
+    <col min="6390" max="6390" width="15.6640625" style="1" hidden="1"/>
+    <col min="6391" max="6391" width="21.83203125" style="1" hidden="1"/>
+    <col min="6392" max="6394" width="11.5" style="1" hidden="1"/>
     <col min="6395" max="6395" width="16" style="1" hidden="1"/>
-    <col min="6396" max="6396" width="20.41796875" style="1" hidden="1"/>
-    <col min="6397" max="6643" width="11.41796875" style="1" hidden="1"/>
-    <col min="6644" max="6644" width="15.41796875" style="1" hidden="1"/>
-    <col min="6645" max="6645" width="11.41796875" style="1" hidden="1"/>
-    <col min="6646" max="6646" width="15.68359375" style="1" hidden="1"/>
-    <col min="6647" max="6647" width="21.83984375" style="1" hidden="1"/>
-    <col min="6648" max="6650" width="11.41796875" style="1" hidden="1"/>
+    <col min="6396" max="6396" width="20.5" style="1" hidden="1"/>
+    <col min="6397" max="6643" width="11.5" style="1" hidden="1"/>
+    <col min="6644" max="6644" width="15.5" style="1" hidden="1"/>
+    <col min="6645" max="6645" width="11.5" style="1" hidden="1"/>
+    <col min="6646" max="6646" width="15.6640625" style="1" hidden="1"/>
+    <col min="6647" max="6647" width="21.83203125" style="1" hidden="1"/>
+    <col min="6648" max="6650" width="11.5" style="1" hidden="1"/>
     <col min="6651" max="6651" width="16" style="1" hidden="1"/>
-    <col min="6652" max="6652" width="20.41796875" style="1" hidden="1"/>
-    <col min="6653" max="6899" width="11.41796875" style="1" hidden="1"/>
-    <col min="6900" max="6900" width="15.41796875" style="1" hidden="1"/>
-    <col min="6901" max="6901" width="11.41796875" style="1" hidden="1"/>
-    <col min="6902" max="6902" width="15.68359375" style="1" hidden="1"/>
-    <col min="6903" max="6903" width="21.83984375" style="1" hidden="1"/>
-    <col min="6904" max="6906" width="11.41796875" style="1" hidden="1"/>
+    <col min="6652" max="6652" width="20.5" style="1" hidden="1"/>
+    <col min="6653" max="6899" width="11.5" style="1" hidden="1"/>
+    <col min="6900" max="6900" width="15.5" style="1" hidden="1"/>
+    <col min="6901" max="6901" width="11.5" style="1" hidden="1"/>
+    <col min="6902" max="6902" width="15.6640625" style="1" hidden="1"/>
+    <col min="6903" max="6903" width="21.83203125" style="1" hidden="1"/>
+    <col min="6904" max="6906" width="11.5" style="1" hidden="1"/>
     <col min="6907" max="6907" width="16" style="1" hidden="1"/>
-    <col min="6908" max="6908" width="20.41796875" style="1" hidden="1"/>
-    <col min="6909" max="7155" width="11.41796875" style="1" hidden="1"/>
-    <col min="7156" max="7156" width="15.41796875" style="1" hidden="1"/>
-    <col min="7157" max="7157" width="11.41796875" style="1" hidden="1"/>
-    <col min="7158" max="7158" width="15.68359375" style="1" hidden="1"/>
-    <col min="7159" max="7159" width="21.83984375" style="1" hidden="1"/>
-    <col min="7160" max="7162" width="11.41796875" style="1" hidden="1"/>
+    <col min="6908" max="6908" width="20.5" style="1" hidden="1"/>
+    <col min="6909" max="7155" width="11.5" style="1" hidden="1"/>
+    <col min="7156" max="7156" width="15.5" style="1" hidden="1"/>
+    <col min="7157" max="7157" width="11.5" style="1" hidden="1"/>
+    <col min="7158" max="7158" width="15.6640625" style="1" hidden="1"/>
+    <col min="7159" max="7159" width="21.83203125" style="1" hidden="1"/>
+    <col min="7160" max="7162" width="11.5" style="1" hidden="1"/>
     <col min="7163" max="7163" width="16" style="1" hidden="1"/>
-    <col min="7164" max="7164" width="20.41796875" style="1" hidden="1"/>
-    <col min="7165" max="7411" width="11.41796875" style="1" hidden="1"/>
-    <col min="7412" max="7412" width="15.41796875" style="1" hidden="1"/>
-    <col min="7413" max="7413" width="11.41796875" style="1" hidden="1"/>
-    <col min="7414" max="7414" width="15.68359375" style="1" hidden="1"/>
-    <col min="7415" max="7415" width="21.83984375" style="1" hidden="1"/>
-    <col min="7416" max="7418" width="11.41796875" style="1" hidden="1"/>
+    <col min="7164" max="7164" width="20.5" style="1" hidden="1"/>
+    <col min="7165" max="7411" width="11.5" style="1" hidden="1"/>
+    <col min="7412" max="7412" width="15.5" style="1" hidden="1"/>
+    <col min="7413" max="7413" width="11.5" style="1" hidden="1"/>
+    <col min="7414" max="7414" width="15.6640625" style="1" hidden="1"/>
+    <col min="7415" max="7415" width="21.83203125" style="1" hidden="1"/>
+    <col min="7416" max="7418" width="11.5" style="1" hidden="1"/>
     <col min="7419" max="7419" width="16" style="1" hidden="1"/>
-    <col min="7420" max="7420" width="20.41796875" style="1" hidden="1"/>
-    <col min="7421" max="7667" width="11.41796875" style="1" hidden="1"/>
-    <col min="7668" max="7668" width="15.41796875" style="1" hidden="1"/>
-    <col min="7669" max="7669" width="11.41796875" style="1" hidden="1"/>
-    <col min="7670" max="7670" width="15.68359375" style="1" hidden="1"/>
-    <col min="7671" max="7671" width="21.83984375" style="1" hidden="1"/>
-    <col min="7672" max="7674" width="11.41796875" style="1" hidden="1"/>
+    <col min="7420" max="7420" width="20.5" style="1" hidden="1"/>
+    <col min="7421" max="7667" width="11.5" style="1" hidden="1"/>
+    <col min="7668" max="7668" width="15.5" style="1" hidden="1"/>
+    <col min="7669" max="7669" width="11.5" style="1" hidden="1"/>
+    <col min="7670" max="7670" width="15.6640625" style="1" hidden="1"/>
+    <col min="7671" max="7671" width="21.83203125" style="1" hidden="1"/>
+    <col min="7672" max="7674" width="11.5" style="1" hidden="1"/>
     <col min="7675" max="7675" width="16" style="1" hidden="1"/>
-    <col min="7676" max="7676" width="20.41796875" style="1" hidden="1"/>
-    <col min="7677" max="7923" width="11.41796875" style="1" hidden="1"/>
-    <col min="7924" max="7924" width="15.41796875" style="1" hidden="1"/>
-    <col min="7925" max="7925" width="11.41796875" style="1" hidden="1"/>
-    <col min="7926" max="7926" width="15.68359375" style="1" hidden="1"/>
-    <col min="7927" max="7927" width="21.83984375" style="1" hidden="1"/>
-    <col min="7928" max="7930" width="11.41796875" style="1" hidden="1"/>
+    <col min="7676" max="7676" width="20.5" style="1" hidden="1"/>
+    <col min="7677" max="7923" width="11.5" style="1" hidden="1"/>
+    <col min="7924" max="7924" width="15.5" style="1" hidden="1"/>
+    <col min="7925" max="7925" width="11.5" style="1" hidden="1"/>
+    <col min="7926" max="7926" width="15.6640625" style="1" hidden="1"/>
+    <col min="7927" max="7927" width="21.83203125" style="1" hidden="1"/>
+    <col min="7928" max="7930" width="11.5" style="1" hidden="1"/>
     <col min="7931" max="7931" width="16" style="1" hidden="1"/>
-    <col min="7932" max="7932" width="20.41796875" style="1" hidden="1"/>
-    <col min="7933" max="8179" width="11.41796875" style="1" hidden="1"/>
-    <col min="8180" max="8180" width="15.41796875" style="1" hidden="1"/>
-    <col min="8181" max="8181" width="11.41796875" style="1" hidden="1"/>
-    <col min="8182" max="8182" width="15.68359375" style="1" hidden="1"/>
-    <col min="8183" max="8183" width="21.83984375" style="1" hidden="1"/>
-    <col min="8184" max="8186" width="11.41796875" style="1" hidden="1"/>
+    <col min="7932" max="7932" width="20.5" style="1" hidden="1"/>
+    <col min="7933" max="8179" width="11.5" style="1" hidden="1"/>
+    <col min="8180" max="8180" width="15.5" style="1" hidden="1"/>
+    <col min="8181" max="8181" width="11.5" style="1" hidden="1"/>
+    <col min="8182" max="8182" width="15.6640625" style="1" hidden="1"/>
+    <col min="8183" max="8183" width="21.83203125" style="1" hidden="1"/>
+    <col min="8184" max="8186" width="11.5" style="1" hidden="1"/>
     <col min="8187" max="8187" width="16" style="1" hidden="1"/>
-    <col min="8188" max="8188" width="20.41796875" style="1" hidden="1"/>
-    <col min="8189" max="8435" width="11.41796875" style="1" hidden="1"/>
-    <col min="8436" max="8436" width="15.41796875" style="1" hidden="1"/>
-    <col min="8437" max="8437" width="11.41796875" style="1" hidden="1"/>
-    <col min="8438" max="8438" width="15.68359375" style="1" hidden="1"/>
-    <col min="8439" max="8439" width="21.83984375" style="1" hidden="1"/>
-    <col min="8440" max="8442" width="11.41796875" style="1" hidden="1"/>
+    <col min="8188" max="8188" width="20.5" style="1" hidden="1"/>
+    <col min="8189" max="8435" width="11.5" style="1" hidden="1"/>
+    <col min="8436" max="8436" width="15.5" style="1" hidden="1"/>
+    <col min="8437" max="8437" width="11.5" style="1" hidden="1"/>
+    <col min="8438" max="8438" width="15.6640625" style="1" hidden="1"/>
+    <col min="8439" max="8439" width="21.83203125" style="1" hidden="1"/>
+    <col min="8440" max="8442" width="11.5" style="1" hidden="1"/>
     <col min="8443" max="8443" width="16" style="1" hidden="1"/>
-    <col min="8444" max="8444" width="20.41796875" style="1" hidden="1"/>
-    <col min="8445" max="8691" width="11.41796875" style="1" hidden="1"/>
-    <col min="8692" max="8692" width="15.41796875" style="1" hidden="1"/>
-    <col min="8693" max="8693" width="11.41796875" style="1" hidden="1"/>
-    <col min="8694" max="8694" width="15.68359375" style="1" hidden="1"/>
-    <col min="8695" max="8695" width="21.83984375" style="1" hidden="1"/>
-    <col min="8696" max="8698" width="11.41796875" style="1" hidden="1"/>
+    <col min="8444" max="8444" width="20.5" style="1" hidden="1"/>
+    <col min="8445" max="8691" width="11.5" style="1" hidden="1"/>
+    <col min="8692" max="8692" width="15.5" style="1" hidden="1"/>
+    <col min="8693" max="8693" width="11.5" style="1" hidden="1"/>
+    <col min="8694" max="8694" width="15.6640625" style="1" hidden="1"/>
+    <col min="8695" max="8695" width="21.83203125" style="1" hidden="1"/>
+    <col min="8696" max="8698" width="11.5" style="1" hidden="1"/>
     <col min="8699" max="8699" width="16" style="1" hidden="1"/>
-    <col min="8700" max="8700" width="20.41796875" style="1" hidden="1"/>
-    <col min="8701" max="8947" width="11.41796875" style="1" hidden="1"/>
-    <col min="8948" max="8948" width="15.41796875" style="1" hidden="1"/>
-    <col min="8949" max="8949" width="11.41796875" style="1" hidden="1"/>
-    <col min="8950" max="8950" width="15.68359375" style="1" hidden="1"/>
-    <col min="8951" max="8951" width="21.83984375" style="1" hidden="1"/>
-    <col min="8952" max="8954" width="11.41796875" style="1" hidden="1"/>
+    <col min="8700" max="8700" width="20.5" style="1" hidden="1"/>
+    <col min="8701" max="8947" width="11.5" style="1" hidden="1"/>
+    <col min="8948" max="8948" width="15.5" style="1" hidden="1"/>
+    <col min="8949" max="8949" width="11.5" style="1" hidden="1"/>
+    <col min="8950" max="8950" width="15.6640625" style="1" hidden="1"/>
+    <col min="8951" max="8951" width="21.83203125" style="1" hidden="1"/>
+    <col min="8952" max="8954" width="11.5" style="1" hidden="1"/>
     <col min="8955" max="8955" width="16" style="1" hidden="1"/>
-    <col min="8956" max="8956" width="20.41796875" style="1" hidden="1"/>
-    <col min="8957" max="9203" width="11.41796875" style="1" hidden="1"/>
-    <col min="9204" max="9204" width="15.41796875" style="1" hidden="1"/>
-    <col min="9205" max="9205" width="11.41796875" style="1" hidden="1"/>
-    <col min="9206" max="9206" width="15.68359375" style="1" hidden="1"/>
-    <col min="9207" max="9207" width="21.83984375" style="1" hidden="1"/>
-    <col min="9208" max="9210" width="11.41796875" style="1" hidden="1"/>
+    <col min="8956" max="8956" width="20.5" style="1" hidden="1"/>
+    <col min="8957" max="9203" width="11.5" style="1" hidden="1"/>
+    <col min="9204" max="9204" width="15.5" style="1" hidden="1"/>
+    <col min="9205" max="9205" width="11.5" style="1" hidden="1"/>
+    <col min="9206" max="9206" width="15.6640625" style="1" hidden="1"/>
+    <col min="9207" max="9207" width="21.83203125" style="1" hidden="1"/>
+    <col min="9208" max="9210" width="11.5" style="1" hidden="1"/>
     <col min="9211" max="9211" width="16" style="1" hidden="1"/>
-    <col min="9212" max="9212" width="20.41796875" style="1" hidden="1"/>
-    <col min="9213" max="9459" width="11.41796875" style="1" hidden="1"/>
-    <col min="9460" max="9460" width="15.41796875" style="1" hidden="1"/>
-    <col min="9461" max="9461" width="11.41796875" style="1" hidden="1"/>
-    <col min="9462" max="9462" width="15.68359375" style="1" hidden="1"/>
-    <col min="9463" max="9463" width="21.83984375" style="1" hidden="1"/>
-    <col min="9464" max="9466" width="11.41796875" style="1" hidden="1"/>
+    <col min="9212" max="9212" width="20.5" style="1" hidden="1"/>
+    <col min="9213" max="9459" width="11.5" style="1" hidden="1"/>
+    <col min="9460" max="9460" width="15.5" style="1" hidden="1"/>
+    <col min="9461" max="9461" width="11.5" style="1" hidden="1"/>
+    <col min="9462" max="9462" width="15.6640625" style="1" hidden="1"/>
+    <col min="9463" max="9463" width="21.83203125" style="1" hidden="1"/>
+    <col min="9464" max="9466" width="11.5" style="1" hidden="1"/>
     <col min="9467" max="9467" width="16" style="1" hidden="1"/>
-    <col min="9468" max="9468" width="20.41796875" style="1" hidden="1"/>
-    <col min="9469" max="9715" width="11.41796875" style="1" hidden="1"/>
-    <col min="9716" max="9716" width="15.41796875" style="1" hidden="1"/>
-    <col min="9717" max="9717" width="11.41796875" style="1" hidden="1"/>
-    <col min="9718" max="9718" width="15.68359375" style="1" hidden="1"/>
-    <col min="9719" max="9719" width="21.83984375" style="1" hidden="1"/>
-    <col min="9720" max="9722" width="11.41796875" style="1" hidden="1"/>
+    <col min="9468" max="9468" width="20.5" style="1" hidden="1"/>
+    <col min="9469" max="9715" width="11.5" style="1" hidden="1"/>
+    <col min="9716" max="9716" width="15.5" style="1" hidden="1"/>
+    <col min="9717" max="9717" width="11.5" style="1" hidden="1"/>
+    <col min="9718" max="9718" width="15.6640625" style="1" hidden="1"/>
+    <col min="9719" max="9719" width="21.83203125" style="1" hidden="1"/>
+    <col min="9720" max="9722" width="11.5" style="1" hidden="1"/>
     <col min="9723" max="9723" width="16" style="1" hidden="1"/>
-    <col min="9724" max="9724" width="20.41796875" style="1" hidden="1"/>
-    <col min="9725" max="9971" width="11.41796875" style="1" hidden="1"/>
-    <col min="9972" max="9972" width="15.41796875" style="1" hidden="1"/>
-    <col min="9973" max="9973" width="11.41796875" style="1" hidden="1"/>
-    <col min="9974" max="9974" width="15.68359375" style="1" hidden="1"/>
-    <col min="9975" max="9975" width="21.83984375" style="1" hidden="1"/>
-    <col min="9976" max="9978" width="11.41796875" style="1" hidden="1"/>
+    <col min="9724" max="9724" width="20.5" style="1" hidden="1"/>
+    <col min="9725" max="9971" width="11.5" style="1" hidden="1"/>
+    <col min="9972" max="9972" width="15.5" style="1" hidden="1"/>
+    <col min="9973" max="9973" width="11.5" style="1" hidden="1"/>
+    <col min="9974" max="9974" width="15.6640625" style="1" hidden="1"/>
+    <col min="9975" max="9975" width="21.83203125" style="1" hidden="1"/>
+    <col min="9976" max="9978" width="11.5" style="1" hidden="1"/>
     <col min="9979" max="9979" width="16" style="1" hidden="1"/>
-    <col min="9980" max="9980" width="20.41796875" style="1" hidden="1"/>
-    <col min="9981" max="10227" width="11.41796875" style="1" hidden="1"/>
-    <col min="10228" max="10228" width="15.41796875" style="1" hidden="1"/>
-    <col min="10229" max="10229" width="11.41796875" style="1" hidden="1"/>
-    <col min="10230" max="10230" width="15.68359375" style="1" hidden="1"/>
-    <col min="10231" max="10231" width="21.83984375" style="1" hidden="1"/>
-    <col min="10232" max="10234" width="11.41796875" style="1" hidden="1"/>
+    <col min="9980" max="9980" width="20.5" style="1" hidden="1"/>
+    <col min="9981" max="10227" width="11.5" style="1" hidden="1"/>
+    <col min="10228" max="10228" width="15.5" style="1" hidden="1"/>
+    <col min="10229" max="10229" width="11.5" style="1" hidden="1"/>
+    <col min="10230" max="10230" width="15.6640625" style="1" hidden="1"/>
+    <col min="10231" max="10231" width="21.83203125" style="1" hidden="1"/>
+    <col min="10232" max="10234" width="11.5" style="1" hidden="1"/>
     <col min="10235" max="10235" width="16" style="1" hidden="1"/>
-    <col min="10236" max="10236" width="20.41796875" style="1" hidden="1"/>
-    <col min="10237" max="10483" width="11.41796875" style="1" hidden="1"/>
-    <col min="10484" max="10484" width="15.41796875" style="1" hidden="1"/>
-    <col min="10485" max="10485" width="11.41796875" style="1" hidden="1"/>
-    <col min="10486" max="10486" width="15.68359375" style="1" hidden="1"/>
-    <col min="10487" max="10487" width="21.83984375" style="1" hidden="1"/>
-    <col min="10488" max="10490" width="11.41796875" style="1" hidden="1"/>
+    <col min="10236" max="10236" width="20.5" style="1" hidden="1"/>
+    <col min="10237" max="10483" width="11.5" style="1" hidden="1"/>
+    <col min="10484" max="10484" width="15.5" style="1" hidden="1"/>
+    <col min="10485" max="10485" width="11.5" style="1" hidden="1"/>
+    <col min="10486" max="10486" width="15.6640625" style="1" hidden="1"/>
+    <col min="10487" max="10487" width="21.83203125" style="1" hidden="1"/>
+    <col min="10488" max="10490" width="11.5" style="1" hidden="1"/>
     <col min="10491" max="10491" width="16" style="1" hidden="1"/>
-    <col min="10492" max="10492" width="20.41796875" style="1" hidden="1"/>
-    <col min="10493" max="10739" width="11.41796875" style="1" hidden="1"/>
-    <col min="10740" max="10740" width="15.41796875" style="1" hidden="1"/>
-    <col min="10741" max="10741" width="11.41796875" style="1" hidden="1"/>
-    <col min="10742" max="10742" width="15.68359375" style="1" hidden="1"/>
-    <col min="10743" max="10743" width="21.83984375" style="1" hidden="1"/>
-    <col min="10744" max="10746" width="11.41796875" style="1" hidden="1"/>
+    <col min="10492" max="10492" width="20.5" style="1" hidden="1"/>
+    <col min="10493" max="10739" width="11.5" style="1" hidden="1"/>
+    <col min="10740" max="10740" width="15.5" style="1" hidden="1"/>
+    <col min="10741" max="10741" width="11.5" style="1" hidden="1"/>
+    <col min="10742" max="10742" width="15.6640625" style="1" hidden="1"/>
+    <col min="10743" max="10743" width="21.83203125" style="1" hidden="1"/>
+    <col min="10744" max="10746" width="11.5" style="1" hidden="1"/>
     <col min="10747" max="10747" width="16" style="1" hidden="1"/>
-    <col min="10748" max="10748" width="20.41796875" style="1" hidden="1"/>
-    <col min="10749" max="10995" width="11.41796875" style="1" hidden="1"/>
-    <col min="10996" max="10996" width="15.41796875" style="1" hidden="1"/>
-    <col min="10997" max="10997" width="11.41796875" style="1" hidden="1"/>
-    <col min="10998" max="10998" width="15.68359375" style="1" hidden="1"/>
-    <col min="10999" max="10999" width="21.83984375" style="1" hidden="1"/>
-    <col min="11000" max="11002" width="11.41796875" style="1" hidden="1"/>
+    <col min="10748" max="10748" width="20.5" style="1" hidden="1"/>
+    <col min="10749" max="10995" width="11.5" style="1" hidden="1"/>
+    <col min="10996" max="10996" width="15.5" style="1" hidden="1"/>
+    <col min="10997" max="10997" width="11.5" style="1" hidden="1"/>
+    <col min="10998" max="10998" width="15.6640625" style="1" hidden="1"/>
+    <col min="10999" max="10999" width="21.83203125" style="1" hidden="1"/>
+    <col min="11000" max="11002" width="11.5" style="1" hidden="1"/>
     <col min="11003" max="11003" width="16" style="1" hidden="1"/>
-    <col min="11004" max="11004" width="20.41796875" style="1" hidden="1"/>
-    <col min="11005" max="11251" width="11.41796875" style="1" hidden="1"/>
-    <col min="11252" max="11252" width="15.41796875" style="1" hidden="1"/>
-    <col min="11253" max="11253" width="11.41796875" style="1" hidden="1"/>
-    <col min="11254" max="11254" width="15.68359375" style="1" hidden="1"/>
-    <col min="11255" max="11255" width="21.83984375" style="1" hidden="1"/>
-    <col min="11256" max="11258" width="11.41796875" style="1" hidden="1"/>
+    <col min="11004" max="11004" width="20.5" style="1" hidden="1"/>
+    <col min="11005" max="11251" width="11.5" style="1" hidden="1"/>
+    <col min="11252" max="11252" width="15.5" style="1" hidden="1"/>
+    <col min="11253" max="11253" width="11.5" style="1" hidden="1"/>
+    <col min="11254" max="11254" width="15.6640625" style="1" hidden="1"/>
+    <col min="11255" max="11255" width="21.83203125" style="1" hidden="1"/>
+    <col min="11256" max="11258" width="11.5" style="1" hidden="1"/>
     <col min="11259" max="11259" width="16" style="1" hidden="1"/>
-    <col min="11260" max="11260" width="20.41796875" style="1" hidden="1"/>
-    <col min="11261" max="11507" width="11.41796875" style="1" hidden="1"/>
-    <col min="11508" max="11508" width="15.41796875" style="1" hidden="1"/>
-    <col min="11509" max="11509" width="11.41796875" style="1" hidden="1"/>
-    <col min="11510" max="11510" width="15.68359375" style="1" hidden="1"/>
-    <col min="11511" max="11511" width="21.83984375" style="1" hidden="1"/>
-    <col min="11512" max="11514" width="11.41796875" style="1" hidden="1"/>
+    <col min="11260" max="11260" width="20.5" style="1" hidden="1"/>
+    <col min="11261" max="11507" width="11.5" style="1" hidden="1"/>
+    <col min="11508" max="11508" width="15.5" style="1" hidden="1"/>
+    <col min="11509" max="11509" width="11.5" style="1" hidden="1"/>
+    <col min="11510" max="11510" width="15.6640625" style="1" hidden="1"/>
+    <col min="11511" max="11511" width="21.83203125" style="1" hidden="1"/>
+    <col min="11512" max="11514" width="11.5" style="1" hidden="1"/>
     <col min="11515" max="11515" width="16" style="1" hidden="1"/>
-    <col min="11516" max="11516" width="20.41796875" style="1" hidden="1"/>
-    <col min="11517" max="11763" width="11.41796875" style="1" hidden="1"/>
-    <col min="11764" max="11764" width="15.41796875" style="1" hidden="1"/>
-    <col min="11765" max="11765" width="11.41796875" style="1" hidden="1"/>
-    <col min="11766" max="11766" width="15.68359375" style="1" hidden="1"/>
-    <col min="11767" max="11767" width="21.83984375" style="1" hidden="1"/>
-    <col min="11768" max="11770" width="11.41796875" style="1" hidden="1"/>
+    <col min="11516" max="11516" width="20.5" style="1" hidden="1"/>
+    <col min="11517" max="11763" width="11.5" style="1" hidden="1"/>
+    <col min="11764" max="11764" width="15.5" style="1" hidden="1"/>
+    <col min="11765" max="11765" width="11.5" style="1" hidden="1"/>
+    <col min="11766" max="11766" width="15.6640625" style="1" hidden="1"/>
+    <col min="11767" max="11767" width="21.83203125" style="1" hidden="1"/>
+    <col min="11768" max="11770" width="11.5" style="1" hidden="1"/>
     <col min="11771" max="11771" width="16" style="1" hidden="1"/>
-    <col min="11772" max="11772" width="20.41796875" style="1" hidden="1"/>
-    <col min="11773" max="12019" width="11.41796875" style="1" hidden="1"/>
-    <col min="12020" max="12020" width="15.41796875" style="1" hidden="1"/>
-    <col min="12021" max="12021" width="11.41796875" style="1" hidden="1"/>
-    <col min="12022" max="12022" width="15.68359375" style="1" hidden="1"/>
-    <col min="12023" max="12023" width="21.83984375" style="1" hidden="1"/>
-    <col min="12024" max="12026" width="11.41796875" style="1" hidden="1"/>
+    <col min="11772" max="11772" width="20.5" style="1" hidden="1"/>
+    <col min="11773" max="12019" width="11.5" style="1" hidden="1"/>
+    <col min="12020" max="12020" width="15.5" style="1" hidden="1"/>
+    <col min="12021" max="12021" width="11.5" style="1" hidden="1"/>
+    <col min="12022" max="12022" width="15.6640625" style="1" hidden="1"/>
+    <col min="12023" max="12023" width="21.83203125" style="1" hidden="1"/>
+    <col min="12024" max="12026" width="11.5" style="1" hidden="1"/>
     <col min="12027" max="12027" width="16" style="1" hidden="1"/>
-    <col min="12028" max="12028" width="20.41796875" style="1" hidden="1"/>
-    <col min="12029" max="12275" width="11.41796875" style="1" hidden="1"/>
-    <col min="12276" max="12276" width="15.41796875" style="1" hidden="1"/>
-    <col min="12277" max="12277" width="11.41796875" style="1" hidden="1"/>
-    <col min="12278" max="12278" width="15.68359375" style="1" hidden="1"/>
-    <col min="12279" max="12279" width="21.83984375" style="1" hidden="1"/>
-    <col min="12280" max="12282" width="11.41796875" style="1" hidden="1"/>
+    <col min="12028" max="12028" width="20.5" style="1" hidden="1"/>
+    <col min="12029" max="12275" width="11.5" style="1" hidden="1"/>
+    <col min="12276" max="12276" width="15.5" style="1" hidden="1"/>
+    <col min="12277" max="12277" width="11.5" style="1" hidden="1"/>
+    <col min="12278" max="12278" width="15.6640625" style="1" hidden="1"/>
+    <col min="12279" max="12279" width="21.83203125" style="1" hidden="1"/>
+    <col min="12280" max="12282" width="11.5" style="1" hidden="1"/>
     <col min="12283" max="12283" width="16" style="1" hidden="1"/>
-    <col min="12284" max="12284" width="20.41796875" style="1" hidden="1"/>
-    <col min="12285" max="12531" width="11.41796875" style="1" hidden="1"/>
-    <col min="12532" max="12532" width="15.41796875" style="1" hidden="1"/>
-    <col min="12533" max="12533" width="11.41796875" style="1" hidden="1"/>
-    <col min="12534" max="12534" width="15.68359375" style="1" hidden="1"/>
-    <col min="12535" max="12535" width="21.83984375" style="1" hidden="1"/>
-    <col min="12536" max="12538" width="11.41796875" style="1" hidden="1"/>
+    <col min="12284" max="12284" width="20.5" style="1" hidden="1"/>
+    <col min="12285" max="12531" width="11.5" style="1" hidden="1"/>
+    <col min="12532" max="12532" width="15.5" style="1" hidden="1"/>
+    <col min="12533" max="12533" width="11.5" style="1" hidden="1"/>
+    <col min="12534" max="12534" width="15.6640625" style="1" hidden="1"/>
+    <col min="12535" max="12535" width="21.83203125" style="1" hidden="1"/>
+    <col min="12536" max="12538" width="11.5" style="1" hidden="1"/>
     <col min="12539" max="12539" width="16" style="1" hidden="1"/>
-    <col min="12540" max="12540" width="20.41796875" style="1" hidden="1"/>
-    <col min="12541" max="12787" width="11.41796875" style="1" hidden="1"/>
-    <col min="12788" max="12788" width="15.41796875" style="1" hidden="1"/>
-    <col min="12789" max="12789" width="11.41796875" style="1" hidden="1"/>
-    <col min="12790" max="12790" width="15.68359375" style="1" hidden="1"/>
-    <col min="12791" max="12791" width="21.83984375" style="1" hidden="1"/>
-    <col min="12792" max="12794" width="11.41796875" style="1" hidden="1"/>
+    <col min="12540" max="12540" width="20.5" style="1" hidden="1"/>
+    <col min="12541" max="12787" width="11.5" style="1" hidden="1"/>
+    <col min="12788" max="12788" width="15.5" style="1" hidden="1"/>
+    <col min="12789" max="12789" width="11.5" style="1" hidden="1"/>
+    <col min="12790" max="12790" width="15.6640625" style="1" hidden="1"/>
+    <col min="12791" max="12791" width="21.83203125" style="1" hidden="1"/>
+    <col min="12792" max="12794" width="11.5" style="1" hidden="1"/>
     <col min="12795" max="12795" width="16" style="1" hidden="1"/>
-    <col min="12796" max="12796" width="20.41796875" style="1" hidden="1"/>
-    <col min="12797" max="13043" width="11.41796875" style="1" hidden="1"/>
-    <col min="13044" max="13044" width="15.41796875" style="1" hidden="1"/>
-    <col min="13045" max="13045" width="11.41796875" style="1" hidden="1"/>
-    <col min="13046" max="13046" width="15.68359375" style="1" hidden="1"/>
-    <col min="13047" max="13047" width="21.83984375" style="1" hidden="1"/>
-    <col min="13048" max="13050" width="11.41796875" style="1" hidden="1"/>
+    <col min="12796" max="12796" width="20.5" style="1" hidden="1"/>
+    <col min="12797" max="13043" width="11.5" style="1" hidden="1"/>
+    <col min="13044" max="13044" width="15.5" style="1" hidden="1"/>
+    <col min="13045" max="13045" width="11.5" style="1" hidden="1"/>
+    <col min="13046" max="13046" width="15.6640625" style="1" hidden="1"/>
+    <col min="13047" max="13047" width="21.83203125" style="1" hidden="1"/>
+    <col min="13048" max="13050" width="11.5" style="1" hidden="1"/>
     <col min="13051" max="13051" width="16" style="1" hidden="1"/>
-    <col min="13052" max="13052" width="20.41796875" style="1" hidden="1"/>
-    <col min="13053" max="13299" width="11.41796875" style="1" hidden="1"/>
-    <col min="13300" max="13300" width="15.41796875" style="1" hidden="1"/>
-    <col min="13301" max="13301" width="11.41796875" style="1" hidden="1"/>
-    <col min="13302" max="13302" width="15.68359375" style="1" hidden="1"/>
-    <col min="13303" max="13303" width="21.83984375" style="1" hidden="1"/>
-    <col min="13304" max="13306" width="11.41796875" style="1" hidden="1"/>
+    <col min="13052" max="13052" width="20.5" style="1" hidden="1"/>
+    <col min="13053" max="13299" width="11.5" style="1" hidden="1"/>
+    <col min="13300" max="13300" width="15.5" style="1" hidden="1"/>
+    <col min="13301" max="13301" width="11.5" style="1" hidden="1"/>
+    <col min="13302" max="13302" width="15.6640625" style="1" hidden="1"/>
+    <col min="13303" max="13303" width="21.83203125" style="1" hidden="1"/>
+    <col min="13304" max="13306" width="11.5" style="1" hidden="1"/>
     <col min="13307" max="13307" width="16" style="1" hidden="1"/>
-    <col min="13308" max="13308" width="20.41796875" style="1" hidden="1"/>
-    <col min="13309" max="13555" width="11.41796875" style="1" hidden="1"/>
-    <col min="13556" max="13556" width="15.41796875" style="1" hidden="1"/>
-    <col min="13557" max="13557" width="11.41796875" style="1" hidden="1"/>
-    <col min="13558" max="13558" width="15.68359375" style="1" hidden="1"/>
-    <col min="13559" max="13559" width="21.83984375" style="1" hidden="1"/>
-    <col min="13560" max="13562" width="11.41796875" style="1" hidden="1"/>
+    <col min="13308" max="13308" width="20.5" style="1" hidden="1"/>
+    <col min="13309" max="13555" width="11.5" style="1" hidden="1"/>
+    <col min="13556" max="13556" width="15.5" style="1" hidden="1"/>
+    <col min="13557" max="13557" width="11.5" style="1" hidden="1"/>
+    <col min="13558" max="13558" width="15.6640625" style="1" hidden="1"/>
+    <col min="13559" max="13559" width="21.83203125" style="1" hidden="1"/>
+    <col min="13560" max="13562" width="11.5" style="1" hidden="1"/>
     <col min="13563" max="13563" width="16" style="1" hidden="1"/>
-    <col min="13564" max="13564" width="20.41796875" style="1" hidden="1"/>
-    <col min="13565" max="13811" width="11.41796875" style="1" hidden="1"/>
-    <col min="13812" max="13812" width="15.41796875" style="1" hidden="1"/>
-    <col min="13813" max="13813" width="11.41796875" style="1" hidden="1"/>
-    <col min="13814" max="13814" width="15.68359375" style="1" hidden="1"/>
-    <col min="13815" max="13815" width="21.83984375" style="1" hidden="1"/>
-    <col min="13816" max="13818" width="11.41796875" style="1" hidden="1"/>
+    <col min="13564" max="13564" width="20.5" style="1" hidden="1"/>
+    <col min="13565" max="13811" width="11.5" style="1" hidden="1"/>
+    <col min="13812" max="13812" width="15.5" style="1" hidden="1"/>
+    <col min="13813" max="13813" width="11.5" style="1" hidden="1"/>
+    <col min="13814" max="13814" width="15.6640625" style="1" hidden="1"/>
+    <col min="13815" max="13815" width="21.83203125" style="1" hidden="1"/>
+    <col min="13816" max="13818" width="11.5" style="1" hidden="1"/>
     <col min="13819" max="13819" width="16" style="1" hidden="1"/>
-    <col min="13820" max="13820" width="20.41796875" style="1" hidden="1"/>
-    <col min="13821" max="14067" width="11.41796875" style="1" hidden="1"/>
-    <col min="14068" max="14068" width="15.41796875" style="1" hidden="1"/>
-    <col min="14069" max="14069" width="11.41796875" style="1" hidden="1"/>
-    <col min="14070" max="14070" width="15.68359375" style="1" hidden="1"/>
-    <col min="14071" max="14071" width="21.83984375" style="1" hidden="1"/>
-    <col min="14072" max="14074" width="11.41796875" style="1" hidden="1"/>
+    <col min="13820" max="13820" width="20.5" style="1" hidden="1"/>
+    <col min="13821" max="14067" width="11.5" style="1" hidden="1"/>
+    <col min="14068" max="14068" width="15.5" style="1" hidden="1"/>
+    <col min="14069" max="14069" width="11.5" style="1" hidden="1"/>
+    <col min="14070" max="14070" width="15.6640625" style="1" hidden="1"/>
+    <col min="14071" max="14071" width="21.83203125" style="1" hidden="1"/>
+    <col min="14072" max="14074" width="11.5" style="1" hidden="1"/>
     <col min="14075" max="14075" width="16" style="1" hidden="1"/>
-    <col min="14076" max="14076" width="20.41796875" style="1" hidden="1"/>
-    <col min="14077" max="14323" width="11.41796875" style="1" hidden="1"/>
-    <col min="14324" max="14324" width="15.41796875" style="1" hidden="1"/>
-    <col min="14325" max="14325" width="11.41796875" style="1" hidden="1"/>
-    <col min="14326" max="14326" width="15.68359375" style="1" hidden="1"/>
-    <col min="14327" max="14327" width="21.83984375" style="1" hidden="1"/>
-    <col min="14328" max="14330" width="11.41796875" style="1" hidden="1"/>
+    <col min="14076" max="14076" width="20.5" style="1" hidden="1"/>
+    <col min="14077" max="14323" width="11.5" style="1" hidden="1"/>
+    <col min="14324" max="14324" width="15.5" style="1" hidden="1"/>
+    <col min="14325" max="14325" width="11.5" style="1" hidden="1"/>
+    <col min="14326" max="14326" width="15.6640625" style="1" hidden="1"/>
+    <col min="14327" max="14327" width="21.83203125" style="1" hidden="1"/>
+    <col min="14328" max="14330" width="11.5" style="1" hidden="1"/>
     <col min="14331" max="14331" width="16" style="1" hidden="1"/>
-    <col min="14332" max="14332" width="20.41796875" style="1" hidden="1"/>
-    <col min="14333" max="14579" width="11.41796875" style="1" hidden="1"/>
-    <col min="14580" max="14580" width="15.41796875" style="1" hidden="1"/>
-    <col min="14581" max="14581" width="11.41796875" style="1" hidden="1"/>
-    <col min="14582" max="14582" width="15.68359375" style="1" hidden="1"/>
-    <col min="14583" max="14583" width="21.83984375" style="1" hidden="1"/>
-    <col min="14584" max="14586" width="11.41796875" style="1" hidden="1"/>
+    <col min="14332" max="14332" width="20.5" style="1" hidden="1"/>
+    <col min="14333" max="14579" width="11.5" style="1" hidden="1"/>
+    <col min="14580" max="14580" width="15.5" style="1" hidden="1"/>
+    <col min="14581" max="14581" width="11.5" style="1" hidden="1"/>
+    <col min="14582" max="14582" width="15.6640625" style="1" hidden="1"/>
+    <col min="14583" max="14583" width="21.83203125" style="1" hidden="1"/>
+    <col min="14584" max="14586" width="11.5" style="1" hidden="1"/>
     <col min="14587" max="14587" width="16" style="1" hidden="1"/>
-    <col min="14588" max="14588" width="20.41796875" style="1" hidden="1"/>
-    <col min="14589" max="14835" width="11.41796875" style="1" hidden="1"/>
-    <col min="14836" max="14836" width="15.41796875" style="1" hidden="1"/>
-    <col min="14837" max="14837" width="11.41796875" style="1" hidden="1"/>
-    <col min="14838" max="14838" width="15.68359375" style="1" hidden="1"/>
-    <col min="14839" max="14839" width="21.83984375" style="1" hidden="1"/>
-    <col min="14840" max="14842" width="11.41796875" style="1" hidden="1"/>
+    <col min="14588" max="14588" width="20.5" style="1" hidden="1"/>
+    <col min="14589" max="14835" width="11.5" style="1" hidden="1"/>
+    <col min="14836" max="14836" width="15.5" style="1" hidden="1"/>
+    <col min="14837" max="14837" width="11.5" style="1" hidden="1"/>
+    <col min="14838" max="14838" width="15.6640625" style="1" hidden="1"/>
+    <col min="14839" max="14839" width="21.83203125" style="1" hidden="1"/>
+    <col min="14840" max="14842" width="11.5" style="1" hidden="1"/>
     <col min="14843" max="14843" width="16" style="1" hidden="1"/>
-    <col min="14844" max="14844" width="20.41796875" style="1" hidden="1"/>
-    <col min="14845" max="15091" width="11.41796875" style="1" hidden="1"/>
-    <col min="15092" max="15092" width="15.41796875" style="1" hidden="1"/>
-    <col min="15093" max="15093" width="11.41796875" style="1" hidden="1"/>
-    <col min="15094" max="15094" width="15.68359375" style="1" hidden="1"/>
-    <col min="15095" max="15095" width="21.83984375" style="1" hidden="1"/>
-    <col min="15096" max="15098" width="11.41796875" style="1" hidden="1"/>
+    <col min="14844" max="14844" width="20.5" style="1" hidden="1"/>
+    <col min="14845" max="15091" width="11.5" style="1" hidden="1"/>
+    <col min="15092" max="15092" width="15.5" style="1" hidden="1"/>
+    <col min="15093" max="15093" width="11.5" style="1" hidden="1"/>
+    <col min="15094" max="15094" width="15.6640625" style="1" hidden="1"/>
+    <col min="15095" max="15095" width="21.83203125" style="1" hidden="1"/>
+    <col min="15096" max="15098" width="11.5" style="1" hidden="1"/>
     <col min="15099" max="15099" width="16" style="1" hidden="1"/>
-    <col min="15100" max="15100" width="20.41796875" style="1" hidden="1"/>
-    <col min="15101" max="15347" width="11.41796875" style="1" hidden="1"/>
-    <col min="15348" max="15348" width="15.41796875" style="1" hidden="1"/>
-    <col min="15349" max="15349" width="11.41796875" style="1" hidden="1"/>
-    <col min="15350" max="15350" width="15.68359375" style="1" hidden="1"/>
-    <col min="15351" max="15351" width="21.83984375" style="1" hidden="1"/>
-    <col min="15352" max="15354" width="11.41796875" style="1" hidden="1"/>
+    <col min="15100" max="15100" width="20.5" style="1" hidden="1"/>
+    <col min="15101" max="15347" width="11.5" style="1" hidden="1"/>
+    <col min="15348" max="15348" width="15.5" style="1" hidden="1"/>
+    <col min="15349" max="15349" width="11.5" style="1" hidden="1"/>
+    <col min="15350" max="15350" width="15.6640625" style="1" hidden="1"/>
+    <col min="15351" max="15351" width="21.83203125" style="1" hidden="1"/>
+    <col min="15352" max="15354" width="11.5" style="1" hidden="1"/>
     <col min="15355" max="15355" width="16" style="1" hidden="1"/>
-    <col min="15356" max="15356" width="20.41796875" style="1" hidden="1"/>
-    <col min="15357" max="15603" width="11.41796875" style="1" hidden="1"/>
-    <col min="15604" max="15604" width="15.41796875" style="1" hidden="1"/>
-    <col min="15605" max="15605" width="11.41796875" style="1" hidden="1"/>
-    <col min="15606" max="15606" width="15.68359375" style="1" hidden="1"/>
-    <col min="15607" max="15607" width="21.83984375" style="1" hidden="1"/>
-    <col min="15608" max="15610" width="11.41796875" style="1" hidden="1"/>
+    <col min="15356" max="15356" width="20.5" style="1" hidden="1"/>
+    <col min="15357" max="15603" width="11.5" style="1" hidden="1"/>
+    <col min="15604" max="15604" width="15.5" style="1" hidden="1"/>
+    <col min="15605" max="15605" width="11.5" style="1" hidden="1"/>
+    <col min="15606" max="15606" width="15.6640625" style="1" hidden="1"/>
+    <col min="15607" max="15607" width="21.83203125" style="1" hidden="1"/>
+    <col min="15608" max="15610" width="11.5" style="1" hidden="1"/>
     <col min="15611" max="15611" width="16" style="1" hidden="1"/>
-    <col min="15612" max="15612" width="20.41796875" style="1" hidden="1"/>
-    <col min="15613" max="15859" width="11.41796875" style="1" hidden="1"/>
-    <col min="15860" max="15860" width="15.41796875" style="1" hidden="1"/>
-    <col min="15861" max="15861" width="11.41796875" style="1" hidden="1"/>
-    <col min="15862" max="15862" width="15.68359375" style="1" hidden="1"/>
-    <col min="15863" max="15863" width="21.83984375" style="1" hidden="1"/>
-    <col min="15864" max="15866" width="11.41796875" style="1" hidden="1"/>
+    <col min="15612" max="15612" width="20.5" style="1" hidden="1"/>
+    <col min="15613" max="15859" width="11.5" style="1" hidden="1"/>
+    <col min="15860" max="15860" width="15.5" style="1" hidden="1"/>
+    <col min="15861" max="15861" width="11.5" style="1" hidden="1"/>
+    <col min="15862" max="15862" width="15.6640625" style="1" hidden="1"/>
+    <col min="15863" max="15863" width="21.83203125" style="1" hidden="1"/>
+    <col min="15864" max="15866" width="11.5" style="1" hidden="1"/>
     <col min="15867" max="15867" width="16" style="1" hidden="1"/>
-    <col min="15868" max="15868" width="20.41796875" style="1" hidden="1"/>
-    <col min="15869" max="16115" width="11.41796875" style="1" hidden="1"/>
-    <col min="16116" max="16116" width="15.41796875" style="1" hidden="1"/>
-    <col min="16117" max="16117" width="11.41796875" style="1" hidden="1"/>
-    <col min="16118" max="16118" width="15.68359375" style="1" hidden="1"/>
-    <col min="16119" max="16119" width="21.83984375" style="1" hidden="1"/>
-    <col min="16120" max="16122" width="11.41796875" style="1" hidden="1"/>
+    <col min="15868" max="15868" width="20.5" style="1" hidden="1"/>
+    <col min="15869" max="16115" width="11.5" style="1" hidden="1"/>
+    <col min="16116" max="16116" width="15.5" style="1" hidden="1"/>
+    <col min="16117" max="16117" width="11.5" style="1" hidden="1"/>
+    <col min="16118" max="16118" width="15.6640625" style="1" hidden="1"/>
+    <col min="16119" max="16119" width="21.83203125" style="1" hidden="1"/>
+    <col min="16120" max="16122" width="11.5" style="1" hidden="1"/>
     <col min="16123" max="16123" width="16" style="1" hidden="1"/>
-    <col min="16124" max="16124" width="20.41796875" style="1" hidden="1"/>
-    <col min="16125" max="16127" width="11.41796875" style="1" hidden="1"/>
-    <col min="16128" max="16128" width="15.41796875" style="1" hidden="1"/>
-    <col min="16129" max="16129" width="11.41796875" style="1" hidden="1"/>
-    <col min="16130" max="16130" width="15.68359375" style="1" hidden="1"/>
-    <col min="16131" max="16131" width="21.83984375" style="1" hidden="1"/>
-    <col min="16132" max="16134" width="11.41796875" style="1" hidden="1"/>
+    <col min="16124" max="16124" width="20.5" style="1" hidden="1"/>
+    <col min="16125" max="16127" width="11.5" style="1" hidden="1"/>
+    <col min="16128" max="16128" width="15.5" style="1" hidden="1"/>
+    <col min="16129" max="16129" width="11.5" style="1" hidden="1"/>
+    <col min="16130" max="16130" width="15.6640625" style="1" hidden="1"/>
+    <col min="16131" max="16131" width="21.83203125" style="1" hidden="1"/>
+    <col min="16132" max="16134" width="11.5" style="1" hidden="1"/>
     <col min="16135" max="16135" width="16" style="1" hidden="1"/>
-    <col min="16136" max="16137" width="20.41796875" style="1" hidden="1"/>
-    <col min="16138" max="16139" width="11.41796875" style="1" hidden="1"/>
+    <col min="16136" max="16137" width="20.5" style="1" hidden="1"/>
+    <col min="16138" max="16139" width="11.5" style="1" hidden="1"/>
     <col min="16140" max="16140" width="16" style="1" hidden="1"/>
-    <col min="16141" max="16143" width="20.41796875" style="1" hidden="1"/>
-    <col min="16144" max="16384" width="11.41796875" style="1" hidden="1"/>
+    <col min="16141" max="16143" width="20.5" style="1" hidden="1"/>
+    <col min="16144" max="16384" width="11.5" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -2436,7 +2443,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A2" s="32" t="str">
         <f>RAWDATA!B2</f>
         <v>applicant.last_name</v>
@@ -2455,7 +2462,7 @@
       </c>
       <c r="E2" s="38"/>
       <c r="F2" s="34" t="str">
-        <f>LOOKUP(E2,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E2,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G2" s="4"/>
@@ -2488,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A3" s="32">
         <f>RAWDATA!B3</f>
         <v>0</v>
@@ -2507,7 +2514,7 @@
       </c>
       <c r="E3" s="38"/>
       <c r="F3" s="34" t="str">
-        <f>LOOKUP(E3,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E3,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G3" s="4"/>
@@ -2540,7 +2547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A4" s="32">
         <f>RAWDATA!B4</f>
         <v>0</v>
@@ -2559,7 +2566,7 @@
       </c>
       <c r="E4" s="38"/>
       <c r="F4" s="34" t="str">
-        <f>LOOKUP(E4,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E4,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G4" s="4"/>
@@ -2592,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A5" s="32">
         <f>RAWDATA!B5</f>
         <v>0</v>
@@ -2611,7 +2618,7 @@
       </c>
       <c r="E5" s="38"/>
       <c r="F5" s="34" t="str">
-        <f>LOOKUP(E5,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E5,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G5" s="4"/>
@@ -2644,7 +2651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A6" s="32">
         <f>RAWDATA!B6</f>
         <v>0</v>
@@ -2663,7 +2670,7 @@
       </c>
       <c r="E6" s="38"/>
       <c r="F6" s="34" t="str">
-        <f>LOOKUP(E6,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E6,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G6" s="4"/>
@@ -2696,7 +2703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A7" s="32">
         <f>RAWDATA!B7</f>
         <v>0</v>
@@ -2715,7 +2722,7 @@
       </c>
       <c r="E7" s="38"/>
       <c r="F7" s="34" t="str">
-        <f>LOOKUP(E7,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E7,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G7" s="4"/>
@@ -2748,7 +2755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A8" s="32">
         <f>RAWDATA!B8</f>
         <v>0</v>
@@ -2767,7 +2774,7 @@
       </c>
       <c r="E8" s="38"/>
       <c r="F8" s="34" t="str">
-        <f>LOOKUP(E8,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E8,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G8" s="4"/>
@@ -2800,7 +2807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A9" s="32">
         <f>RAWDATA!B9</f>
         <v>0</v>
@@ -2819,7 +2826,7 @@
       </c>
       <c r="E9" s="38"/>
       <c r="F9" s="34" t="str">
-        <f>LOOKUP(E9,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E9,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G9" s="4"/>
@@ -2852,7 +2859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A10" s="32">
         <f>RAWDATA!B10</f>
         <v>0</v>
@@ -2871,7 +2878,7 @@
       </c>
       <c r="E10" s="38"/>
       <c r="F10" s="34" t="str">
-        <f>LOOKUP(E10,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E10,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G10" s="4"/>
@@ -2904,7 +2911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A11" s="32">
         <f>RAWDATA!B11</f>
         <v>0</v>
@@ -2923,7 +2930,7 @@
       </c>
       <c r="E11" s="38"/>
       <c r="F11" s="34" t="str">
-        <f>LOOKUP(E11,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E11,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G11" s="4"/>
@@ -2956,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A12" s="32">
         <f>RAWDATA!B12</f>
         <v>0</v>
@@ -2975,7 +2982,7 @@
       </c>
       <c r="E12" s="38"/>
       <c r="F12" s="34" t="str">
-        <f>LOOKUP(E12,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E12,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G12" s="4"/>
@@ -3008,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A13" s="32">
         <f>RAWDATA!B13</f>
         <v>0</v>
@@ -3027,7 +3034,7 @@
       </c>
       <c r="E13" s="38"/>
       <c r="F13" s="34" t="str">
-        <f>LOOKUP(E13,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E13,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G13" s="4"/>
@@ -3060,7 +3067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A14" s="32">
         <f>RAWDATA!B14</f>
         <v>0</v>
@@ -3079,7 +3086,7 @@
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="34" t="str">
-        <f>LOOKUP(E14,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E14,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G14" s="4"/>
@@ -3112,7 +3119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A15" s="32">
         <f>RAWDATA!B15</f>
         <v>0</v>
@@ -3131,7 +3138,7 @@
       </c>
       <c r="E15" s="38"/>
       <c r="F15" s="34" t="str">
-        <f>LOOKUP(E15,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E15,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G15" s="4"/>
@@ -3164,7 +3171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A16" s="32">
         <f>RAWDATA!B16</f>
         <v>0</v>
@@ -3183,7 +3190,7 @@
       </c>
       <c r="E16" s="38"/>
       <c r="F16" s="34" t="str">
-        <f>LOOKUP(E16,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E16,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G16" s="4"/>
@@ -3216,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A17" s="32">
         <f>RAWDATA!B17</f>
         <v>0</v>
@@ -3235,7 +3242,7 @@
       </c>
       <c r="E17" s="38"/>
       <c r="F17" s="34" t="str">
-        <f>LOOKUP(E17,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E17,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G17" s="4"/>
@@ -3268,7 +3275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A18" s="32">
         <f>RAWDATA!B18</f>
         <v>0</v>
@@ -3287,7 +3294,7 @@
       </c>
       <c r="E18" s="38"/>
       <c r="F18" s="34" t="str">
-        <f>LOOKUP(E18,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E18,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G18" s="4"/>
@@ -3320,7 +3327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A19" s="32">
         <f>RAWDATA!B19</f>
         <v>0</v>
@@ -3339,7 +3346,7 @@
       </c>
       <c r="E19" s="38"/>
       <c r="F19" s="34" t="str">
-        <f>LOOKUP(E19,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E19,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G19" s="4"/>
@@ -3372,7 +3379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A20" s="32">
         <f>RAWDATA!B20</f>
         <v>0</v>
@@ -3391,7 +3398,7 @@
       </c>
       <c r="E20" s="38"/>
       <c r="F20" s="34" t="str">
-        <f>LOOKUP(E20,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E20,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G20" s="4"/>
@@ -3424,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A21" s="32">
         <f>RAWDATA!B21</f>
         <v>0</v>
@@ -3443,7 +3450,7 @@
       </c>
       <c r="E21" s="38"/>
       <c r="F21" s="34" t="str">
-        <f>LOOKUP(E21,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E21,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G21" s="4"/>
@@ -3476,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A22" s="32">
         <f>RAWDATA!B22</f>
         <v>0</v>
@@ -3495,7 +3502,7 @@
       </c>
       <c r="E22" s="38"/>
       <c r="F22" s="34" t="str">
-        <f>LOOKUP(E22,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E22,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G22" s="4"/>
@@ -3528,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A23" s="32">
         <f>RAWDATA!B23</f>
         <v>0</v>
@@ -3547,7 +3554,7 @@
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="34" t="str">
-        <f>LOOKUP(E23,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E23,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G23" s="4"/>
@@ -3580,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A24" s="32">
         <f>RAWDATA!B24</f>
         <v>0</v>
@@ -3599,7 +3606,7 @@
       </c>
       <c r="E24" s="38"/>
       <c r="F24" s="34" t="str">
-        <f>LOOKUP(E24,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E24,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G24" s="4"/>
@@ -3632,7 +3639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A25" s="32">
         <f>RAWDATA!B25</f>
         <v>0</v>
@@ -3651,7 +3658,7 @@
       </c>
       <c r="E25" s="38"/>
       <c r="F25" s="34" t="str">
-        <f>LOOKUP(E25,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E25,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G25" s="4"/>
@@ -3667,7 +3674,7 @@
       <c r="N25" s="2"/>
       <c r="O25" s="11"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A26" s="32">
         <f>RAWDATA!B26</f>
         <v>0</v>
@@ -3686,7 +3693,7 @@
       </c>
       <c r="E26" s="38"/>
       <c r="F26" s="34" t="str">
-        <f>LOOKUP(E26,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E26,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G26" s="4"/>
@@ -3702,7 +3709,7 @@
       <c r="N26" s="2"/>
       <c r="O26" s="11"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A27" s="32">
         <f>RAWDATA!B27</f>
         <v>0</v>
@@ -3721,7 +3728,7 @@
       </c>
       <c r="E27" s="38"/>
       <c r="F27" s="34" t="str">
-        <f>LOOKUP(E27,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E27,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G27" s="4"/>
@@ -3737,7 +3744,7 @@
       <c r="N27" s="2"/>
       <c r="O27" s="11"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A28" s="32">
         <f>RAWDATA!B28</f>
         <v>0</v>
@@ -3756,7 +3763,7 @@
       </c>
       <c r="E28" s="38"/>
       <c r="F28" s="34" t="str">
-        <f>LOOKUP(E28,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E28,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G28" s="4"/>
@@ -3772,7 +3779,7 @@
       <c r="N28" s="2"/>
       <c r="O28" s="11"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A29" s="32">
         <f>RAWDATA!B29</f>
         <v>0</v>
@@ -3791,7 +3798,7 @@
       </c>
       <c r="E29" s="38"/>
       <c r="F29" s="34" t="str">
-        <f>LOOKUP(E29,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E29,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G29" s="4"/>
@@ -3807,7 +3814,7 @@
       <c r="N29" s="2"/>
       <c r="O29" s="11"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A30" s="32">
         <f>RAWDATA!B30</f>
         <v>0</v>
@@ -3826,7 +3833,7 @@
       </c>
       <c r="E30" s="38"/>
       <c r="F30" s="34" t="str">
-        <f>LOOKUP(E30,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E30,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G30" s="4"/>
@@ -3842,7 +3849,7 @@
       <c r="N30" s="2"/>
       <c r="O30" s="11"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A31" s="32">
         <f>RAWDATA!B31</f>
         <v>0</v>
@@ -3861,7 +3868,7 @@
       </c>
       <c r="E31" s="38"/>
       <c r="F31" s="34" t="str">
-        <f>LOOKUP(E31,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E31,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G31" s="4"/>
@@ -3877,7 +3884,7 @@
       <c r="N31" s="2"/>
       <c r="O31" s="11"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A32" s="32">
         <f>RAWDATA!B32</f>
         <v>0</v>
@@ -3896,7 +3903,7 @@
       </c>
       <c r="E32" s="38"/>
       <c r="F32" s="34" t="str">
-        <f>LOOKUP(E32,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E32,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G32" s="4"/>
@@ -3912,7 +3919,7 @@
       <c r="N32" s="2"/>
       <c r="O32" s="11"/>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A33" s="32">
         <f>RAWDATA!B33</f>
         <v>0</v>
@@ -3931,7 +3938,7 @@
       </c>
       <c r="E33" s="38"/>
       <c r="F33" s="34" t="str">
-        <f>LOOKUP(E33,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E33,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G33" s="4"/>
@@ -3947,7 +3954,7 @@
       <c r="N33" s="2"/>
       <c r="O33" s="11"/>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A34" s="32">
         <f>RAWDATA!B34</f>
         <v>0</v>
@@ -3966,7 +3973,7 @@
       </c>
       <c r="E34" s="38"/>
       <c r="F34" s="34" t="str">
-        <f>LOOKUP(E34,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E34,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G34" s="4"/>
@@ -3982,7 +3989,7 @@
       <c r="N34" s="2"/>
       <c r="O34" s="11"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A35" s="32">
         <f>RAWDATA!B35</f>
         <v>0</v>
@@ -4001,7 +4008,7 @@
       </c>
       <c r="E35" s="38"/>
       <c r="F35" s="34" t="str">
-        <f>LOOKUP(E35,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E35,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G35" s="4"/>
@@ -4034,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A36" s="32">
         <f>RAWDATA!B36</f>
         <v>0</v>
@@ -4053,7 +4060,7 @@
       </c>
       <c r="E36" s="38"/>
       <c r="F36" s="34" t="str">
-        <f>LOOKUP(E36,{0,1,49.75,55.75,61.75,67.75,72.75,78.75,84.75,89.75,94.75,97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
+        <f>LOOKUP(E36,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
       </c>
       <c r="G36" s="4"/>
@@ -4086,7 +4093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A37" s="4"/>
       <c r="B37" s="4" t="s">
         <v>10</v>
@@ -4105,7 +4112,7 @@
       <c r="L37" s="25"/>
       <c r="Q37" s="13"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
@@ -4121,7 +4128,7 @@
       <c r="L38" s="25"/>
       <c r="Q38" s="13"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A39" s="4"/>
       <c r="B39" s="4" t="s">
         <v>11</v>
@@ -4141,7 +4148,7 @@
       <c r="L39" s="25"/>
       <c r="Q39" s="13"/>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A40" s="25"/>
       <c r="B40" s="25"/>
       <c r="C40" s="26"/>
@@ -4155,11 +4162,13 @@
       <c r="K40" s="25"/>
       <c r="L40" s="25"/>
     </row>
-    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="10"/>
+      <c r="B41" s="10" t="s">
+        <v>53</v>
+      </c>
       <c r="C41" s="26"/>
       <c r="D41" s="75" t="s">
         <v>34</v>
@@ -4173,12 +4182,12 @@
       <c r="K41" s="35"/>
       <c r="L41" s="25"/>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C42" s="26"/>
       <c r="D42" s="75"/>
@@ -4191,7 +4200,7 @@
       <c r="K42" s="35"/>
       <c r="L42" s="25"/>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>16</v>
       </c>
@@ -4209,7 +4218,7 @@
       <c r="K43" s="35"/>
       <c r="L43" s="25"/>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>17</v>
       </c>
@@ -4227,7 +4236,7 @@
       <c r="K44" s="35"/>
       <c r="L44" s="25"/>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
         <v>43</v>
       </c>
@@ -4243,12 +4252,12 @@
       <c r="K45" s="35"/>
       <c r="L45" s="25"/>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
         <v>51</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C46" s="26"/>
       <c r="D46" s="75"/>
@@ -4261,12 +4270,12 @@
       <c r="K46" s="35"/>
       <c r="L46" s="25"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C47" s="26"/>
       <c r="D47" s="75"/>
@@ -4279,7 +4288,7 @@
       <c r="K47" s="35"/>
       <c r="L47" s="25"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
         <v>44</v>
       </c>
@@ -4297,68 +4306,62 @@
       <c r="K48" s="25"/>
       <c r="L48" s="25"/>
     </row>
-    <row r="49" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
-    <row r="50" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
-    <row r="51" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
-    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A52" s="59"/>
     </row>
-    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A53" s="59"/>
     </row>
-    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A54" s="59"/>
     </row>
-    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A55" s="59"/>
     </row>
-    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A56" s="59"/>
     </row>
-    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A57" s="59"/>
     </row>
-    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A58" s="59"/>
     </row>
-    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A59" s="59"/>
     </row>
-    <row r="60" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
-    <row r="61" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
-    <row r="62" spans="1:1" hidden="1" x14ac:dyDescent="0.4"/>
-    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A63" s="59"/>
     </row>
-    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A64" s="59"/>
     </row>
-    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A65" s="59"/>
     </row>
-    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A66" s="59"/>
     </row>
-    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A67" s="59"/>
     </row>
-    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A68" s="59"/>
     </row>
-    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A69" s="59"/>
     </row>
-    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:1" hidden="1" x14ac:dyDescent="0.15">
       <c r="A70" s="59"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.4"/>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0" selectLockedCells="1"/>
+  <sheetProtection sheet="1" formatColumns="0" selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="D41:G48"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Inkorrekte Semesterangabe" error="Bitte wählen Sie aus der Dropdown-Liste aus._x000a__x000a_Ihre Eingabe wird nicht automatisch korrigiert." promptTitle="Semester" prompt="Bitte geben Sie das entsprechende Semester an. Wählen Sie aus der Dropdown-Liste." sqref="B47" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.2598425196850394" bottom="1.0629921259842521" header="0.59055118110236227" footer="0.78740157480314965"/>
@@ -4382,15 +4385,15 @@
       <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.41796875" customWidth="1"/>
-    <col min="2" max="2" width="11.41796875" style="7" customWidth="1"/>
-    <col min="3" max="8" width="11.41796875" customWidth="1"/>
-    <col min="9" max="16384" width="11.41796875" hidden="1"/>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="7" customWidth="1"/>
+    <col min="3" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="16384" width="11.5" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="76" t="str">
         <f>Notenliste!B44</f>
         <v>Arabisch 1</v>
@@ -4404,7 +4407,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
@@ -4412,7 +4415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -4421,7 +4424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>1.3</v>
       </c>
@@ -4430,7 +4433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>1.7</v>
       </c>
@@ -4439,7 +4442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>2</v>
       </c>
@@ -4448,7 +4451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>2.2999999999999998</v>
       </c>
@@ -4457,7 +4460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>2.7</v>
       </c>
@@ -4466,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>3</v>
       </c>
@@ -4475,7 +4478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>3.3</v>
       </c>
@@ -4484,7 +4487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>3.7</v>
       </c>
@@ -4493,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>4</v>
       </c>
@@ -4502,7 +4505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>32</v>
       </c>
@@ -4533,22 +4536,22 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.68359375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="30.68359375" style="21" customWidth="1"/>
-    <col min="4" max="5" width="10.68359375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="39.26171875" style="21" customWidth="1"/>
-    <col min="7" max="7" width="30.68359375" style="21" customWidth="1"/>
-    <col min="8" max="8" width="10.68359375" style="21" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.15625" style="21" hidden="1" customWidth="1"/>
-    <col min="10" max="13" width="10.68359375" style="22" customWidth="1"/>
-    <col min="14" max="14" width="10.68359375" style="21" customWidth="1"/>
-    <col min="15" max="15" width="1.68359375" style="21" customWidth="1"/>
-    <col min="16" max="16384" width="11.41796875" style="21" hidden="1"/>
+    <col min="1" max="1" width="3.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.6640625" style="21" customWidth="1"/>
+    <col min="4" max="5" width="10.6640625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="21" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="21" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="21" hidden="1" customWidth="1"/>
+    <col min="10" max="13" width="10.6640625" style="22" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="21" customWidth="1"/>
+    <col min="15" max="15" width="1.6640625" style="21" customWidth="1"/>
+    <col min="16" max="16384" width="11.5" style="21" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="64" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" s="64" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="77" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
         <v>Arabisch 1</v>
@@ -4567,10 +4570,10 @@
       <c r="M1" s="77"/>
       <c r="N1" s="77"/>
     </row>
-    <row r="2" spans="1:14" s="64" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" s="64" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="78" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
-        <v xml:space="preserve">Dozent/in: </v>
+        <v>Dozent/in: Alaa Khalil</v>
       </c>
       <c r="B2" s="78"/>
       <c r="C2" s="78"/>
@@ -4589,7 +4592,7 @@
       <c r="M2" s="79"/>
       <c r="N2" s="79"/>
     </row>
-    <row r="3" spans="1:14" s="65" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" s="65" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
         <v>26</v>
       </c>
@@ -4633,7 +4636,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -4690,7 +4693,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -4747,7 +4750,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -4804,7 +4807,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>4</v>
       </c>
@@ -4861,7 +4864,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>5</v>
       </c>
@@ -4918,7 +4921,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>6</v>
       </c>
@@ -4975,7 +4978,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>7</v>
       </c>
@@ -5032,7 +5035,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>8</v>
       </c>
@@ -5089,7 +5092,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>9</v>
       </c>
@@ -5146,7 +5149,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>10</v>
       </c>
@@ -5203,7 +5206,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>11</v>
       </c>
@@ -5260,7 +5263,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>12</v>
       </c>
@@ -5317,7 +5320,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>13</v>
       </c>
@@ -5374,7 +5377,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>14</v>
       </c>
@@ -5431,7 +5434,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>15</v>
       </c>
@@ -5488,7 +5491,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>16</v>
       </c>
@@ -5545,7 +5548,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>17</v>
       </c>
@@ -5602,7 +5605,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>18</v>
       </c>
@@ -5659,7 +5662,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>19</v>
       </c>
@@ -5716,7 +5719,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>20</v>
       </c>
@@ -5773,7 +5776,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>21</v>
       </c>
@@ -5830,7 +5833,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>22</v>
       </c>
@@ -5887,7 +5890,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>23</v>
       </c>
@@ -5944,7 +5947,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>24</v>
       </c>
@@ -6001,7 +6004,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>25</v>
       </c>
@@ -6058,7 +6061,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>26</v>
       </c>
@@ -6115,7 +6118,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>27</v>
       </c>
@@ -6172,7 +6175,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>28</v>
       </c>
@@ -6229,7 +6232,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:14" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>29</v>
       </c>
@@ -6286,7 +6289,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>30</v>
       </c>
@@ -6343,7 +6346,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>31</v>
       </c>
@@ -6400,7 +6403,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>32</v>
       </c>
@@ -6457,7 +6460,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>33</v>
       </c>
@@ -6514,7 +6517,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>34</v>
       </c>
@@ -6571,7 +6574,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
         <v>35</v>
       </c>
@@ -6628,7 +6631,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="61"/>
       <c r="B39" s="62"/>
       <c r="C39" s="62"/>
@@ -6650,7 +6653,7 @@
       <c r="M39" s="61"/>
       <c r="N39" s="63"/>
     </row>
-    <row r="40" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="80" t="s">
         <v>42</v>
       </c>
@@ -6668,7 +6671,7 @@
       <c r="M40" s="80"/>
       <c r="N40" s="80"/>
     </row>
-    <row r="41" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="81"/>
       <c r="B41" s="81"/>
       <c r="C41" s="81"/>
@@ -6684,7 +6687,7 @@
       <c r="M41" s="81"/>
       <c r="N41" s="81"/>
     </row>
-    <row r="42" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="81"/>
       <c r="B42" s="81"/>
       <c r="C42" s="81"/>
@@ -6700,7 +6703,7 @@
       <c r="M42" s="81"/>
       <c r="N42" s="81"/>
     </row>
-    <row r="43" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:15" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="81"/>
       <c r="B43" s="81"/>
       <c r="C43" s="81"/>
@@ -6716,7 +6719,7 @@
       <c r="M43" s="81"/>
       <c r="N43" s="81"/>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="81"/>
       <c r="B44" s="81"/>
       <c r="C44" s="81"/>
@@ -6762,24 +6765,24 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.68359375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.578125" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.41796875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="6.41796875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="9.68359375" style="23" customWidth="1"/>
-    <col min="6" max="6" width="0.83984375" style="23" customWidth="1"/>
-    <col min="7" max="20" width="7.68359375" style="23" customWidth="1"/>
-    <col min="21" max="21" width="0.83984375" style="23" customWidth="1"/>
-    <col min="22" max="22" width="10.68359375" style="57" customWidth="1"/>
-    <col min="23" max="23" width="10.68359375" style="58" customWidth="1"/>
-    <col min="24" max="24" width="10.68359375" style="44" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" style="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="21" customWidth="1"/>
+    <col min="4" max="4" width="6.5" style="23" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="0.83203125" style="23" customWidth="1"/>
+    <col min="7" max="20" width="7.6640625" style="23" customWidth="1"/>
+    <col min="21" max="21" width="0.83203125" style="23" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" style="57" customWidth="1"/>
+    <col min="23" max="23" width="10.6640625" style="58" customWidth="1"/>
+    <col min="24" max="24" width="10.6640625" style="44" customWidth="1"/>
     <col min="25" max="31" width="0" style="21" hidden="1" customWidth="1"/>
-    <col min="32" max="16384" width="11.41796875" style="21" hidden="1"/>
+    <col min="32" max="16384" width="11.5" style="21" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:24" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="84" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
         <v>Arabisch 1</v>
@@ -6808,7 +6811,7 @@
       <c r="W1" s="84"/>
       <c r="X1" s="84"/>
     </row>
-    <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:24" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="84" t="s">
         <v>40</v>
       </c>
@@ -6836,10 +6839,10 @@
       <c r="W2" s="84"/>
       <c r="X2" s="84"/>
     </row>
-    <row r="3" spans="1:24" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:24" s="48" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="85" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
-        <v xml:space="preserve">Dozent/in: </v>
+        <v>Dozent/in: Alaa Khalil</v>
       </c>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -6865,7 +6868,7 @@
       <c r="W3" s="86"/>
       <c r="X3" s="86"/>
     </row>
-    <row r="4" spans="1:24" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:24" s="17" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="87" t="s">
         <v>26</v>
       </c>
@@ -6907,7 +6910,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="17" customFormat="1" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="88"/>
       <c r="B5" s="88"/>
       <c r="C5" s="88"/>
@@ -6961,7 +6964,7 @@
       <c r="W5" s="83"/>
       <c r="X5" s="83"/>
     </row>
-    <row r="6" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="18">
         <v>1</v>
       </c>
@@ -7001,7 +7004,7 @@
       <c r="W6" s="56"/>
       <c r="X6" s="56"/>
     </row>
-    <row r="7" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>2</v>
       </c>
@@ -7041,7 +7044,7 @@
       <c r="W7" s="56"/>
       <c r="X7" s="56"/>
     </row>
-    <row r="8" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>3</v>
       </c>
@@ -7081,7 +7084,7 @@
       <c r="W8" s="56"/>
       <c r="X8" s="56"/>
     </row>
-    <row r="9" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>4</v>
       </c>
@@ -7121,7 +7124,7 @@
       <c r="W9" s="56"/>
       <c r="X9" s="56"/>
     </row>
-    <row r="10" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="18">
         <v>5</v>
       </c>
@@ -7161,7 +7164,7 @@
       <c r="W10" s="56"/>
       <c r="X10" s="56"/>
     </row>
-    <row r="11" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="18">
         <v>6</v>
       </c>
@@ -7201,7 +7204,7 @@
       <c r="W11" s="56"/>
       <c r="X11" s="56"/>
     </row>
-    <row r="12" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="18">
         <v>7</v>
       </c>
@@ -7241,7 +7244,7 @@
       <c r="W12" s="56"/>
       <c r="X12" s="56"/>
     </row>
-    <row r="13" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="18">
         <v>8</v>
       </c>
@@ -7281,7 +7284,7 @@
       <c r="W13" s="56"/>
       <c r="X13" s="56"/>
     </row>
-    <row r="14" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="18">
         <v>9</v>
       </c>
@@ -7321,7 +7324,7 @@
       <c r="W14" s="56"/>
       <c r="X14" s="56"/>
     </row>
-    <row r="15" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="18">
         <v>10</v>
       </c>
@@ -7361,7 +7364,7 @@
       <c r="W15" s="56"/>
       <c r="X15" s="56"/>
     </row>
-    <row r="16" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="18">
         <v>11</v>
       </c>
@@ -7401,7 +7404,7 @@
       <c r="W16" s="56"/>
       <c r="X16" s="56"/>
     </row>
-    <row r="17" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="18">
         <v>12</v>
       </c>
@@ -7441,7 +7444,7 @@
       <c r="W17" s="56"/>
       <c r="X17" s="56"/>
     </row>
-    <row r="18" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="18">
         <v>13</v>
       </c>
@@ -7481,7 +7484,7 @@
       <c r="W18" s="56"/>
       <c r="X18" s="56"/>
     </row>
-    <row r="19" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="18">
         <v>14</v>
       </c>
@@ -7521,7 +7524,7 @@
       <c r="W19" s="56"/>
       <c r="X19" s="56"/>
     </row>
-    <row r="20" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="18">
         <v>15</v>
       </c>
@@ -7561,7 +7564,7 @@
       <c r="W20" s="56"/>
       <c r="X20" s="56"/>
     </row>
-    <row r="21" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="18">
         <v>16</v>
       </c>
@@ -7601,7 +7604,7 @@
       <c r="W21" s="56"/>
       <c r="X21" s="56"/>
     </row>
-    <row r="22" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
         <v>17</v>
       </c>
@@ -7641,7 +7644,7 @@
       <c r="W22" s="56"/>
       <c r="X22" s="56"/>
     </row>
-    <row r="23" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
         <v>18</v>
       </c>
@@ -7681,7 +7684,7 @@
       <c r="W23" s="56"/>
       <c r="X23" s="56"/>
     </row>
-    <row r="24" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="18">
         <v>19</v>
       </c>
@@ -7721,7 +7724,7 @@
       <c r="W24" s="56"/>
       <c r="X24" s="56"/>
     </row>
-    <row r="25" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="18">
         <v>20</v>
       </c>
@@ -7761,7 +7764,7 @@
       <c r="W25" s="56"/>
       <c r="X25" s="56"/>
     </row>
-    <row r="26" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="18">
         <v>21</v>
       </c>
@@ -7801,7 +7804,7 @@
       <c r="W26" s="56"/>
       <c r="X26" s="56"/>
     </row>
-    <row r="27" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="18">
         <v>22</v>
       </c>
@@ -7841,7 +7844,7 @@
       <c r="W27" s="56"/>
       <c r="X27" s="56"/>
     </row>
-    <row r="28" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="18">
         <v>23</v>
       </c>
@@ -7881,7 +7884,7 @@
       <c r="W28" s="56"/>
       <c r="X28" s="56"/>
     </row>
-    <row r="29" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="18">
         <v>24</v>
       </c>
@@ -7921,7 +7924,7 @@
       <c r="W29" s="56"/>
       <c r="X29" s="56"/>
     </row>
-    <row r="30" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="18">
         <v>25</v>
       </c>
@@ -7961,7 +7964,7 @@
       <c r="W30" s="56"/>
       <c r="X30" s="56"/>
     </row>
-    <row r="31" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="18">
         <v>26</v>
       </c>
@@ -8001,7 +8004,7 @@
       <c r="W31" s="56"/>
       <c r="X31" s="56"/>
     </row>
-    <row r="32" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="18">
         <v>27</v>
       </c>
@@ -8041,7 +8044,7 @@
       <c r="W32" s="56"/>
       <c r="X32" s="56"/>
     </row>
-    <row r="33" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="18">
         <v>28</v>
       </c>
@@ -8081,7 +8084,7 @@
       <c r="W33" s="56"/>
       <c r="X33" s="56"/>
     </row>
-    <row r="34" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="18">
         <v>29</v>
       </c>
@@ -8121,7 +8124,7 @@
       <c r="W34" s="56"/>
       <c r="X34" s="56"/>
     </row>
-    <row r="35" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="18">
         <v>30</v>
       </c>
@@ -8161,7 +8164,7 @@
       <c r="W35" s="56"/>
       <c r="X35" s="56"/>
     </row>
-    <row r="36" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="18">
         <v>31</v>
       </c>
@@ -8201,7 +8204,7 @@
       <c r="W36" s="56"/>
       <c r="X36" s="56"/>
     </row>
-    <row r="37" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="18">
         <v>32</v>
       </c>
@@ -8241,7 +8244,7 @@
       <c r="W37" s="56"/>
       <c r="X37" s="56"/>
     </row>
-    <row r="38" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="18">
         <v>33</v>
       </c>
@@ -8281,7 +8284,7 @@
       <c r="W38" s="56"/>
       <c r="X38" s="56"/>
     </row>
-    <row r="39" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="18">
         <v>34</v>
       </c>
@@ -8321,7 +8324,7 @@
       <c r="W39" s="56"/>
       <c r="X39" s="56"/>
     </row>
-    <row r="40" spans="1:24" ht="14.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="18">
         <v>35</v>
       </c>
@@ -8392,21 +8395,21 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" style="67" customWidth="1"/>
-    <col min="2" max="2" width="12.83984375" customWidth="1"/>
-    <col min="4" max="4" width="15.578125" style="70" customWidth="1"/>
-    <col min="5" max="5" width="18.15625" style="69" customWidth="1"/>
-    <col min="6" max="6" width="35.578125" customWidth="1"/>
-    <col min="7" max="7" width="31.578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="46.578125" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="70" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="69" customWidth="1"/>
+    <col min="6" max="6" width="35.5" customWidth="1"/>
+    <col min="7" max="7" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="67" t="s">
         <v>27</v>
       </c>
@@ -8432,7 +8435,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="71" t="str">
         <f>IF(Notenliste!D2=0," ",Notenliste!D2)</f>
         <v>applicant.tag</v>
@@ -8454,7 +8457,7 @@
       <c r="G2" s="72"/>
       <c r="H2" s="44"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="71" t="str">
         <f>IF(Notenliste!D3=0," ",Notenliste!D3)</f>
         <v xml:space="preserve"> </v>
@@ -8476,7 +8479,7 @@
       <c r="G3" s="72"/>
       <c r="H3" s="44"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="71" t="str">
         <f>IF(Notenliste!D4=0," ",Notenliste!D4)</f>
         <v xml:space="preserve"> </v>
@@ -8498,7 +8501,7 @@
       <c r="G4" s="72"/>
       <c r="H4" s="44"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="71" t="str">
         <f>IF(Notenliste!D5=0," ",Notenliste!D5)</f>
         <v xml:space="preserve"> </v>
@@ -8520,7 +8523,7 @@
       <c r="G5" s="72"/>
       <c r="H5" s="44"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="71" t="str">
         <f>IF(Notenliste!D6=0," ",Notenliste!D6)</f>
         <v xml:space="preserve"> </v>
@@ -8542,7 +8545,7 @@
       <c r="G6" s="72"/>
       <c r="H6" s="44"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="71" t="str">
         <f>IF(Notenliste!D7=0," ",Notenliste!D7)</f>
         <v xml:space="preserve"> </v>
@@ -8564,7 +8567,7 @@
       <c r="G7" s="72"/>
       <c r="H7" s="44"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="71" t="str">
         <f>IF(Notenliste!D8=0," ",Notenliste!D8)</f>
         <v xml:space="preserve"> </v>
@@ -8586,7 +8589,7 @@
       <c r="G8" s="72"/>
       <c r="H8" s="44"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="71" t="str">
         <f>IF(Notenliste!D9=0," ",Notenliste!D9)</f>
         <v xml:space="preserve"> </v>
@@ -8608,7 +8611,7 @@
       <c r="G9" s="72"/>
       <c r="H9" s="44"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="71" t="str">
         <f>IF(Notenliste!D10=0," ",Notenliste!D10)</f>
         <v xml:space="preserve"> </v>
@@ -8630,7 +8633,7 @@
       <c r="G10" s="72"/>
       <c r="H10" s="44"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="71" t="str">
         <f>IF(Notenliste!D11=0," ",Notenliste!D11)</f>
         <v xml:space="preserve"> </v>
@@ -8652,7 +8655,7 @@
       <c r="G11" s="72"/>
       <c r="H11" s="44"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="71" t="str">
         <f>IF(Notenliste!D12=0," ",Notenliste!D12)</f>
         <v xml:space="preserve"> </v>
@@ -8674,7 +8677,7 @@
       <c r="G12" s="72"/>
       <c r="H12" s="44"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="71" t="str">
         <f>IF(Notenliste!D13=0," ",Notenliste!D13)</f>
         <v xml:space="preserve"> </v>
@@ -8696,7 +8699,7 @@
       <c r="G13" s="72"/>
       <c r="H13" s="44"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="71" t="str">
         <f>IF(Notenliste!D14=0," ",Notenliste!D14)</f>
         <v xml:space="preserve"> </v>
@@ -8718,7 +8721,7 @@
       <c r="G14" s="72"/>
       <c r="H14" s="44"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="71" t="str">
         <f>IF(Notenliste!D15=0," ",Notenliste!D15)</f>
         <v xml:space="preserve"> </v>
@@ -8740,7 +8743,7 @@
       <c r="G15" s="72"/>
       <c r="H15" s="44"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="71" t="str">
         <f>IF(Notenliste!D16=0," ",Notenliste!D16)</f>
         <v xml:space="preserve"> </v>
@@ -8762,7 +8765,7 @@
       <c r="G16" s="72"/>
       <c r="H16" s="44"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="71" t="str">
         <f>IF(Notenliste!D17=0," ",Notenliste!D17)</f>
         <v xml:space="preserve"> </v>
@@ -8784,7 +8787,7 @@
       <c r="G17" s="72"/>
       <c r="H17" s="44"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="71" t="str">
         <f>IF(Notenliste!D18=0," ",Notenliste!D18)</f>
         <v xml:space="preserve"> </v>
@@ -8806,7 +8809,7 @@
       <c r="G18" s="72"/>
       <c r="H18" s="44"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="71" t="str">
         <f>IF(Notenliste!D19=0," ",Notenliste!D19)</f>
         <v xml:space="preserve"> </v>
@@ -8828,7 +8831,7 @@
       <c r="G19" s="72"/>
       <c r="H19" s="44"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="71" t="str">
         <f>IF(Notenliste!D20=0," ",Notenliste!D20)</f>
         <v xml:space="preserve"> </v>
@@ -8850,7 +8853,7 @@
       <c r="G20" s="72"/>
       <c r="H20" s="44"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="71" t="str">
         <f>IF(Notenliste!D21=0," ",Notenliste!D21)</f>
         <v xml:space="preserve"> </v>
@@ -8872,7 +8875,7 @@
       <c r="G21" s="72"/>
       <c r="H21" s="44"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="71" t="str">
         <f>IF(Notenliste!D22=0," ",Notenliste!D22)</f>
         <v xml:space="preserve"> </v>
@@ -8894,7 +8897,7 @@
       <c r="G22" s="72"/>
       <c r="H22" s="44"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="71" t="str">
         <f>IF(Notenliste!D23=0," ",Notenliste!D23)</f>
         <v xml:space="preserve"> </v>
@@ -8916,7 +8919,7 @@
       <c r="G23" s="72"/>
       <c r="H23" s="44"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="71" t="str">
         <f>IF(Notenliste!D24=0," ",Notenliste!D24)</f>
         <v xml:space="preserve"> </v>
@@ -8938,7 +8941,7 @@
       <c r="G24" s="72"/>
       <c r="H24" s="44"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="71" t="str">
         <f>IF(Notenliste!D25=0," ",Notenliste!D25)</f>
         <v xml:space="preserve"> </v>
@@ -8960,7 +8963,7 @@
       <c r="G25" s="72"/>
       <c r="H25" s="44"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="71" t="str">
         <f>IF(Notenliste!D26=0," ",Notenliste!D26)</f>
         <v xml:space="preserve"> </v>
@@ -8982,7 +8985,7 @@
       <c r="G26" s="72"/>
       <c r="H26" s="44"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="71" t="str">
         <f>IF(Notenliste!D27=0," ",Notenliste!D27)</f>
         <v xml:space="preserve"> </v>
@@ -9004,7 +9007,7 @@
       <c r="G27" s="72"/>
       <c r="H27" s="44"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="71" t="str">
         <f>IF(Notenliste!D28=0," ",Notenliste!D28)</f>
         <v xml:space="preserve"> </v>
@@ -9026,7 +9029,7 @@
       <c r="G28" s="72"/>
       <c r="H28" s="44"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="71" t="str">
         <f>IF(Notenliste!D29=0," ",Notenliste!D29)</f>
         <v xml:space="preserve"> </v>
@@ -9048,7 +9051,7 @@
       <c r="G29" s="72"/>
       <c r="H29" s="44"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="71" t="str">
         <f>IF(Notenliste!D30=0," ",Notenliste!D30)</f>
         <v xml:space="preserve"> </v>
@@ -9070,7 +9073,7 @@
       <c r="G30" s="72"/>
       <c r="H30" s="44"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="71" t="str">
         <f>IF(Notenliste!D31=0," ",Notenliste!D31)</f>
         <v xml:space="preserve"> </v>
@@ -9092,7 +9095,7 @@
       <c r="G31" s="72"/>
       <c r="H31" s="44"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="71" t="str">
         <f>IF(Notenliste!D32=0," ",Notenliste!D32)</f>
         <v xml:space="preserve"> </v>
@@ -9114,7 +9117,7 @@
       <c r="G32" s="72"/>
       <c r="H32" s="44"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="71" t="str">
         <f>IF(Notenliste!D33=0," ",Notenliste!D33)</f>
         <v xml:space="preserve"> </v>
@@ -9136,7 +9139,7 @@
       <c r="G33" s="72"/>
       <c r="H33" s="44"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="71" t="str">
         <f>IF(Notenliste!D34=0," ",Notenliste!D34)</f>
         <v xml:space="preserve"> </v>
@@ -9158,7 +9161,7 @@
       <c r="G34" s="72"/>
       <c r="H34" s="44"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="71" t="str">
         <f>IF(Notenliste!D35=0," ",Notenliste!D35)</f>
         <v xml:space="preserve"> </v>
@@ -9180,7 +9183,7 @@
       <c r="G35" s="72"/>
       <c r="H35" s="44"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="71" t="str">
         <f>IF(Notenliste!D36=0," ",Notenliste!D36)</f>
         <v xml:space="preserve"> </v>

</xml_diff>

<commit_message>
Update spanish export template
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/courselist-enhanced.xlsx
+++ b/src/spz/templates/export/courselist-enhanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiasdierich/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tobiasdierich/Code/spz/spz-signup-app/src/spz/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F353F99A-3958-8B4E-B73A-8A9270567995}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B48D5C-8D3A-6B45-95EC-C341B48E4AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="11" r:id="rId1"/>
@@ -804,36 +804,6 @@
   </cellStyles>
   <dxfs count="19">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -873,6 +843,36 @@
     </dxf>
     <dxf>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1145,40 +1145,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB3762C0-B84C-7842-884D-F1AF8DEB89A7}" name="DATA" displayName="DATA" ref="B1:G2" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DB3762C0-B84C-7842-884D-F1AF8DEB89A7}" name="DATA" displayName="DATA" ref="B1:G2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="B1:G2" xr:uid="{CC3A94DF-ED58-BC4D-81B4-531D123D1578}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0C760751-8195-ED40-BAD1-1742CEDD2F2A}" name="Nachname" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{D514A574-7540-8D48-AA1C-519DDA696DBD}" name="Vorname" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{9DDCA179-D1CF-BD4C-A77C-AADB4AE9A4AE}" name="Hochschule" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{3FDFBCBF-BABE-7240-8A25-C665ECC07111}" name="Matrikelnummer" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{1844E8D5-5CA1-8448-8686-148586CBBBFC}" name="E-Mail" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{E23CCDE5-D5A2-6149-A990-1E8F99CDA73B}" name="Telefon" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0C760751-8195-ED40-BAD1-1742CEDD2F2A}" name="Nachname" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{D514A574-7540-8D48-AA1C-519DDA696DBD}" name="Vorname" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{9DDCA179-D1CF-BD4C-A77C-AADB4AE9A4AE}" name="Hochschule" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{3FDFBCBF-BABE-7240-8A25-C665ECC07111}" name="Matrikelnummer" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{1844E8D5-5CA1-8448-8686-148586CBBBFC}" name="E-Mail" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{E23CCDE5-D5A2-6149-A990-1E8F99CDA73B}" name="Telefon" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:H36" totalsRowShown="0" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A1:H36" totalsRowShown="0" dataDxfId="10">
   <autoFilter ref="A1:H36" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Matrikelnummer" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Matrikelnummer" dataDxfId="9" totalsRowDxfId="8">
       <calculatedColumnFormula>IF(Notenliste!D2=0," ",Notenliste!D2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Status" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="LP" dataDxfId="14">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Status" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="LP" dataDxfId="6">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$43," ")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Note" dataDxfId="13" totalsRowDxfId="12">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Note" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",Notenliste!F2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Datum" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Datum" dataDxfId="3">
       <calculatedColumnFormula>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$48," ")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Individueller Titel deutsch" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Individueller Titel englisch" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Anmerkungen" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Individueller Titel deutsch" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Individueller Titel englisch" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Anmerkungen" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1507,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -1839,7 +1839,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatColumns="0" selectLockedCells="1"/>
+  <sheetProtection sheet="1" formatColumns="0" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1854,8 +1854,8 @@
   </sheetPr>
   <dimension ref="A1:WVW71"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="13" zeroHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
correct course name and alternative in excel export templates
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/courselist-enhanced.xlsx
+++ b/src/spz/templates/export/courselist-enhanced.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hiwi\Datenbank\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69F35E5-CFCC-4CEC-B6FD-09307D39C444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F18CCA8-9678-4B1E-A0A9-240DDF0D2E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="11" r:id="rId1"/>
@@ -289,22 +289,22 @@
     <t>course.ger</t>
   </si>
   <si>
-    <t>course.full_name</t>
-  </si>
-  <si>
     <t>semester</t>
-  </si>
-  <si>
-    <t>course.full_name_english</t>
-  </si>
-  <si>
-    <t>course.level</t>
   </si>
   <si>
     <t>course.ects_points</t>
   </si>
   <si>
     <t>exam_date</t>
+  </si>
+  <si>
+    <t>course.name</t>
+  </si>
+  <si>
+    <t>course.name_english</t>
+  </si>
+  <si>
+    <t>course.alternative</t>
   </si>
 </sst>
 </file>
@@ -1847,7 +1847,7 @@
   <dimension ref="A1:WVW71"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -4194,7 +4194,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="67"/>
@@ -4212,7 +4212,7 @@
         <v>17</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="67"/>
@@ -4230,7 +4230,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="67"/>
@@ -4248,7 +4248,7 @@
         <v>51</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="67"/>
@@ -4266,7 +4266,7 @@
         <v>33</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="67"/>
@@ -4284,7 +4284,7 @@
         <v>44</v>
       </c>
       <c r="B48" s="60" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="67"/>
@@ -4387,7 +4387,7 @@
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="68" t="str">
         <f>Notenliste!B44</f>
-        <v>course.full_name</v>
+        <v>course.name</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="8" t="s">
@@ -4545,7 +4545,7 @@
     <row r="1" spans="1:14" s="58" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="69" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
-        <v>course.full_namecourse.level</v>
+        <v>course.namecourse.alternative</v>
       </c>
       <c r="B1" s="69"/>
       <c r="C1" s="69"/>
@@ -6776,7 +6776,7 @@
     <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="75" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
-        <v>course.full_namecourse.level</v>
+        <v>course.namecourse.alternative</v>
       </c>
       <c r="B1" s="75"/>
       <c r="C1" s="75"/>

</xml_diff>

<commit_message>
write grade to export templates, add english template
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/courselist-enhanced.xlsx
+++ b/src/spz/templates/export/courselist-enhanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hiwi\Datenbank\excel_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\04_Hiwi\Datenbank\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F18CCA8-9678-4B1E-A0A9-240DDF0D2E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D009D7-03F3-407D-A160-B7844263A5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="11" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -265,9 +265,6 @@
     <t>Arabisch 1</t>
   </si>
   <si>
-    <t>Alaa Khalil</t>
-  </si>
-  <si>
     <t>applicant.last_name</t>
   </si>
   <si>
@@ -305,6 +302,9 @@
   </si>
   <si>
     <t>course.alternative</t>
+  </si>
+  <si>
+    <t>applicant.sanitized_grade</t>
   </si>
 </sst>
 </file>
@@ -791,10 +791,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="20">
     <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -858,6 +858,9 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -887,7 +890,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1137,13 +1140,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DATA" displayName="DATA" ref="B1:G2" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
-  <autoFilter ref="B1:G2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nachname" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Vorname" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hochschule" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Matrikelnummer" dataDxfId="13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DATA" displayName="DATA" ref="B1:H2" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="B1:H2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nachname" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Vorname" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hochschule" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Matrikelnummer" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{DF1C2C88-275C-4D8A-BD91-B3992E33C931}" name="Note" dataDxfId="13"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="E-Mail" dataDxfId="12"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Telefon" dataDxfId="11"/>
   </tableColumns>
@@ -1177,9 +1181,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1217,9 +1221,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1252,26 +1256,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1304,26 +1291,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1497,27 +1467,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.44140625" style="39" customWidth="1"/>
     <col min="3" max="3" width="26.109375" style="39" customWidth="1"/>
     <col min="4" max="4" width="13.109375" style="39" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" style="40" customWidth="1"/>
-    <col min="6" max="6" width="31.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.88671875" style="39" customWidth="1"/>
-    <col min="8" max="8" width="45.109375" style="39" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.44140625" style="39" hidden="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.44140625" hidden="1"/>
+    <col min="6" max="6" width="9" style="40" customWidth="1"/>
+    <col min="7" max="7" width="31.88671875" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.88671875" style="39" customWidth="1"/>
+    <col min="9" max="9" width="45.109375" style="39" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" style="39" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.44140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>26</v>
       </c>
@@ -1533,279 +1504,307 @@
       <c r="E1" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="D2" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="E2" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="F2" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="H2" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="39" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="39" t="s">
+      <c r="I2" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="E3" s="39"/>
-      <c r="H3" s="39" t="s">
+      <c r="F3" s="39"/>
+      <c r="I3" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="E4" s="39"/>
-      <c r="H4" s="39" t="s">
+      <c r="F4" s="39"/>
+      <c r="I4" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="E5" s="39"/>
-      <c r="H5" s="39" t="s">
+      <c r="F5" s="39"/>
+      <c r="I5" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="E6" s="39"/>
-      <c r="H6" s="39" t="s">
+      <c r="F6" s="39"/>
+      <c r="I6" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="E7" s="39"/>
-      <c r="H7" s="39" t="s">
+      <c r="F7" s="39"/>
+      <c r="I7" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="E8" s="39"/>
-      <c r="H8" s="39" t="s">
+      <c r="F8" s="39"/>
+      <c r="I8" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="E9" s="39"/>
-      <c r="H9" s="39" t="s">
+      <c r="F9" s="39"/>
+      <c r="I9" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="E10" s="39"/>
-      <c r="H10" s="39" t="s">
+      <c r="F10" s="39"/>
+      <c r="I10" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="E11" s="39"/>
-      <c r="H11" s="39" t="s">
+      <c r="F11" s="39"/>
+      <c r="I11" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="E12" s="39"/>
-      <c r="H12" s="39" t="s">
+      <c r="F12" s="39"/>
+      <c r="I12" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="E13" s="39"/>
-      <c r="H13" s="39" t="s">
+      <c r="F13" s="39"/>
+      <c r="I13" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="E14" s="39"/>
-      <c r="H14" s="39" t="s">
+      <c r="F14" s="39"/>
+      <c r="I14" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="E15" s="39"/>
-      <c r="H15" s="39" t="s">
+      <c r="F15" s="39"/>
+      <c r="I15" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="E16" s="39"/>
-      <c r="H16" s="39" t="s">
+      <c r="F16" s="39"/>
+      <c r="I16" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="E17" s="39"/>
-      <c r="H17" s="39" t="s">
+      <c r="F17" s="39"/>
+      <c r="I17" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="E18" s="39"/>
-      <c r="H18" s="39" t="s">
+      <c r="F18" s="39"/>
+      <c r="I18" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="E19" s="39"/>
-      <c r="H19" s="39" t="s">
+      <c r="F19" s="39"/>
+      <c r="I19" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="E20" s="39"/>
-      <c r="H20" s="39" t="s">
+      <c r="F20" s="39"/>
+      <c r="I20" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="E21" s="39"/>
-      <c r="H21" s="39" t="s">
+      <c r="F21" s="39"/>
+      <c r="I21" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="E22" s="39"/>
-      <c r="H22" s="39" t="s">
+      <c r="F22" s="39"/>
+      <c r="I22" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="E23" s="39"/>
-      <c r="H23" s="39" t="s">
+      <c r="F23" s="39"/>
+      <c r="I23" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="E24" s="39"/>
-      <c r="H24" s="39" t="s">
+      <c r="F24" s="39"/>
+      <c r="I24" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1846,11 +1845,11 @@
   </sheetPr>
   <dimension ref="A1:WVW71"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="27.44140625" style="1" customWidth="1"/>
@@ -2452,35 +2451,38 @@
         <f>RAWDATA!E2</f>
         <v>applicant.tag</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="30" t="str">
+      <c r="E2" s="34" t="str">
+        <f>RAWDATA!F2</f>
+        <v>applicant.sanitized_grade</v>
+      </c>
+      <c r="F2" s="30" t="e">
         <f>LOOKUP(E2,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
-        <v>KP</v>
+        <v>#N/A</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="35"/>
       <c r="I2" s="33" t="str">
         <f t="shared" ref="I2" si="0">IF(E2&gt;0,"X","")</f>
-        <v/>
+        <v>X</v>
       </c>
       <c r="J2" s="35"/>
       <c r="K2" s="4"/>
       <c r="L2" s="22"/>
-      <c r="M2" s="2">
+      <c r="M2" s="2" t="str">
         <f>IF(E2&gt;0,$B$43,0)</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
+        <v>course.ects_points</v>
+      </c>
+      <c r="N2" s="2" t="str">
         <f>IF(E2&gt;0,$B$42,0)</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="11">
+        <v>course.ger</v>
+      </c>
+      <c r="O2" s="11" t="e">
         <f>IF(E2&gt;0,$F$38,0)</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P2" s="1" t="str">
         <f>IF(E2&gt;0,$B$44,0)</f>
-        <v>0</v>
+        <v>course.name</v>
       </c>
       <c r="Q2" s="1">
         <f>IF(E2&gt;0,$B$41,0)</f>
@@ -2504,7 +2506,10 @@
         <f>RAWDATA!E3</f>
         <v>0</v>
       </c>
-      <c r="E3" s="34"/>
+      <c r="E3" s="34">
+        <f>RAWDATA!F3</f>
+        <v>0</v>
+      </c>
       <c r="F3" s="30" t="str">
         <f>LOOKUP(E3,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2556,7 +2561,10 @@
         <f>RAWDATA!E4</f>
         <v>0</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="34">
+        <f>RAWDATA!F4</f>
+        <v>0</v>
+      </c>
       <c r="F4" s="30" t="str">
         <f>LOOKUP(E4,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2608,7 +2616,10 @@
         <f>RAWDATA!E5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="34"/>
+      <c r="E5" s="34">
+        <f>RAWDATA!F5</f>
+        <v>0</v>
+      </c>
       <c r="F5" s="30" t="str">
         <f>LOOKUP(E5,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2660,7 +2671,10 @@
         <f>RAWDATA!E6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="34"/>
+      <c r="E6" s="34">
+        <f>RAWDATA!F6</f>
+        <v>0</v>
+      </c>
       <c r="F6" s="30" t="str">
         <f>LOOKUP(E6,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2712,7 +2726,10 @@
         <f>RAWDATA!E7</f>
         <v>0</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="34">
+        <f>RAWDATA!F7</f>
+        <v>0</v>
+      </c>
       <c r="F7" s="30" t="str">
         <f>LOOKUP(E7,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2764,7 +2781,10 @@
         <f>RAWDATA!E8</f>
         <v>0</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="34">
+        <f>RAWDATA!F8</f>
+        <v>0</v>
+      </c>
       <c r="F8" s="30" t="str">
         <f>LOOKUP(E8,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2816,7 +2836,10 @@
         <f>RAWDATA!E9</f>
         <v>0</v>
       </c>
-      <c r="E9" s="34"/>
+      <c r="E9" s="34">
+        <f>RAWDATA!F9</f>
+        <v>0</v>
+      </c>
       <c r="F9" s="30" t="str">
         <f>LOOKUP(E9,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2868,7 +2891,10 @@
         <f>RAWDATA!E10</f>
         <v>0</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="34">
+        <f>RAWDATA!F10</f>
+        <v>0</v>
+      </c>
       <c r="F10" s="30" t="str">
         <f>LOOKUP(E10,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2920,7 +2946,10 @@
         <f>RAWDATA!E11</f>
         <v>0</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="34">
+        <f>RAWDATA!F11</f>
+        <v>0</v>
+      </c>
       <c r="F11" s="30" t="str">
         <f>LOOKUP(E11,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -2972,7 +3001,10 @@
         <f>RAWDATA!E12</f>
         <v>0</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="34">
+        <f>RAWDATA!F12</f>
+        <v>0</v>
+      </c>
       <c r="F12" s="30" t="str">
         <f>LOOKUP(E12,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3024,7 +3056,10 @@
         <f>RAWDATA!E13</f>
         <v>0</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="E13" s="34">
+        <f>RAWDATA!F13</f>
+        <v>0</v>
+      </c>
       <c r="F13" s="30" t="str">
         <f>LOOKUP(E13,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3076,7 +3111,10 @@
         <f>RAWDATA!E14</f>
         <v>0</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="34">
+        <f>RAWDATA!F14</f>
+        <v>0</v>
+      </c>
       <c r="F14" s="30" t="str">
         <f>LOOKUP(E14,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3128,7 +3166,10 @@
         <f>RAWDATA!E15</f>
         <v>0</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="34">
+        <f>RAWDATA!F15</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="30" t="str">
         <f>LOOKUP(E15,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3180,7 +3221,10 @@
         <f>RAWDATA!E16</f>
         <v>0</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="34">
+        <f>RAWDATA!F16</f>
+        <v>0</v>
+      </c>
       <c r="F16" s="30" t="str">
         <f>LOOKUP(E16,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3232,7 +3276,10 @@
         <f>RAWDATA!E17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="34">
+        <f>RAWDATA!F17</f>
+        <v>0</v>
+      </c>
       <c r="F17" s="30" t="str">
         <f>LOOKUP(E17,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3284,7 +3331,10 @@
         <f>RAWDATA!E18</f>
         <v>0</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="E18" s="34">
+        <f>RAWDATA!F18</f>
+        <v>0</v>
+      </c>
       <c r="F18" s="30" t="str">
         <f>LOOKUP(E18,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3336,7 +3386,10 @@
         <f>RAWDATA!E19</f>
         <v>0</v>
       </c>
-      <c r="E19" s="34"/>
+      <c r="E19" s="34">
+        <f>RAWDATA!F19</f>
+        <v>0</v>
+      </c>
       <c r="F19" s="30" t="str">
         <f>LOOKUP(E19,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3388,7 +3441,10 @@
         <f>RAWDATA!E20</f>
         <v>0</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="34">
+        <f>RAWDATA!F20</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="30" t="str">
         <f>LOOKUP(E20,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3440,7 +3496,10 @@
         <f>RAWDATA!E21</f>
         <v>0</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="E21" s="34">
+        <f>RAWDATA!F21</f>
+        <v>0</v>
+      </c>
       <c r="F21" s="30" t="str">
         <f>LOOKUP(E21,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3492,7 +3551,10 @@
         <f>RAWDATA!E22</f>
         <v>0</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="E22" s="34">
+        <f>RAWDATA!F22</f>
+        <v>0</v>
+      </c>
       <c r="F22" s="30" t="str">
         <f>LOOKUP(E22,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3544,7 +3606,10 @@
         <f>RAWDATA!E23</f>
         <v>0</v>
       </c>
-      <c r="E23" s="34"/>
+      <c r="E23" s="34">
+        <f>RAWDATA!F23</f>
+        <v>0</v>
+      </c>
       <c r="F23" s="30" t="str">
         <f>LOOKUP(E23,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3596,7 +3661,10 @@
         <f>RAWDATA!E24</f>
         <v>0</v>
       </c>
-      <c r="E24" s="34"/>
+      <c r="E24" s="34">
+        <f>RAWDATA!F24</f>
+        <v>0</v>
+      </c>
       <c r="F24" s="30" t="str">
         <f>LOOKUP(E24,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3648,7 +3716,10 @@
         <f>RAWDATA!E25</f>
         <v>0</v>
       </c>
-      <c r="E25" s="34"/>
+      <c r="E25" s="34">
+        <f>RAWDATA!F25</f>
+        <v>0</v>
+      </c>
       <c r="F25" s="30" t="str">
         <f>LOOKUP(E25,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3683,7 +3754,10 @@
         <f>RAWDATA!E26</f>
         <v>0</v>
       </c>
-      <c r="E26" s="34"/>
+      <c r="E26" s="34">
+        <f>RAWDATA!F26</f>
+        <v>0</v>
+      </c>
       <c r="F26" s="30" t="str">
         <f>LOOKUP(E26,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3718,7 +3792,10 @@
         <f>RAWDATA!E27</f>
         <v>0</v>
       </c>
-      <c r="E27" s="34"/>
+      <c r="E27" s="34">
+        <f>RAWDATA!F27</f>
+        <v>0</v>
+      </c>
       <c r="F27" s="30" t="str">
         <f>LOOKUP(E27,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3753,7 +3830,10 @@
         <f>RAWDATA!E28</f>
         <v>0</v>
       </c>
-      <c r="E28" s="34"/>
+      <c r="E28" s="34">
+        <f>RAWDATA!F28</f>
+        <v>0</v>
+      </c>
       <c r="F28" s="30" t="str">
         <f>LOOKUP(E28,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3788,7 +3868,10 @@
         <f>RAWDATA!E29</f>
         <v>0</v>
       </c>
-      <c r="E29" s="34"/>
+      <c r="E29" s="34">
+        <f>RAWDATA!F29</f>
+        <v>0</v>
+      </c>
       <c r="F29" s="30" t="str">
         <f>LOOKUP(E29,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3823,7 +3906,10 @@
         <f>RAWDATA!E30</f>
         <v>0</v>
       </c>
-      <c r="E30" s="34"/>
+      <c r="E30" s="34">
+        <f>RAWDATA!F30</f>
+        <v>0</v>
+      </c>
       <c r="F30" s="30" t="str">
         <f>LOOKUP(E30,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3858,7 +3944,10 @@
         <f>RAWDATA!E31</f>
         <v>0</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="34">
+        <f>RAWDATA!F31</f>
+        <v>0</v>
+      </c>
       <c r="F31" s="30" t="str">
         <f>LOOKUP(E31,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3893,7 +3982,10 @@
         <f>RAWDATA!E32</f>
         <v>0</v>
       </c>
-      <c r="E32" s="34"/>
+      <c r="E32" s="34">
+        <f>RAWDATA!F32</f>
+        <v>0</v>
+      </c>
       <c r="F32" s="30" t="str">
         <f>LOOKUP(E32,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3928,7 +4020,10 @@
         <f>RAWDATA!E33</f>
         <v>0</v>
       </c>
-      <c r="E33" s="34"/>
+      <c r="E33" s="34">
+        <f>RAWDATA!F33</f>
+        <v>0</v>
+      </c>
       <c r="F33" s="30" t="str">
         <f>LOOKUP(E33,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3963,7 +4058,10 @@
         <f>RAWDATA!E34</f>
         <v>0</v>
       </c>
-      <c r="E34" s="34"/>
+      <c r="E34" s="34">
+        <f>RAWDATA!F34</f>
+        <v>0</v>
+      </c>
       <c r="F34" s="30" t="str">
         <f>LOOKUP(E34,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -3998,7 +4096,10 @@
         <f>RAWDATA!E35</f>
         <v>0</v>
       </c>
-      <c r="E35" s="34"/>
+      <c r="E35" s="34">
+        <f>RAWDATA!F35</f>
+        <v>0</v>
+      </c>
       <c r="F35" s="30" t="str">
         <f>LOOKUP(E35,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -4050,7 +4151,10 @@
         <f>RAWDATA!E36</f>
         <v>0</v>
       </c>
-      <c r="E36" s="34"/>
+      <c r="E36" s="34">
+        <f>RAWDATA!F36</f>
+        <v>0</v>
+      </c>
       <c r="F36" s="30" t="str">
         <f>LOOKUP(E36,{0;1;49.75;55.75;61.75;67.75;72.75;78.75;84.75;89.75;94.75;97.75},{"KP";"NB";4;3.7;3.3;3;2.7;2.3;2;1.7;1.3;1})</f>
         <v>KP</v>
@@ -4128,7 +4232,7 @@
       <c r="E39" s="9"/>
       <c r="F39" s="5" t="e">
         <f>ROUNDUP(STDEVP(F2:F18),1)</f>
-        <v>#DIV/0!</v>
+        <v>#N/A</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -4155,9 +4259,7 @@
       <c r="A41" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>53</v>
-      </c>
+      <c r="B41" s="10"/>
       <c r="C41" s="23"/>
       <c r="D41" s="67" t="s">
         <v>34</v>
@@ -4176,7 +4278,7 @@
         <v>15</v>
       </c>
       <c r="B42" s="36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="23"/>
       <c r="D42" s="67"/>
@@ -4194,7 +4296,7 @@
         <v>16</v>
       </c>
       <c r="B43" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C43" s="23"/>
       <c r="D43" s="67"/>
@@ -4212,7 +4314,7 @@
         <v>17</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" s="23"/>
       <c r="D44" s="67"/>
@@ -4230,7 +4332,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C45" s="23"/>
       <c r="D45" s="67"/>
@@ -4248,7 +4350,7 @@
         <v>51</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="23"/>
       <c r="D46" s="67"/>
@@ -4266,7 +4368,7 @@
         <v>33</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="67"/>
@@ -4284,7 +4386,7 @@
         <v>44</v>
       </c>
       <c r="B48" s="60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="23"/>
       <c r="D48" s="67"/>
@@ -4352,7 +4454,7 @@
   <mergeCells count="1">
     <mergeCell ref="D41:G48"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Inkorrekte Semesterangabe" error="Bitte wählen Sie aus der Dropdown-Liste aus._x000a__x000a_Ihre Eingabe wird nicht automatisch korrigiert." promptTitle="Semester" prompt="Bitte geben Sie das entsprechende Semester an. Wählen Sie aus der Dropdown-Liste." sqref="B47" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="1.2598425196850394" bottom="1.0629921259842521" header="0.59055118110236227" footer="0.78740157480314965"/>
@@ -4376,7 +4478,7 @@
       <selection activeCell="A39" sqref="A39:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" style="7" customWidth="1"/>
@@ -4527,7 +4629,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.6640625" customWidth="1"/>
@@ -4564,7 +4666,7 @@
     <row r="2" spans="1:14" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
-        <v>Dozent/in: Alaa Khalil</v>
+        <v xml:space="preserve">Dozent/in: </v>
       </c>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
@@ -4648,36 +4750,36 @@
         <v>applicant.tag</v>
       </c>
       <c r="F4" s="18" t="str">
-        <f>RAWDATA!F2</f>
+        <f>RAWDATA!G2</f>
         <v>applicant.mail</v>
       </c>
       <c r="G4" s="18" t="str">
-        <f>RAWDATA!G2</f>
+        <f>RAWDATA!H2</f>
         <v>applicant.phone</v>
       </c>
       <c r="H4" s="19" t="str">
-        <f>RAWDATA!H2</f>
+        <f>RAWDATA!I2</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I4" s="19">
-        <f>RAWDATA!I2</f>
+        <f>RAWDATA!J2</f>
         <v>0</v>
       </c>
       <c r="J4" s="17" t="str">
         <f>UPPER(Notenliste!H2)</f>
         <v/>
       </c>
-      <c r="K4" s="17" t="str">
+      <c r="K4" s="17" t="e">
         <f>IF(L4&lt;=4,"X","")</f>
-        <v/>
-      </c>
-      <c r="L4" s="17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L4" s="17" t="e">
         <f>Notenliste!F2</f>
-        <v>KP</v>
-      </c>
-      <c r="M4" s="17">
+        <v>#N/A</v>
+      </c>
+      <c r="M4" s="17" t="str">
         <f>Notenliste!E2</f>
-        <v>0</v>
+        <v>applicant.sanitized_grade</v>
       </c>
       <c r="N4" s="19" t="str">
         <f>UPPER(Notenliste!J2)</f>
@@ -4705,19 +4807,19 @@
         <v>0</v>
       </c>
       <c r="F5" s="18">
-        <f>RAWDATA!F3</f>
+        <f>RAWDATA!G3</f>
         <v>0</v>
       </c>
       <c r="G5" s="18">
-        <f>RAWDATA!G3</f>
+        <f>RAWDATA!H3</f>
         <v>0</v>
       </c>
       <c r="H5" s="19" t="str">
-        <f>RAWDATA!H3</f>
+        <f>RAWDATA!I3</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I5" s="19">
-        <f>RAWDATA!I3</f>
+        <f>RAWDATA!J3</f>
         <v>0</v>
       </c>
       <c r="J5" s="17" t="str">
@@ -4762,19 +4864,19 @@
         <v>0</v>
       </c>
       <c r="F6" s="18">
-        <f>RAWDATA!F4</f>
+        <f>RAWDATA!G4</f>
         <v>0</v>
       </c>
       <c r="G6" s="18">
-        <f>RAWDATA!G4</f>
+        <f>RAWDATA!H4</f>
         <v>0</v>
       </c>
       <c r="H6" s="19" t="str">
-        <f>RAWDATA!H4</f>
+        <f>RAWDATA!I4</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I6" s="19">
-        <f>RAWDATA!I4</f>
+        <f>RAWDATA!J4</f>
         <v>0</v>
       </c>
       <c r="J6" s="17" t="str">
@@ -4819,19 +4921,19 @@
         <v>0</v>
       </c>
       <c r="F7" s="18">
-        <f>RAWDATA!F5</f>
+        <f>RAWDATA!G5</f>
         <v>0</v>
       </c>
       <c r="G7" s="18">
-        <f>RAWDATA!G5</f>
+        <f>RAWDATA!H5</f>
         <v>0</v>
       </c>
       <c r="H7" s="19" t="str">
-        <f>RAWDATA!H5</f>
+        <f>RAWDATA!I5</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I7" s="19">
-        <f>RAWDATA!I5</f>
+        <f>RAWDATA!J5</f>
         <v>0</v>
       </c>
       <c r="J7" s="17" t="str">
@@ -4876,19 +4978,19 @@
         <v>0</v>
       </c>
       <c r="F8" s="18">
-        <f>RAWDATA!F6</f>
+        <f>RAWDATA!G6</f>
         <v>0</v>
       </c>
       <c r="G8" s="18">
-        <f>RAWDATA!G6</f>
+        <f>RAWDATA!H6</f>
         <v>0</v>
       </c>
       <c r="H8" s="19" t="str">
-        <f>RAWDATA!H6</f>
+        <f>RAWDATA!I6</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I8" s="19">
-        <f>RAWDATA!I6</f>
+        <f>RAWDATA!J6</f>
         <v>0</v>
       </c>
       <c r="J8" s="17" t="str">
@@ -4933,19 +5035,19 @@
         <v>0</v>
       </c>
       <c r="F9" s="18">
-        <f>RAWDATA!F7</f>
+        <f>RAWDATA!G7</f>
         <v>0</v>
       </c>
       <c r="G9" s="18">
-        <f>RAWDATA!G7</f>
+        <f>RAWDATA!H7</f>
         <v>0</v>
       </c>
       <c r="H9" s="19" t="str">
-        <f>RAWDATA!H7</f>
+        <f>RAWDATA!I7</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I9" s="19">
-        <f>RAWDATA!I7</f>
+        <f>RAWDATA!J7</f>
         <v>0</v>
       </c>
       <c r="J9" s="17" t="str">
@@ -4990,19 +5092,19 @@
         <v>0</v>
       </c>
       <c r="F10" s="18">
-        <f>RAWDATA!F8</f>
+        <f>RAWDATA!G8</f>
         <v>0</v>
       </c>
       <c r="G10" s="18">
-        <f>RAWDATA!G8</f>
+        <f>RAWDATA!H8</f>
         <v>0</v>
       </c>
       <c r="H10" s="19" t="str">
-        <f>RAWDATA!H8</f>
+        <f>RAWDATA!I8</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I10" s="19">
-        <f>RAWDATA!I8</f>
+        <f>RAWDATA!J8</f>
         <v>0</v>
       </c>
       <c r="J10" s="17" t="str">
@@ -5047,19 +5149,19 @@
         <v>0</v>
       </c>
       <c r="F11" s="18">
-        <f>RAWDATA!F9</f>
+        <f>RAWDATA!G9</f>
         <v>0</v>
       </c>
       <c r="G11" s="18">
-        <f>RAWDATA!G9</f>
+        <f>RAWDATA!H9</f>
         <v>0</v>
       </c>
       <c r="H11" s="19" t="str">
-        <f>RAWDATA!H9</f>
+        <f>RAWDATA!I9</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I11" s="19">
-        <f>RAWDATA!I9</f>
+        <f>RAWDATA!J9</f>
         <v>0</v>
       </c>
       <c r="J11" s="17" t="str">
@@ -5104,19 +5206,19 @@
         <v>0</v>
       </c>
       <c r="F12" s="18">
-        <f>RAWDATA!F10</f>
+        <f>RAWDATA!G10</f>
         <v>0</v>
       </c>
       <c r="G12" s="18">
-        <f>RAWDATA!G10</f>
+        <f>RAWDATA!H10</f>
         <v>0</v>
       </c>
       <c r="H12" s="19" t="str">
-        <f>RAWDATA!H10</f>
+        <f>RAWDATA!I10</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I12" s="19">
-        <f>RAWDATA!I10</f>
+        <f>RAWDATA!J10</f>
         <v>0</v>
       </c>
       <c r="J12" s="17" t="str">
@@ -5161,19 +5263,19 @@
         <v>0</v>
       </c>
       <c r="F13" s="18">
-        <f>RAWDATA!F11</f>
+        <f>RAWDATA!G11</f>
         <v>0</v>
       </c>
       <c r="G13" s="18">
-        <f>RAWDATA!G11</f>
+        <f>RAWDATA!H11</f>
         <v>0</v>
       </c>
       <c r="H13" s="19" t="str">
-        <f>RAWDATA!H11</f>
+        <f>RAWDATA!I11</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I13" s="19">
-        <f>RAWDATA!I11</f>
+        <f>RAWDATA!J11</f>
         <v>0</v>
       </c>
       <c r="J13" s="17" t="str">
@@ -5218,19 +5320,19 @@
         <v>0</v>
       </c>
       <c r="F14" s="18">
-        <f>RAWDATA!F12</f>
+        <f>RAWDATA!G12</f>
         <v>0</v>
       </c>
       <c r="G14" s="18">
-        <f>RAWDATA!G12</f>
+        <f>RAWDATA!H12</f>
         <v>0</v>
       </c>
       <c r="H14" s="19" t="str">
-        <f>RAWDATA!H12</f>
+        <f>RAWDATA!I12</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I14" s="19">
-        <f>RAWDATA!I12</f>
+        <f>RAWDATA!J12</f>
         <v>0</v>
       </c>
       <c r="J14" s="17" t="str">
@@ -5275,19 +5377,19 @@
         <v>0</v>
       </c>
       <c r="F15" s="18">
-        <f>RAWDATA!F13</f>
+        <f>RAWDATA!G13</f>
         <v>0</v>
       </c>
       <c r="G15" s="18">
-        <f>RAWDATA!G13</f>
+        <f>RAWDATA!H13</f>
         <v>0</v>
       </c>
       <c r="H15" s="19" t="str">
-        <f>RAWDATA!H13</f>
+        <f>RAWDATA!I13</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I15" s="19">
-        <f>RAWDATA!I13</f>
+        <f>RAWDATA!J13</f>
         <v>0</v>
       </c>
       <c r="J15" s="17" t="str">
@@ -5332,19 +5434,19 @@
         <v>0</v>
       </c>
       <c r="F16" s="18">
-        <f>RAWDATA!F14</f>
+        <f>RAWDATA!G14</f>
         <v>0</v>
       </c>
       <c r="G16" s="18">
-        <f>RAWDATA!G14</f>
+        <f>RAWDATA!H14</f>
         <v>0</v>
       </c>
       <c r="H16" s="19" t="str">
-        <f>RAWDATA!H14</f>
+        <f>RAWDATA!I14</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I16" s="19">
-        <f>RAWDATA!I14</f>
+        <f>RAWDATA!J14</f>
         <v>0</v>
       </c>
       <c r="J16" s="17" t="str">
@@ -5389,19 +5491,19 @@
         <v>0</v>
       </c>
       <c r="F17" s="18">
-        <f>RAWDATA!F15</f>
+        <f>RAWDATA!G15</f>
         <v>0</v>
       </c>
       <c r="G17" s="18">
-        <f>RAWDATA!G15</f>
+        <f>RAWDATA!H15</f>
         <v>0</v>
       </c>
       <c r="H17" s="19" t="str">
-        <f>RAWDATA!H15</f>
+        <f>RAWDATA!I15</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I17" s="19">
-        <f>RAWDATA!I15</f>
+        <f>RAWDATA!J15</f>
         <v>0</v>
       </c>
       <c r="J17" s="17" t="str">
@@ -5446,19 +5548,19 @@
         <v>0</v>
       </c>
       <c r="F18" s="18">
-        <f>RAWDATA!F16</f>
+        <f>RAWDATA!G16</f>
         <v>0</v>
       </c>
       <c r="G18" s="18">
-        <f>RAWDATA!G16</f>
+        <f>RAWDATA!H16</f>
         <v>0</v>
       </c>
       <c r="H18" s="19" t="str">
-        <f>RAWDATA!H16</f>
+        <f>RAWDATA!I16</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I18" s="19">
-        <f>RAWDATA!I16</f>
+        <f>RAWDATA!J16</f>
         <v>0</v>
       </c>
       <c r="J18" s="17" t="str">
@@ -5503,19 +5605,19 @@
         <v>0</v>
       </c>
       <c r="F19" s="18">
-        <f>RAWDATA!F17</f>
+        <f>RAWDATA!G17</f>
         <v>0</v>
       </c>
       <c r="G19" s="18">
-        <f>RAWDATA!G17</f>
+        <f>RAWDATA!H17</f>
         <v>0</v>
       </c>
       <c r="H19" s="19" t="str">
-        <f>RAWDATA!H17</f>
+        <f>RAWDATA!I17</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I19" s="19">
-        <f>RAWDATA!I17</f>
+        <f>RAWDATA!J17</f>
         <v>0</v>
       </c>
       <c r="J19" s="17" t="str">
@@ -5560,19 +5662,19 @@
         <v>0</v>
       </c>
       <c r="F20" s="18">
-        <f>RAWDATA!F18</f>
+        <f>RAWDATA!G18</f>
         <v>0</v>
       </c>
       <c r="G20" s="18">
-        <f>RAWDATA!G18</f>
+        <f>RAWDATA!H18</f>
         <v>0</v>
       </c>
       <c r="H20" s="19" t="str">
-        <f>RAWDATA!H18</f>
+        <f>RAWDATA!I18</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I20" s="19">
-        <f>RAWDATA!I18</f>
+        <f>RAWDATA!J18</f>
         <v>0</v>
       </c>
       <c r="J20" s="17" t="str">
@@ -5617,19 +5719,19 @@
         <v>0</v>
       </c>
       <c r="F21" s="18">
-        <f>RAWDATA!F19</f>
+        <f>RAWDATA!G19</f>
         <v>0</v>
       </c>
       <c r="G21" s="18">
-        <f>RAWDATA!G19</f>
+        <f>RAWDATA!H19</f>
         <v>0</v>
       </c>
       <c r="H21" s="19" t="str">
-        <f>RAWDATA!H19</f>
+        <f>RAWDATA!I19</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I21" s="19">
-        <f>RAWDATA!I19</f>
+        <f>RAWDATA!J19</f>
         <v>0</v>
       </c>
       <c r="J21" s="17" t="str">
@@ -5674,19 +5776,19 @@
         <v>0</v>
       </c>
       <c r="F22" s="18">
-        <f>RAWDATA!F20</f>
+        <f>RAWDATA!G20</f>
         <v>0</v>
       </c>
       <c r="G22" s="18">
-        <f>RAWDATA!G20</f>
+        <f>RAWDATA!H20</f>
         <v>0</v>
       </c>
       <c r="H22" s="19" t="str">
-        <f>RAWDATA!H20</f>
+        <f>RAWDATA!I20</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I22" s="19">
-        <f>RAWDATA!I20</f>
+        <f>RAWDATA!J20</f>
         <v>0</v>
       </c>
       <c r="J22" s="17" t="str">
@@ -5731,19 +5833,19 @@
         <v>0</v>
       </c>
       <c r="F23" s="18">
-        <f>RAWDATA!F21</f>
+        <f>RAWDATA!G21</f>
         <v>0</v>
       </c>
       <c r="G23" s="18">
-        <f>RAWDATA!G21</f>
+        <f>RAWDATA!H21</f>
         <v>0</v>
       </c>
       <c r="H23" s="19" t="str">
-        <f>RAWDATA!H21</f>
+        <f>RAWDATA!I21</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I23" s="19">
-        <f>RAWDATA!I21</f>
+        <f>RAWDATA!J21</f>
         <v>0</v>
       </c>
       <c r="J23" s="17" t="str">
@@ -5788,19 +5890,19 @@
         <v>0</v>
       </c>
       <c r="F24" s="18">
-        <f>RAWDATA!F22</f>
+        <f>RAWDATA!G22</f>
         <v>0</v>
       </c>
       <c r="G24" s="18">
-        <f>RAWDATA!G22</f>
+        <f>RAWDATA!H22</f>
         <v>0</v>
       </c>
       <c r="H24" s="19" t="str">
-        <f>RAWDATA!H22</f>
+        <f>RAWDATA!I22</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I24" s="19">
-        <f>RAWDATA!I22</f>
+        <f>RAWDATA!J22</f>
         <v>0</v>
       </c>
       <c r="J24" s="17" t="str">
@@ -5845,19 +5947,19 @@
         <v>0</v>
       </c>
       <c r="F25" s="18">
-        <f>RAWDATA!F23</f>
+        <f>RAWDATA!G23</f>
         <v>0</v>
       </c>
       <c r="G25" s="18">
-        <f>RAWDATA!G23</f>
+        <f>RAWDATA!H23</f>
         <v>0</v>
       </c>
       <c r="H25" s="19" t="str">
-        <f>RAWDATA!H23</f>
+        <f>RAWDATA!I23</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I25" s="19">
-        <f>RAWDATA!I23</f>
+        <f>RAWDATA!J23</f>
         <v>0</v>
       </c>
       <c r="J25" s="17" t="str">
@@ -5902,19 +6004,19 @@
         <v>0</v>
       </c>
       <c r="F26" s="18">
-        <f>RAWDATA!F24</f>
+        <f>RAWDATA!G24</f>
         <v>0</v>
       </c>
       <c r="G26" s="18">
-        <f>RAWDATA!G24</f>
+        <f>RAWDATA!H24</f>
         <v>0</v>
       </c>
       <c r="H26" s="19" t="str">
-        <f>RAWDATA!H24</f>
+        <f>RAWDATA!I24</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I26" s="19">
-        <f>RAWDATA!I24</f>
+        <f>RAWDATA!J24</f>
         <v>0</v>
       </c>
       <c r="J26" s="17" t="str">
@@ -5959,19 +6061,19 @@
         <v>0</v>
       </c>
       <c r="F27" s="18">
-        <f>RAWDATA!F25</f>
+        <f>RAWDATA!G25</f>
         <v>0</v>
       </c>
       <c r="G27" s="18">
-        <f>RAWDATA!G25</f>
+        <f>RAWDATA!H25</f>
         <v>0</v>
       </c>
       <c r="H27" s="19">
-        <f>RAWDATA!H25</f>
+        <f>RAWDATA!I25</f>
         <v>0</v>
       </c>
       <c r="I27" s="19">
-        <f>RAWDATA!I25</f>
+        <f>RAWDATA!J25</f>
         <v>0</v>
       </c>
       <c r="J27" s="17" t="str">
@@ -6016,19 +6118,19 @@
         <v>0</v>
       </c>
       <c r="F28" s="18">
-        <f>RAWDATA!F26</f>
+        <f>RAWDATA!G26</f>
         <v>0</v>
       </c>
       <c r="G28" s="18">
-        <f>RAWDATA!G26</f>
+        <f>RAWDATA!H26</f>
         <v>0</v>
       </c>
       <c r="H28" s="19">
-        <f>RAWDATA!H26</f>
+        <f>RAWDATA!I26</f>
         <v>0</v>
       </c>
       <c r="I28" s="19">
-        <f>RAWDATA!I26</f>
+        <f>RAWDATA!J26</f>
         <v>0</v>
       </c>
       <c r="J28" s="17" t="str">
@@ -6073,19 +6175,19 @@
         <v>0</v>
       </c>
       <c r="F29" s="18">
-        <f>RAWDATA!F27</f>
+        <f>RAWDATA!G27</f>
         <v>0</v>
       </c>
       <c r="G29" s="18">
-        <f>RAWDATA!G27</f>
+        <f>RAWDATA!H27</f>
         <v>0</v>
       </c>
       <c r="H29" s="19">
-        <f>RAWDATA!H27</f>
+        <f>RAWDATA!I27</f>
         <v>0</v>
       </c>
       <c r="I29" s="19">
-        <f>RAWDATA!I27</f>
+        <f>RAWDATA!J27</f>
         <v>0</v>
       </c>
       <c r="J29" s="17" t="str">
@@ -6130,19 +6232,19 @@
         <v>0</v>
       </c>
       <c r="F30" s="18">
-        <f>RAWDATA!F28</f>
+        <f>RAWDATA!G28</f>
         <v>0</v>
       </c>
       <c r="G30" s="18">
-        <f>RAWDATA!G28</f>
+        <f>RAWDATA!H28</f>
         <v>0</v>
       </c>
       <c r="H30" s="19">
-        <f>RAWDATA!H28</f>
+        <f>RAWDATA!I28</f>
         <v>0</v>
       </c>
       <c r="I30" s="19">
-        <f>RAWDATA!I28</f>
+        <f>RAWDATA!J28</f>
         <v>0</v>
       </c>
       <c r="J30" s="17" t="str">
@@ -6187,19 +6289,19 @@
         <v>0</v>
       </c>
       <c r="F31" s="18">
-        <f>RAWDATA!F29</f>
+        <f>RAWDATA!G29</f>
         <v>0</v>
       </c>
       <c r="G31" s="18">
-        <f>RAWDATA!G29</f>
+        <f>RAWDATA!H29</f>
         <v>0</v>
       </c>
       <c r="H31" s="19">
-        <f>RAWDATA!H29</f>
+        <f>RAWDATA!I29</f>
         <v>0</v>
       </c>
       <c r="I31" s="19">
-        <f>RAWDATA!I29</f>
+        <f>RAWDATA!J29</f>
         <v>0</v>
       </c>
       <c r="J31" s="17" t="str">
@@ -6244,19 +6346,19 @@
         <v>0</v>
       </c>
       <c r="F32" s="18">
-        <f>RAWDATA!F30</f>
+        <f>RAWDATA!G30</f>
         <v>0</v>
       </c>
       <c r="G32" s="18">
-        <f>RAWDATA!G30</f>
+        <f>RAWDATA!H30</f>
         <v>0</v>
       </c>
       <c r="H32" s="19">
-        <f>RAWDATA!H30</f>
+        <f>RAWDATA!I30</f>
         <v>0</v>
       </c>
       <c r="I32" s="19">
-        <f>RAWDATA!I30</f>
+        <f>RAWDATA!J30</f>
         <v>0</v>
       </c>
       <c r="J32" s="17" t="str">
@@ -6301,19 +6403,19 @@
         <v>0</v>
       </c>
       <c r="F33" s="18">
-        <f>RAWDATA!F31</f>
+        <f>RAWDATA!G31</f>
         <v>0</v>
       </c>
       <c r="G33" s="18">
-        <f>RAWDATA!G31</f>
+        <f>RAWDATA!H31</f>
         <v>0</v>
       </c>
       <c r="H33" s="19">
-        <f>RAWDATA!H31</f>
+        <f>RAWDATA!I31</f>
         <v>0</v>
       </c>
       <c r="I33" s="19">
-        <f>RAWDATA!I31</f>
+        <f>RAWDATA!J31</f>
         <v>0</v>
       </c>
       <c r="J33" s="17" t="str">
@@ -6358,19 +6460,19 @@
         <v>0</v>
       </c>
       <c r="F34" s="18">
-        <f>RAWDATA!F32</f>
+        <f>RAWDATA!G32</f>
         <v>0</v>
       </c>
       <c r="G34" s="18">
-        <f>RAWDATA!G32</f>
+        <f>RAWDATA!H32</f>
         <v>0</v>
       </c>
       <c r="H34" s="19">
-        <f>RAWDATA!H32</f>
+        <f>RAWDATA!I32</f>
         <v>0</v>
       </c>
       <c r="I34" s="19">
-        <f>RAWDATA!I32</f>
+        <f>RAWDATA!J32</f>
         <v>0</v>
       </c>
       <c r="J34" s="17" t="str">
@@ -6415,19 +6517,19 @@
         <v>0</v>
       </c>
       <c r="F35" s="18">
-        <f>RAWDATA!F33</f>
+        <f>RAWDATA!G33</f>
         <v>0</v>
       </c>
       <c r="G35" s="18">
-        <f>RAWDATA!G33</f>
+        <f>RAWDATA!H33</f>
         <v>0</v>
       </c>
       <c r="H35" s="19">
-        <f>RAWDATA!H33</f>
+        <f>RAWDATA!I33</f>
         <v>0</v>
       </c>
       <c r="I35" s="19">
-        <f>RAWDATA!I33</f>
+        <f>RAWDATA!J33</f>
         <v>0</v>
       </c>
       <c r="J35" s="17" t="str">
@@ -6472,19 +6574,19 @@
         <v>0</v>
       </c>
       <c r="F36" s="18">
-        <f>RAWDATA!F34</f>
+        <f>RAWDATA!G34</f>
         <v>0</v>
       </c>
       <c r="G36" s="18">
-        <f>RAWDATA!G34</f>
+        <f>RAWDATA!H34</f>
         <v>0</v>
       </c>
       <c r="H36" s="19">
-        <f>RAWDATA!H34</f>
+        <f>RAWDATA!I34</f>
         <v>0</v>
       </c>
       <c r="I36" s="19">
-        <f>RAWDATA!I34</f>
+        <f>RAWDATA!J34</f>
         <v>0</v>
       </c>
       <c r="J36" s="17" t="str">
@@ -6529,19 +6631,19 @@
         <v>0</v>
       </c>
       <c r="F37" s="18">
-        <f>RAWDATA!F35</f>
+        <f>RAWDATA!G35</f>
         <v>0</v>
       </c>
       <c r="G37" s="18">
-        <f>RAWDATA!G35</f>
+        <f>RAWDATA!H35</f>
         <v>0</v>
       </c>
       <c r="H37" s="19">
-        <f>RAWDATA!H35</f>
+        <f>RAWDATA!I35</f>
         <v>0</v>
       </c>
       <c r="I37" s="19">
-        <f>RAWDATA!I35</f>
+        <f>RAWDATA!J35</f>
         <v>0</v>
       </c>
       <c r="J37" s="17" t="str">
@@ -6586,19 +6688,19 @@
         <v>0</v>
       </c>
       <c r="F38" s="18">
-        <f>RAWDATA!F36</f>
+        <f>RAWDATA!G36</f>
         <v>0</v>
       </c>
       <c r="G38" s="18">
-        <f>RAWDATA!G36</f>
+        <f>RAWDATA!H36</f>
         <v>0</v>
       </c>
       <c r="H38" s="19">
-        <f>RAWDATA!H36</f>
+        <f>RAWDATA!I36</f>
         <v>0</v>
       </c>
       <c r="I38" s="19">
-        <f>RAWDATA!I36</f>
+        <f>RAWDATA!J36</f>
         <v>0</v>
       </c>
       <c r="J38" s="17" t="str">
@@ -6756,7 +6858,7 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.6640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
@@ -6833,7 +6935,7 @@
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
-        <v>Dozent/in: Alaa Khalil</v>
+        <v xml:space="preserve">Dozent/in: </v>
       </c>
       <c r="B3" s="76"/>
       <c r="C3" s="76"/>
@@ -8389,7 +8491,7 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" style="61" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
@@ -8436,9 +8538,9 @@
         <f>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$43," ")</f>
         <v>course.ects_points</v>
       </c>
-      <c r="D2" s="65" t="str">
+      <c r="D2" s="65" t="e">
         <f>IF(Notenliste!F2="KP"," ",IF(Notenliste!F2="NB","nicht bestanden",Notenliste!F2))</f>
-        <v xml:space="preserve"> </v>
+        <v>#N/A</v>
       </c>
       <c r="E2" s="66" t="str">
         <f>IF(Notenliste!D2&lt;&gt;0,Notenliste!$B$48," ")</f>

</xml_diff>

<commit_message>
remove PS column, export TS requested/received status into excel grade lists
</commit_message>
<xml_diff>
--- a/src/spz/templates/export/courselist-enhanced.xlsx
+++ b/src/spz/templates/export/courselist-enhanced.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr updateLinks="never" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\04_Hiwi\Datenbank\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0563BC-4C68-41AE-A2DC-4E85508FE7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F83EEB9-3E77-4744-AE7C-2068325D6D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAWDATA" sheetId="11" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -312,6 +312,18 @@
   <si>
     <t>attendance.ects_points</t>
   </si>
+  <si>
+    <t>Teilnahmeschein</t>
+  </si>
+  <si>
+    <t>Schein erhalten</t>
+  </si>
+  <si>
+    <t>attendance.ts_requested_str</t>
+  </si>
+  <si>
+    <t>attendance.ts_received_str</t>
+  </si>
 </sst>
 </file>
 
@@ -320,7 +332,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +378,12 @@
       <color rgb="FFCCCC00"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -550,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -744,6 +762,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -800,7 +822,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
     <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
@@ -837,6 +859,12 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -1149,17 +1177,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DATA" displayName="DATA" ref="B1:I2" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="B1:I2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nachname" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Vorname" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hochschule" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Matrikelnummer" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{DF1C2C88-275C-4D8A-BD91-B3992E33C931}" name="Note" dataDxfId="14"/>
-    <tableColumn id="7" xr3:uid="{4C72B6BD-5346-447B-9F0F-4B0A565AEA16}" name="LP" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="E-Mail" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Telefon" dataDxfId="11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="DATA" displayName="DATA" ref="B1:K2" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
+  <autoFilter ref="B1:K2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Nachname" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Vorname" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Hochschule" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Matrikelnummer" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{DF1C2C88-275C-4D8A-BD91-B3992E33C931}" name="Note" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{4C72B6BD-5346-447B-9F0F-4B0A565AEA16}" name="LP" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="E-Mail" dataDxfId="14"/>
+    <tableColumn id="9" xr3:uid="{B3D6AD29-4B6D-497F-AE26-E1D310B5915C}" name="Telefon" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{C59980A3-2986-4FC5-B761-5AD4C725E3DF}" name="Teilnahmeschein" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Schein erhalten" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1477,10 +1507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" zeroHeight="1" x14ac:dyDescent="0.3"/>
@@ -1492,13 +1522,15 @@
     <col min="5" max="5" width="17.88671875" style="40" customWidth="1"/>
     <col min="6" max="7" width="9" style="40" customWidth="1"/>
     <col min="8" max="8" width="31.88671875" style="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" style="39" customWidth="1"/>
-    <col min="10" max="10" width="45.109375" style="39" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="9.44140625" style="39" hidden="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.44140625" hidden="1"/>
+    <col min="9" max="9" width="31.88671875" style="39" customWidth="1"/>
+    <col min="10" max="10" width="21.33203125" style="39" customWidth="1"/>
+    <col min="11" max="11" width="22.44140625" style="39" customWidth="1"/>
+    <col min="12" max="12" width="45.109375" style="39" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" style="39" hidden="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.44140625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>26</v>
       </c>
@@ -1527,13 +1559,19 @@
         <v>21</v>
       </c>
       <c r="J1" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="M1" s="37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1562,287 +1600,293 @@
         <v>58</v>
       </c>
       <c r="J2" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="L2" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="E3" s="39"/>
       <c r="F3" s="39"/>
       <c r="G3" s="39"/>
-      <c r="J3" s="39" t="s">
+      <c r="L3" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
-      <c r="J4" s="39" t="s">
+      <c r="L4" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
-      <c r="J5" s="39" t="s">
+      <c r="L5" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
-      <c r="J6" s="39" t="s">
+      <c r="L6" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
-      <c r="J7" s="39" t="s">
+      <c r="L7" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="E8" s="39"/>
       <c r="F8" s="39"/>
       <c r="G8" s="39"/>
-      <c r="J8" s="39" t="s">
+      <c r="L8" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="E9" s="39"/>
       <c r="F9" s="39"/>
       <c r="G9" s="39"/>
-      <c r="J9" s="39" t="s">
+      <c r="L9" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="E10" s="39"/>
       <c r="F10" s="39"/>
       <c r="G10" s="39"/>
-      <c r="J10" s="39" t="s">
+      <c r="L10" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="E11" s="39"/>
       <c r="F11" s="39"/>
       <c r="G11" s="39"/>
-      <c r="J11" s="39" t="s">
+      <c r="L11" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="E12" s="39"/>
       <c r="F12" s="39"/>
       <c r="G12" s="39"/>
-      <c r="J12" s="39" t="s">
+      <c r="L12" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="39"/>
       <c r="G13" s="39"/>
-      <c r="J13" s="39" t="s">
+      <c r="L13" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="E14" s="39"/>
       <c r="F14" s="39"/>
       <c r="G14" s="39"/>
-      <c r="J14" s="39" t="s">
+      <c r="L14" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="E15" s="39"/>
       <c r="F15" s="39"/>
       <c r="G15" s="39"/>
-      <c r="J15" s="39" t="s">
+      <c r="L15" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="E16" s="39"/>
       <c r="F16" s="39"/>
       <c r="G16" s="39"/>
-      <c r="J16" s="39" t="s">
+      <c r="L16" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="E17" s="39"/>
       <c r="F17" s="39"/>
       <c r="G17" s="39"/>
-      <c r="J17" s="39" t="s">
+      <c r="L17" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="E18" s="39"/>
       <c r="F18" s="39"/>
       <c r="G18" s="39"/>
-      <c r="J18" s="39" t="s">
+      <c r="L18" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="E19" s="39"/>
       <c r="F19" s="39"/>
       <c r="G19" s="39"/>
-      <c r="J19" s="39" t="s">
+      <c r="L19" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="E20" s="39"/>
       <c r="F20" s="39"/>
       <c r="G20" s="39"/>
-      <c r="J20" s="39" t="s">
+      <c r="L20" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="E21" s="39"/>
       <c r="F21" s="39"/>
       <c r="G21" s="39"/>
-      <c r="J21" s="39" t="s">
+      <c r="L21" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="E22" s="39"/>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
-      <c r="J22" s="39" t="s">
+      <c r="L22" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="E23" s="39"/>
       <c r="F23" s="39"/>
       <c r="G23" s="39"/>
-      <c r="J23" s="39" t="s">
+      <c r="L23" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="E24" s="39"/>
       <c r="F24" s="39"/>
       <c r="G24" s="39"/>
-      <c r="J24" s="39" t="s">
+      <c r="L24" s="39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1869,6 +1913,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1" formatColumns="0" selectLockedCells="1"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1883,8 +1928,8 @@
   </sheetPr>
   <dimension ref="A1:WVX71"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="13.2" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -2476,7 +2521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" s="29" t="str">
         <f>RAWDATA!B2</f>
         <v>applicant.last_name</v>
@@ -2506,12 +2551,18 @@
         <f>RAWDATA!G2</f>
         <v>attendance.ects_points</v>
       </c>
-      <c r="I2" s="35"/>
+      <c r="I2" s="35" t="str">
+        <f>RAWDATA!J2</f>
+        <v>attendance.ts_requested_str</v>
+      </c>
       <c r="J2" s="33" t="str">
         <f t="shared" ref="J2" si="0">IF(E2&gt;0,"X","")</f>
         <v>X</v>
       </c>
-      <c r="K2" s="35"/>
+      <c r="K2" s="35" t="str">
+        <f>RAWDATA!K2</f>
+        <v>attendance.ts_received_str</v>
+      </c>
       <c r="L2" s="4"/>
       <c r="M2" s="22"/>
       <c r="N2" s="2" t="str">
@@ -2565,12 +2616,18 @@
         <f>RAWDATA!G3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="35"/>
+      <c r="I3" s="35">
+        <f>RAWDATA!J3</f>
+        <v>0</v>
+      </c>
       <c r="J3" s="33" t="str">
         <f t="shared" ref="J3:J36" si="1">IF(E3&gt;0,"X","")</f>
         <v/>
       </c>
-      <c r="K3" s="35"/>
+      <c r="K3" s="35">
+        <f>RAWDATA!K3</f>
+        <v>0</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="22"/>
       <c r="N3" s="2">
@@ -2624,12 +2681,18 @@
         <f>RAWDATA!G4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="35"/>
+      <c r="I4" s="35">
+        <f>RAWDATA!J4</f>
+        <v>0</v>
+      </c>
       <c r="J4" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K4" s="35"/>
+      <c r="K4" s="35">
+        <f>RAWDATA!K4</f>
+        <v>0</v>
+      </c>
       <c r="L4" s="4"/>
       <c r="M4" s="22"/>
       <c r="N4" s="2">
@@ -2683,12 +2746,18 @@
         <f>RAWDATA!G5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="35"/>
+      <c r="I5" s="35">
+        <f>RAWDATA!J5</f>
+        <v>0</v>
+      </c>
       <c r="J5" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K5" s="35"/>
+      <c r="K5" s="35">
+        <f>RAWDATA!K5</f>
+        <v>0</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="22"/>
       <c r="N5" s="2">
@@ -2742,12 +2811,18 @@
         <f>RAWDATA!G6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="35"/>
+      <c r="I6" s="35">
+        <f>RAWDATA!J6</f>
+        <v>0</v>
+      </c>
       <c r="J6" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K6" s="35"/>
+      <c r="K6" s="35">
+        <f>RAWDATA!K6</f>
+        <v>0</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="22"/>
       <c r="N6" s="2">
@@ -2801,12 +2876,18 @@
         <f>RAWDATA!G7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="35"/>
+      <c r="I7" s="35">
+        <f>RAWDATA!J7</f>
+        <v>0</v>
+      </c>
       <c r="J7" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K7" s="35"/>
+      <c r="K7" s="35">
+        <f>RAWDATA!K7</f>
+        <v>0</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="22"/>
       <c r="N7" s="2">
@@ -2860,12 +2941,18 @@
         <f>RAWDATA!G8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="35"/>
+      <c r="I8" s="35">
+        <f>RAWDATA!J8</f>
+        <v>0</v>
+      </c>
       <c r="J8" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K8" s="35"/>
+      <c r="K8" s="35">
+        <f>RAWDATA!K8</f>
+        <v>0</v>
+      </c>
       <c r="L8" s="4"/>
       <c r="M8" s="22"/>
       <c r="N8" s="2">
@@ -2919,12 +3006,18 @@
         <f>RAWDATA!G9</f>
         <v>0</v>
       </c>
-      <c r="I9" s="35"/>
+      <c r="I9" s="35">
+        <f>RAWDATA!J9</f>
+        <v>0</v>
+      </c>
       <c r="J9" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K9" s="35"/>
+      <c r="K9" s="35">
+        <f>RAWDATA!K9</f>
+        <v>0</v>
+      </c>
       <c r="L9" s="4"/>
       <c r="M9" s="22"/>
       <c r="N9" s="2">
@@ -2978,12 +3071,18 @@
         <f>RAWDATA!G10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="35"/>
+      <c r="I10" s="35">
+        <f>RAWDATA!J10</f>
+        <v>0</v>
+      </c>
       <c r="J10" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K10" s="35"/>
+      <c r="K10" s="35">
+        <f>RAWDATA!K10</f>
+        <v>0</v>
+      </c>
       <c r="L10" s="4"/>
       <c r="M10" s="22"/>
       <c r="N10" s="2">
@@ -3037,12 +3136,18 @@
         <f>RAWDATA!G11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="35"/>
+      <c r="I11" s="35">
+        <f>RAWDATA!J11</f>
+        <v>0</v>
+      </c>
       <c r="J11" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K11" s="35"/>
+      <c r="K11" s="35">
+        <f>RAWDATA!K11</f>
+        <v>0</v>
+      </c>
       <c r="L11" s="4"/>
       <c r="M11" s="22"/>
       <c r="N11" s="2">
@@ -3096,12 +3201,18 @@
         <f>RAWDATA!G12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="35"/>
+      <c r="I12" s="35">
+        <f>RAWDATA!J12</f>
+        <v>0</v>
+      </c>
       <c r="J12" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K12" s="35"/>
+      <c r="K12" s="35">
+        <f>RAWDATA!K12</f>
+        <v>0</v>
+      </c>
       <c r="L12" s="4"/>
       <c r="M12" s="22"/>
       <c r="N12" s="2">
@@ -3155,12 +3266,18 @@
         <f>RAWDATA!G13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="35"/>
+      <c r="I13" s="35">
+        <f>RAWDATA!J13</f>
+        <v>0</v>
+      </c>
       <c r="J13" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K13" s="35"/>
+      <c r="K13" s="35">
+        <f>RAWDATA!K13</f>
+        <v>0</v>
+      </c>
       <c r="L13" s="4"/>
       <c r="M13" s="22"/>
       <c r="N13" s="2">
@@ -3214,12 +3331,18 @@
         <f>RAWDATA!G14</f>
         <v>0</v>
       </c>
-      <c r="I14" s="35"/>
+      <c r="I14" s="35">
+        <f>RAWDATA!J14</f>
+        <v>0</v>
+      </c>
       <c r="J14" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K14" s="35"/>
+      <c r="K14" s="35">
+        <f>RAWDATA!K14</f>
+        <v>0</v>
+      </c>
       <c r="L14" s="4"/>
       <c r="M14" s="22"/>
       <c r="N14" s="2">
@@ -3273,12 +3396,18 @@
         <f>RAWDATA!G15</f>
         <v>0</v>
       </c>
-      <c r="I15" s="35"/>
+      <c r="I15" s="35">
+        <f>RAWDATA!J15</f>
+        <v>0</v>
+      </c>
       <c r="J15" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K15" s="35"/>
+      <c r="K15" s="35">
+        <f>RAWDATA!K15</f>
+        <v>0</v>
+      </c>
       <c r="L15" s="4"/>
       <c r="M15" s="22"/>
       <c r="N15" s="2">
@@ -3332,12 +3461,18 @@
         <f>RAWDATA!G16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="35"/>
+      <c r="I16" s="35">
+        <f>RAWDATA!J16</f>
+        <v>0</v>
+      </c>
       <c r="J16" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K16" s="35"/>
+      <c r="K16" s="35">
+        <f>RAWDATA!K16</f>
+        <v>0</v>
+      </c>
       <c r="L16" s="4"/>
       <c r="M16" s="22"/>
       <c r="N16" s="2">
@@ -3391,12 +3526,18 @@
         <f>RAWDATA!G17</f>
         <v>0</v>
       </c>
-      <c r="I17" s="35"/>
+      <c r="I17" s="35">
+        <f>RAWDATA!J17</f>
+        <v>0</v>
+      </c>
       <c r="J17" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K17" s="35"/>
+      <c r="K17" s="35">
+        <f>RAWDATA!K17</f>
+        <v>0</v>
+      </c>
       <c r="L17" s="4"/>
       <c r="M17" s="22"/>
       <c r="N17" s="2">
@@ -3450,12 +3591,18 @@
         <f>RAWDATA!G18</f>
         <v>0</v>
       </c>
-      <c r="I18" s="35"/>
+      <c r="I18" s="35">
+        <f>RAWDATA!J18</f>
+        <v>0</v>
+      </c>
       <c r="J18" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K18" s="35"/>
+      <c r="K18" s="35">
+        <f>RAWDATA!K18</f>
+        <v>0</v>
+      </c>
       <c r="L18" s="4"/>
       <c r="M18" s="22"/>
       <c r="N18" s="2">
@@ -3509,12 +3656,18 @@
         <f>RAWDATA!G19</f>
         <v>0</v>
       </c>
-      <c r="I19" s="35"/>
+      <c r="I19" s="35">
+        <f>RAWDATA!J19</f>
+        <v>0</v>
+      </c>
       <c r="J19" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K19" s="35"/>
+      <c r="K19" s="35">
+        <f>RAWDATA!K19</f>
+        <v>0</v>
+      </c>
       <c r="L19" s="4"/>
       <c r="M19" s="22"/>
       <c r="N19" s="2">
@@ -3568,12 +3721,18 @@
         <f>RAWDATA!G20</f>
         <v>0</v>
       </c>
-      <c r="I20" s="35"/>
+      <c r="I20" s="35">
+        <f>RAWDATA!J20</f>
+        <v>0</v>
+      </c>
       <c r="J20" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K20" s="35"/>
+      <c r="K20" s="35">
+        <f>RAWDATA!K20</f>
+        <v>0</v>
+      </c>
       <c r="L20" s="4"/>
       <c r="M20" s="22"/>
       <c r="N20" s="2">
@@ -3627,12 +3786,18 @@
         <f>RAWDATA!G21</f>
         <v>0</v>
       </c>
-      <c r="I21" s="35"/>
+      <c r="I21" s="35">
+        <f>RAWDATA!J21</f>
+        <v>0</v>
+      </c>
       <c r="J21" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K21" s="35"/>
+      <c r="K21" s="35">
+        <f>RAWDATA!K21</f>
+        <v>0</v>
+      </c>
       <c r="L21" s="4"/>
       <c r="M21" s="22"/>
       <c r="N21" s="2">
@@ -3686,12 +3851,18 @@
         <f>RAWDATA!G22</f>
         <v>0</v>
       </c>
-      <c r="I22" s="35"/>
+      <c r="I22" s="35">
+        <f>RAWDATA!J22</f>
+        <v>0</v>
+      </c>
       <c r="J22" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K22" s="35"/>
+      <c r="K22" s="35">
+        <f>RAWDATA!K22</f>
+        <v>0</v>
+      </c>
       <c r="L22" s="4"/>
       <c r="M22" s="22"/>
       <c r="N22" s="2">
@@ -3745,12 +3916,18 @@
         <f>RAWDATA!G23</f>
         <v>0</v>
       </c>
-      <c r="I23" s="35"/>
+      <c r="I23" s="35">
+        <f>RAWDATA!J23</f>
+        <v>0</v>
+      </c>
       <c r="J23" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K23" s="35"/>
+      <c r="K23" s="35">
+        <f>RAWDATA!K23</f>
+        <v>0</v>
+      </c>
       <c r="L23" s="4"/>
       <c r="M23" s="22"/>
       <c r="N23" s="2">
@@ -3804,12 +3981,18 @@
         <f>RAWDATA!G24</f>
         <v>0</v>
       </c>
-      <c r="I24" s="35"/>
+      <c r="I24" s="35">
+        <f>RAWDATA!J24</f>
+        <v>0</v>
+      </c>
       <c r="J24" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K24" s="35"/>
+      <c r="K24" s="35">
+        <f>RAWDATA!K24</f>
+        <v>0</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="22"/>
       <c r="N24" s="2">
@@ -3863,12 +4046,18 @@
         <f>RAWDATA!G25</f>
         <v>0</v>
       </c>
-      <c r="I25" s="35"/>
+      <c r="I25" s="35">
+        <f>RAWDATA!J25</f>
+        <v>0</v>
+      </c>
       <c r="J25" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K25" s="35"/>
+      <c r="K25" s="35">
+        <f>RAWDATA!K25</f>
+        <v>0</v>
+      </c>
       <c r="L25" s="4"/>
       <c r="M25" s="22"/>
       <c r="N25" s="2"/>
@@ -3905,12 +4094,18 @@
         <f>RAWDATA!G26</f>
         <v>0</v>
       </c>
-      <c r="I26" s="35"/>
+      <c r="I26" s="35">
+        <f>RAWDATA!J26</f>
+        <v>0</v>
+      </c>
       <c r="J26" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K26" s="35"/>
+      <c r="K26" s="35">
+        <f>RAWDATA!K26</f>
+        <v>0</v>
+      </c>
       <c r="L26" s="4"/>
       <c r="M26" s="22"/>
       <c r="N26" s="2"/>
@@ -3947,12 +4142,18 @@
         <f>RAWDATA!G27</f>
         <v>0</v>
       </c>
-      <c r="I27" s="35"/>
+      <c r="I27" s="35">
+        <f>RAWDATA!J27</f>
+        <v>0</v>
+      </c>
       <c r="J27" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K27" s="35"/>
+      <c r="K27" s="35">
+        <f>RAWDATA!K27</f>
+        <v>0</v>
+      </c>
       <c r="L27" s="4"/>
       <c r="M27" s="22"/>
       <c r="N27" s="2"/>
@@ -3989,12 +4190,18 @@
         <f>RAWDATA!G28</f>
         <v>0</v>
       </c>
-      <c r="I28" s="35"/>
+      <c r="I28" s="35">
+        <f>RAWDATA!J28</f>
+        <v>0</v>
+      </c>
       <c r="J28" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K28" s="35"/>
+      <c r="K28" s="35">
+        <f>RAWDATA!K28</f>
+        <v>0</v>
+      </c>
       <c r="L28" s="4"/>
       <c r="M28" s="22"/>
       <c r="N28" s="2"/>
@@ -4031,12 +4238,18 @@
         <f>RAWDATA!G29</f>
         <v>0</v>
       </c>
-      <c r="I29" s="35"/>
+      <c r="I29" s="35">
+        <f>RAWDATA!J29</f>
+        <v>0</v>
+      </c>
       <c r="J29" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K29" s="35"/>
+      <c r="K29" s="35">
+        <f>RAWDATA!K29</f>
+        <v>0</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" s="22"/>
       <c r="N29" s="2"/>
@@ -4073,12 +4286,18 @@
         <f>RAWDATA!G30</f>
         <v>0</v>
       </c>
-      <c r="I30" s="35"/>
+      <c r="I30" s="35">
+        <f>RAWDATA!J30</f>
+        <v>0</v>
+      </c>
       <c r="J30" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K30" s="35"/>
+      <c r="K30" s="35">
+        <f>RAWDATA!K30</f>
+        <v>0</v>
+      </c>
       <c r="L30" s="4"/>
       <c r="M30" s="22"/>
       <c r="N30" s="2"/>
@@ -4115,12 +4334,18 @@
         <f>RAWDATA!G31</f>
         <v>0</v>
       </c>
-      <c r="I31" s="35"/>
+      <c r="I31" s="35">
+        <f>RAWDATA!J31</f>
+        <v>0</v>
+      </c>
       <c r="J31" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K31" s="35"/>
+      <c r="K31" s="35">
+        <f>RAWDATA!K31</f>
+        <v>0</v>
+      </c>
       <c r="L31" s="4"/>
       <c r="M31" s="22"/>
       <c r="N31" s="2"/>
@@ -4157,12 +4382,18 @@
         <f>RAWDATA!G32</f>
         <v>0</v>
       </c>
-      <c r="I32" s="35"/>
+      <c r="I32" s="35">
+        <f>RAWDATA!J32</f>
+        <v>0</v>
+      </c>
       <c r="J32" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K32" s="35"/>
+      <c r="K32" s="35">
+        <f>RAWDATA!K32</f>
+        <v>0</v>
+      </c>
       <c r="L32" s="4"/>
       <c r="M32" s="22"/>
       <c r="N32" s="2"/>
@@ -4199,12 +4430,18 @@
         <f>RAWDATA!G33</f>
         <v>0</v>
       </c>
-      <c r="I33" s="35"/>
+      <c r="I33" s="35">
+        <f>RAWDATA!J33</f>
+        <v>0</v>
+      </c>
       <c r="J33" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K33" s="35"/>
+      <c r="K33" s="35">
+        <f>RAWDATA!K33</f>
+        <v>0</v>
+      </c>
       <c r="L33" s="4"/>
       <c r="M33" s="22"/>
       <c r="N33" s="2"/>
@@ -4241,12 +4478,18 @@
         <f>RAWDATA!G34</f>
         <v>0</v>
       </c>
-      <c r="I34" s="35"/>
+      <c r="I34" s="35">
+        <f>RAWDATA!J34</f>
+        <v>0</v>
+      </c>
       <c r="J34" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K34" s="35"/>
+      <c r="K34" s="35">
+        <f>RAWDATA!K34</f>
+        <v>0</v>
+      </c>
       <c r="L34" s="4"/>
       <c r="M34" s="22"/>
       <c r="N34" s="2"/>
@@ -4283,12 +4526,18 @@
         <f>RAWDATA!G35</f>
         <v>0</v>
       </c>
-      <c r="I35" s="35"/>
+      <c r="I35" s="35">
+        <f>RAWDATA!J35</f>
+        <v>0</v>
+      </c>
       <c r="J35" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K35" s="35"/>
+      <c r="K35" s="35">
+        <f>RAWDATA!K35</f>
+        <v>0</v>
+      </c>
       <c r="L35" s="4"/>
       <c r="M35" s="22"/>
       <c r="N35" s="2">
@@ -4342,12 +4591,18 @@
         <f>RAWDATA!G36</f>
         <v>0</v>
       </c>
-      <c r="I36" s="35"/>
+      <c r="I36" s="35">
+        <f>RAWDATA!J36</f>
+        <v>0</v>
+      </c>
       <c r="J36" s="33" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="K36" s="35"/>
+      <c r="K36" s="35">
+        <f>RAWDATA!K36</f>
+        <v>0</v>
+      </c>
       <c r="L36" s="4"/>
       <c r="M36" s="22"/>
       <c r="N36" s="2">
@@ -4449,12 +4704,12 @@
         <v>66</v>
       </c>
       <c r="C41" s="23"/>
-      <c r="D41" s="67" t="s">
+      <c r="D41" s="68" t="s">
         <v>34</v>
       </c>
-      <c r="E41" s="67"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="68"/>
+      <c r="G41" s="68"/>
       <c r="H41" s="25"/>
       <c r="I41" s="31"/>
       <c r="J41" s="25"/>
@@ -4470,10 +4725,10 @@
         <v>59</v>
       </c>
       <c r="C42" s="23"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="67"/>
-      <c r="F42" s="67"/>
-      <c r="G42" s="67"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="68"/>
+      <c r="G42" s="68"/>
       <c r="H42" s="25"/>
       <c r="I42" s="31"/>
       <c r="J42" s="25"/>
@@ -4489,10 +4744,10 @@
         <v>61</v>
       </c>
       <c r="C43" s="23"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="67"/>
-      <c r="G43" s="67"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="68"/>
+      <c r="F43" s="68"/>
+      <c r="G43" s="68"/>
       <c r="H43" s="25"/>
       <c r="I43" s="31"/>
       <c r="J43" s="25"/>
@@ -4508,10 +4763,10 @@
         <v>63</v>
       </c>
       <c r="C44" s="23"/>
-      <c r="D44" s="67"/>
-      <c r="E44" s="67"/>
-      <c r="F44" s="67"/>
-      <c r="G44" s="67"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="68"/>
+      <c r="G44" s="68"/>
       <c r="H44" s="25"/>
       <c r="I44" s="31"/>
       <c r="J44" s="25"/>
@@ -4527,10 +4782,10 @@
         <v>65</v>
       </c>
       <c r="C45" s="23"/>
-      <c r="D45" s="67"/>
-      <c r="E45" s="67"/>
-      <c r="F45" s="67"/>
-      <c r="G45" s="67"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
       <c r="H45" s="25"/>
       <c r="I45" s="31"/>
       <c r="J45" s="25"/>
@@ -4546,10 +4801,10 @@
         <v>64</v>
       </c>
       <c r="C46" s="23"/>
-      <c r="D46" s="67"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="67"/>
-      <c r="G46" s="67"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="68"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="68"/>
       <c r="H46" s="25"/>
       <c r="I46" s="31"/>
       <c r="J46" s="25"/>
@@ -4565,10 +4820,10 @@
         <v>60</v>
       </c>
       <c r="C47" s="23"/>
-      <c r="D47" s="67"/>
-      <c r="E47" s="67"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="68"/>
+      <c r="F47" s="68"/>
+      <c r="G47" s="68"/>
       <c r="H47" s="25"/>
       <c r="I47" s="31"/>
       <c r="J47" s="25"/>
@@ -4584,10 +4839,10 @@
         <v>62</v>
       </c>
       <c r="C48" s="23"/>
-      <c r="D48" s="67"/>
-      <c r="E48" s="67"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="68"/>
+      <c r="F48" s="68"/>
+      <c r="G48" s="68"/>
       <c r="H48" s="25"/>
       <c r="I48" s="22"/>
       <c r="J48" s="25"/>
@@ -4683,11 +4938,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="68" t="str">
+      <c r="A1" s="69" t="str">
         <f>Notenliste!B44</f>
         <v>course.name</v>
       </c>
-      <c r="B1" s="68"/>
+      <c r="B1" s="69"/>
       <c r="C1" s="8" t="s">
         <v>13</v>
       </c>
@@ -4841,45 +5096,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="58" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="str">
+      <c r="A1" s="70" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
         <v>course.namecourse.alternative</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
     </row>
     <row r="2" spans="1:14" s="58" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="70" t="str">
+      <c r="A2" s="71" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
         <v>Dozent/in: course.teacher_name</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="71" t="str">
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="72" t="str">
         <f>"Semster: "&amp;Notenliste!B47</f>
         <v>Semster: semester</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
     </row>
     <row r="3" spans="1:14" s="59" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -4954,16 +5209,16 @@
         <v>applicant.phone</v>
       </c>
       <c r="H4" s="19" t="str">
-        <f>RAWDATA!J2</f>
+        <f>RAWDATA!L2</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I4" s="19">
-        <f>RAWDATA!K2</f>
+        <f>RAWDATA!M2</f>
         <v>0</v>
       </c>
       <c r="J4" s="17" t="str">
         <f>UPPER(Notenliste!I2)</f>
-        <v/>
+        <v>ATTENDANCE.TS_REQUESTED_STR</v>
       </c>
       <c r="K4" s="17" t="e">
         <f>IF(L4&lt;=4,"X","")</f>
@@ -4979,7 +5234,7 @@
       </c>
       <c r="N4" s="19" t="str">
         <f>UPPER(Notenliste!K2)</f>
-        <v/>
+        <v>ATTENDANCE.TS_RECEIVED_STR</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5007,20 +5262,20 @@
         <v>0</v>
       </c>
       <c r="G5" s="18">
-        <f>RAWDATA!I3</f>
+        <f>RAWDATA!K3</f>
         <v>0</v>
       </c>
       <c r="H5" s="19" t="str">
-        <f>RAWDATA!J3</f>
+        <f>RAWDATA!L3</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I5" s="19">
-        <f>RAWDATA!K3</f>
+        <f>RAWDATA!M3</f>
         <v>0</v>
       </c>
       <c r="J5" s="17" t="str">
         <f>UPPER(Notenliste!I3)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K5" s="17" t="str">
         <f t="shared" ref="K5:K38" si="0">IF(L5&lt;=4,"X","")</f>
@@ -5036,7 +5291,7 @@
       </c>
       <c r="N5" s="19" t="str">
         <f>UPPER(Notenliste!K3)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5064,20 +5319,20 @@
         <v>0</v>
       </c>
       <c r="G6" s="18">
-        <f>RAWDATA!I4</f>
+        <f>RAWDATA!K4</f>
         <v>0</v>
       </c>
       <c r="H6" s="19" t="str">
-        <f>RAWDATA!J4</f>
+        <f>RAWDATA!L4</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I6" s="19">
-        <f>RAWDATA!K4</f>
+        <f>RAWDATA!M4</f>
         <v>0</v>
       </c>
       <c r="J6" s="17" t="str">
         <f>UPPER(Notenliste!I4)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K6" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5093,7 +5348,7 @@
       </c>
       <c r="N6" s="19" t="str">
         <f>UPPER(Notenliste!K4)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5121,20 +5376,20 @@
         <v>0</v>
       </c>
       <c r="G7" s="18">
-        <f>RAWDATA!I5</f>
+        <f>RAWDATA!K5</f>
         <v>0</v>
       </c>
       <c r="H7" s="19" t="str">
-        <f>RAWDATA!J5</f>
+        <f>RAWDATA!L5</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I7" s="19">
-        <f>RAWDATA!K5</f>
+        <f>RAWDATA!M5</f>
         <v>0</v>
       </c>
       <c r="J7" s="17" t="str">
         <f>UPPER(Notenliste!I5)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K7" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5150,7 +5405,7 @@
       </c>
       <c r="N7" s="19" t="str">
         <f>UPPER(Notenliste!K5)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5178,20 +5433,20 @@
         <v>0</v>
       </c>
       <c r="G8" s="18">
-        <f>RAWDATA!I6</f>
+        <f>RAWDATA!K6</f>
         <v>0</v>
       </c>
       <c r="H8" s="19" t="str">
-        <f>RAWDATA!J6</f>
+        <f>RAWDATA!L6</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I8" s="19">
-        <f>RAWDATA!K6</f>
+        <f>RAWDATA!M6</f>
         <v>0</v>
       </c>
       <c r="J8" s="17" t="str">
         <f>UPPER(Notenliste!I6)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K8" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5207,7 +5462,7 @@
       </c>
       <c r="N8" s="19" t="str">
         <f>UPPER(Notenliste!K6)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5235,20 +5490,20 @@
         <v>0</v>
       </c>
       <c r="G9" s="18">
-        <f>RAWDATA!I7</f>
+        <f>RAWDATA!K7</f>
         <v>0</v>
       </c>
       <c r="H9" s="19" t="str">
-        <f>RAWDATA!J7</f>
+        <f>RAWDATA!L7</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I9" s="19">
-        <f>RAWDATA!K7</f>
+        <f>RAWDATA!M7</f>
         <v>0</v>
       </c>
       <c r="J9" s="17" t="str">
         <f>UPPER(Notenliste!I7)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K9" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5264,7 +5519,7 @@
       </c>
       <c r="N9" s="19" t="str">
         <f>UPPER(Notenliste!K7)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5292,20 +5547,20 @@
         <v>0</v>
       </c>
       <c r="G10" s="18">
-        <f>RAWDATA!I8</f>
+        <f>RAWDATA!K8</f>
         <v>0</v>
       </c>
       <c r="H10" s="19" t="str">
-        <f>RAWDATA!J8</f>
+        <f>RAWDATA!L8</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I10" s="19">
-        <f>RAWDATA!K8</f>
+        <f>RAWDATA!M8</f>
         <v>0</v>
       </c>
       <c r="J10" s="17" t="str">
         <f>UPPER(Notenliste!I8)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K10" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5321,7 +5576,7 @@
       </c>
       <c r="N10" s="19" t="str">
         <f>UPPER(Notenliste!K8)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5349,20 +5604,20 @@
         <v>0</v>
       </c>
       <c r="G11" s="18">
-        <f>RAWDATA!I9</f>
+        <f>RAWDATA!K9</f>
         <v>0</v>
       </c>
       <c r="H11" s="19" t="str">
-        <f>RAWDATA!J9</f>
+        <f>RAWDATA!L9</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I11" s="19">
-        <f>RAWDATA!K9</f>
+        <f>RAWDATA!M9</f>
         <v>0</v>
       </c>
       <c r="J11" s="17" t="str">
         <f>UPPER(Notenliste!I9)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K11" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5378,7 +5633,7 @@
       </c>
       <c r="N11" s="19" t="str">
         <f>UPPER(Notenliste!K9)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5406,20 +5661,20 @@
         <v>0</v>
       </c>
       <c r="G12" s="18">
-        <f>RAWDATA!I10</f>
+        <f>RAWDATA!K10</f>
         <v>0</v>
       </c>
       <c r="H12" s="19" t="str">
-        <f>RAWDATA!J10</f>
+        <f>RAWDATA!L10</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I12" s="19">
-        <f>RAWDATA!K10</f>
+        <f>RAWDATA!M10</f>
         <v>0</v>
       </c>
       <c r="J12" s="17" t="str">
         <f>UPPER(Notenliste!I10)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K12" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5435,7 +5690,7 @@
       </c>
       <c r="N12" s="19" t="str">
         <f>UPPER(Notenliste!K10)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5463,20 +5718,20 @@
         <v>0</v>
       </c>
       <c r="G13" s="18">
-        <f>RAWDATA!I11</f>
+        <f>RAWDATA!K11</f>
         <v>0</v>
       </c>
       <c r="H13" s="19" t="str">
-        <f>RAWDATA!J11</f>
+        <f>RAWDATA!L11</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I13" s="19">
-        <f>RAWDATA!K11</f>
+        <f>RAWDATA!M11</f>
         <v>0</v>
       </c>
       <c r="J13" s="17" t="str">
         <f>UPPER(Notenliste!I11)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K13" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5492,7 +5747,7 @@
       </c>
       <c r="N13" s="19" t="str">
         <f>UPPER(Notenliste!K11)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5520,20 +5775,20 @@
         <v>0</v>
       </c>
       <c r="G14" s="18">
-        <f>RAWDATA!I12</f>
+        <f>RAWDATA!K12</f>
         <v>0</v>
       </c>
       <c r="H14" s="19" t="str">
-        <f>RAWDATA!J12</f>
+        <f>RAWDATA!L12</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I14" s="19">
-        <f>RAWDATA!K12</f>
+        <f>RAWDATA!M12</f>
         <v>0</v>
       </c>
       <c r="J14" s="17" t="str">
         <f>UPPER(Notenliste!I12)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K14" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5549,7 +5804,7 @@
       </c>
       <c r="N14" s="19" t="str">
         <f>UPPER(Notenliste!K12)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5577,20 +5832,20 @@
         <v>0</v>
       </c>
       <c r="G15" s="18">
-        <f>RAWDATA!I13</f>
+        <f>RAWDATA!K13</f>
         <v>0</v>
       </c>
       <c r="H15" s="19" t="str">
-        <f>RAWDATA!J13</f>
+        <f>RAWDATA!L13</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I15" s="19">
-        <f>RAWDATA!K13</f>
+        <f>RAWDATA!M13</f>
         <v>0</v>
       </c>
       <c r="J15" s="17" t="str">
         <f>UPPER(Notenliste!I13)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K15" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5606,7 +5861,7 @@
       </c>
       <c r="N15" s="19" t="str">
         <f>UPPER(Notenliste!K13)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5634,20 +5889,20 @@
         <v>0</v>
       </c>
       <c r="G16" s="18">
-        <f>RAWDATA!I14</f>
+        <f>RAWDATA!K14</f>
         <v>0</v>
       </c>
       <c r="H16" s="19" t="str">
-        <f>RAWDATA!J14</f>
+        <f>RAWDATA!L14</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I16" s="19">
-        <f>RAWDATA!K14</f>
+        <f>RAWDATA!M14</f>
         <v>0</v>
       </c>
       <c r="J16" s="17" t="str">
         <f>UPPER(Notenliste!I14)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K16" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5663,7 +5918,7 @@
       </c>
       <c r="N16" s="19" t="str">
         <f>UPPER(Notenliste!K14)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5691,20 +5946,20 @@
         <v>0</v>
       </c>
       <c r="G17" s="18">
-        <f>RAWDATA!I15</f>
+        <f>RAWDATA!K15</f>
         <v>0</v>
       </c>
       <c r="H17" s="19" t="str">
-        <f>RAWDATA!J15</f>
+        <f>RAWDATA!L15</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I17" s="19">
-        <f>RAWDATA!K15</f>
+        <f>RAWDATA!M15</f>
         <v>0</v>
       </c>
       <c r="J17" s="17" t="str">
         <f>UPPER(Notenliste!I15)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K17" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5720,7 +5975,7 @@
       </c>
       <c r="N17" s="19" t="str">
         <f>UPPER(Notenliste!K15)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5748,20 +6003,20 @@
         <v>0</v>
       </c>
       <c r="G18" s="18">
-        <f>RAWDATA!I16</f>
+        <f>RAWDATA!K16</f>
         <v>0</v>
       </c>
       <c r="H18" s="19" t="str">
-        <f>RAWDATA!J16</f>
+        <f>RAWDATA!L16</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I18" s="19">
-        <f>RAWDATA!K16</f>
+        <f>RAWDATA!M16</f>
         <v>0</v>
       </c>
       <c r="J18" s="17" t="str">
         <f>UPPER(Notenliste!I16)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K18" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5777,7 +6032,7 @@
       </c>
       <c r="N18" s="19" t="str">
         <f>UPPER(Notenliste!K16)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5805,20 +6060,20 @@
         <v>0</v>
       </c>
       <c r="G19" s="18">
-        <f>RAWDATA!I17</f>
+        <f>RAWDATA!K17</f>
         <v>0</v>
       </c>
       <c r="H19" s="19" t="str">
-        <f>RAWDATA!J17</f>
+        <f>RAWDATA!L17</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I19" s="19">
-        <f>RAWDATA!K17</f>
+        <f>RAWDATA!M17</f>
         <v>0</v>
       </c>
       <c r="J19" s="17" t="str">
         <f>UPPER(Notenliste!I17)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K19" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5834,7 +6089,7 @@
       </c>
       <c r="N19" s="19" t="str">
         <f>UPPER(Notenliste!K17)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5862,20 +6117,20 @@
         <v>0</v>
       </c>
       <c r="G20" s="18">
-        <f>RAWDATA!I18</f>
+        <f>RAWDATA!K18</f>
         <v>0</v>
       </c>
       <c r="H20" s="19" t="str">
-        <f>RAWDATA!J18</f>
+        <f>RAWDATA!L18</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I20" s="19">
-        <f>RAWDATA!K18</f>
+        <f>RAWDATA!M18</f>
         <v>0</v>
       </c>
       <c r="J20" s="17" t="str">
         <f>UPPER(Notenliste!I18)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K20" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5891,7 +6146,7 @@
       </c>
       <c r="N20" s="19" t="str">
         <f>UPPER(Notenliste!K18)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5919,20 +6174,20 @@
         <v>0</v>
       </c>
       <c r="G21" s="18">
-        <f>RAWDATA!I19</f>
+        <f>RAWDATA!K19</f>
         <v>0</v>
       </c>
       <c r="H21" s="19" t="str">
-        <f>RAWDATA!J19</f>
+        <f>RAWDATA!L19</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I21" s="19">
-        <f>RAWDATA!K19</f>
+        <f>RAWDATA!M19</f>
         <v>0</v>
       </c>
       <c r="J21" s="17" t="str">
         <f>UPPER(Notenliste!I19)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K21" s="17" t="str">
         <f t="shared" si="0"/>
@@ -5948,7 +6203,7 @@
       </c>
       <c r="N21" s="19" t="str">
         <f>UPPER(Notenliste!K19)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -5976,20 +6231,20 @@
         <v>0</v>
       </c>
       <c r="G22" s="18">
-        <f>RAWDATA!I20</f>
+        <f>RAWDATA!K20</f>
         <v>0</v>
       </c>
       <c r="H22" s="19" t="str">
-        <f>RAWDATA!J20</f>
+        <f>RAWDATA!L20</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I22" s="19">
-        <f>RAWDATA!K20</f>
+        <f>RAWDATA!M20</f>
         <v>0</v>
       </c>
       <c r="J22" s="17" t="str">
         <f>UPPER(Notenliste!I20)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K22" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6005,7 +6260,7 @@
       </c>
       <c r="N22" s="19" t="str">
         <f>UPPER(Notenliste!K20)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6033,20 +6288,20 @@
         <v>0</v>
       </c>
       <c r="G23" s="18">
-        <f>RAWDATA!I21</f>
+        <f>RAWDATA!K21</f>
         <v>0</v>
       </c>
       <c r="H23" s="19" t="str">
-        <f>RAWDATA!J21</f>
+        <f>RAWDATA!L21</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I23" s="19">
-        <f>RAWDATA!K21</f>
+        <f>RAWDATA!M21</f>
         <v>0</v>
       </c>
       <c r="J23" s="17" t="str">
         <f>UPPER(Notenliste!I21)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K23" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6062,7 +6317,7 @@
       </c>
       <c r="N23" s="19" t="str">
         <f>UPPER(Notenliste!K21)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6090,20 +6345,20 @@
         <v>0</v>
       </c>
       <c r="G24" s="18">
-        <f>RAWDATA!I22</f>
+        <f>RAWDATA!K22</f>
         <v>0</v>
       </c>
       <c r="H24" s="19" t="str">
-        <f>RAWDATA!J22</f>
+        <f>RAWDATA!L22</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I24" s="19">
-        <f>RAWDATA!K22</f>
+        <f>RAWDATA!M22</f>
         <v>0</v>
       </c>
       <c r="J24" s="17" t="str">
         <f>UPPER(Notenliste!I22)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K24" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6119,7 +6374,7 @@
       </c>
       <c r="N24" s="19" t="str">
         <f>UPPER(Notenliste!K22)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6147,20 +6402,20 @@
         <v>0</v>
       </c>
       <c r="G25" s="18">
-        <f>RAWDATA!I23</f>
+        <f>RAWDATA!K23</f>
         <v>0</v>
       </c>
       <c r="H25" s="19" t="str">
-        <f>RAWDATA!J23</f>
+        <f>RAWDATA!L23</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I25" s="19">
-        <f>RAWDATA!K23</f>
+        <f>RAWDATA!M23</f>
         <v>0</v>
       </c>
       <c r="J25" s="17" t="str">
         <f>UPPER(Notenliste!I23)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K25" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6176,7 +6431,7 @@
       </c>
       <c r="N25" s="19" t="str">
         <f>UPPER(Notenliste!K23)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6204,20 +6459,20 @@
         <v>0</v>
       </c>
       <c r="G26" s="18">
-        <f>RAWDATA!I24</f>
+        <f>RAWDATA!K24</f>
         <v>0</v>
       </c>
       <c r="H26" s="19" t="str">
-        <f>RAWDATA!J24</f>
+        <f>RAWDATA!L24</f>
         <v>Arabisch 1</v>
       </c>
       <c r="I26" s="19">
-        <f>RAWDATA!K24</f>
+        <f>RAWDATA!M24</f>
         <v>0</v>
       </c>
       <c r="J26" s="17" t="str">
         <f>UPPER(Notenliste!I24)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K26" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6233,7 +6488,7 @@
       </c>
       <c r="N26" s="19" t="str">
         <f>UPPER(Notenliste!K24)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6261,20 +6516,20 @@
         <v>0</v>
       </c>
       <c r="G27" s="18">
-        <f>RAWDATA!I25</f>
+        <f>RAWDATA!K25</f>
         <v>0</v>
       </c>
       <c r="H27" s="19">
-        <f>RAWDATA!J25</f>
+        <f>RAWDATA!L25</f>
         <v>0</v>
       </c>
       <c r="I27" s="19">
-        <f>RAWDATA!K25</f>
+        <f>RAWDATA!M25</f>
         <v>0</v>
       </c>
       <c r="J27" s="17" t="str">
         <f>UPPER(Notenliste!I25)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K27" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6290,7 +6545,7 @@
       </c>
       <c r="N27" s="19" t="str">
         <f>UPPER(Notenliste!K25)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6318,20 +6573,20 @@
         <v>0</v>
       </c>
       <c r="G28" s="18">
-        <f>RAWDATA!I26</f>
+        <f>RAWDATA!K26</f>
         <v>0</v>
       </c>
       <c r="H28" s="19">
-        <f>RAWDATA!J26</f>
+        <f>RAWDATA!L26</f>
         <v>0</v>
       </c>
       <c r="I28" s="19">
-        <f>RAWDATA!K26</f>
+        <f>RAWDATA!M26</f>
         <v>0</v>
       </c>
       <c r="J28" s="17" t="str">
         <f>UPPER(Notenliste!I26)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K28" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6347,7 +6602,7 @@
       </c>
       <c r="N28" s="19" t="str">
         <f>UPPER(Notenliste!K26)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6375,20 +6630,20 @@
         <v>0</v>
       </c>
       <c r="G29" s="18">
-        <f>RAWDATA!I27</f>
+        <f>RAWDATA!K27</f>
         <v>0</v>
       </c>
       <c r="H29" s="19">
-        <f>RAWDATA!J27</f>
+        <f>RAWDATA!L27</f>
         <v>0</v>
       </c>
       <c r="I29" s="19">
-        <f>RAWDATA!K27</f>
+        <f>RAWDATA!M27</f>
         <v>0</v>
       </c>
       <c r="J29" s="17" t="str">
         <f>UPPER(Notenliste!I27)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K29" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6404,7 +6659,7 @@
       </c>
       <c r="N29" s="19" t="str">
         <f>UPPER(Notenliste!K27)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6432,20 +6687,20 @@
         <v>0</v>
       </c>
       <c r="G30" s="18">
-        <f>RAWDATA!I28</f>
+        <f>RAWDATA!K28</f>
         <v>0</v>
       </c>
       <c r="H30" s="19">
-        <f>RAWDATA!J28</f>
+        <f>RAWDATA!L28</f>
         <v>0</v>
       </c>
       <c r="I30" s="19">
-        <f>RAWDATA!K28</f>
+        <f>RAWDATA!M28</f>
         <v>0</v>
       </c>
       <c r="J30" s="17" t="str">
         <f>UPPER(Notenliste!I28)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K30" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6461,7 +6716,7 @@
       </c>
       <c r="N30" s="19" t="str">
         <f>UPPER(Notenliste!K28)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6489,20 +6744,20 @@
         <v>0</v>
       </c>
       <c r="G31" s="18">
-        <f>RAWDATA!I29</f>
+        <f>RAWDATA!K29</f>
         <v>0</v>
       </c>
       <c r="H31" s="19">
-        <f>RAWDATA!J29</f>
+        <f>RAWDATA!L29</f>
         <v>0</v>
       </c>
       <c r="I31" s="19">
-        <f>RAWDATA!K29</f>
+        <f>RAWDATA!M29</f>
         <v>0</v>
       </c>
       <c r="J31" s="17" t="str">
         <f>UPPER(Notenliste!I29)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K31" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6518,7 +6773,7 @@
       </c>
       <c r="N31" s="19" t="str">
         <f>UPPER(Notenliste!K29)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:14" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6546,20 +6801,20 @@
         <v>0</v>
       </c>
       <c r="G32" s="18">
-        <f>RAWDATA!I30</f>
+        <f>RAWDATA!K30</f>
         <v>0</v>
       </c>
       <c r="H32" s="19">
-        <f>RAWDATA!J30</f>
+        <f>RAWDATA!L30</f>
         <v>0</v>
       </c>
       <c r="I32" s="19">
-        <f>RAWDATA!K30</f>
+        <f>RAWDATA!M30</f>
         <v>0</v>
       </c>
       <c r="J32" s="17" t="str">
         <f>UPPER(Notenliste!I30)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K32" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6575,7 +6830,7 @@
       </c>
       <c r="N32" s="19" t="str">
         <f>UPPER(Notenliste!K30)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6603,20 +6858,20 @@
         <v>0</v>
       </c>
       <c r="G33" s="18">
-        <f>RAWDATA!I31</f>
+        <f>RAWDATA!K31</f>
         <v>0</v>
       </c>
       <c r="H33" s="19">
-        <f>RAWDATA!J31</f>
+        <f>RAWDATA!L31</f>
         <v>0</v>
       </c>
       <c r="I33" s="19">
-        <f>RAWDATA!K31</f>
+        <f>RAWDATA!M31</f>
         <v>0</v>
       </c>
       <c r="J33" s="17" t="str">
         <f>UPPER(Notenliste!I31)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K33" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6632,7 +6887,7 @@
       </c>
       <c r="N33" s="19" t="str">
         <f>UPPER(Notenliste!K31)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6660,20 +6915,20 @@
         <v>0</v>
       </c>
       <c r="G34" s="18">
-        <f>RAWDATA!I32</f>
+        <f>RAWDATA!K32</f>
         <v>0</v>
       </c>
       <c r="H34" s="19">
-        <f>RAWDATA!J32</f>
+        <f>RAWDATA!L32</f>
         <v>0</v>
       </c>
       <c r="I34" s="19">
-        <f>RAWDATA!K32</f>
+        <f>RAWDATA!M32</f>
         <v>0</v>
       </c>
       <c r="J34" s="17" t="str">
         <f>UPPER(Notenliste!I32)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K34" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6689,7 +6944,7 @@
       </c>
       <c r="N34" s="19" t="str">
         <f>UPPER(Notenliste!K32)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6717,20 +6972,20 @@
         <v>0</v>
       </c>
       <c r="G35" s="18">
-        <f>RAWDATA!I33</f>
+        <f>RAWDATA!K33</f>
         <v>0</v>
       </c>
       <c r="H35" s="19">
-        <f>RAWDATA!J33</f>
+        <f>RAWDATA!L33</f>
         <v>0</v>
       </c>
       <c r="I35" s="19">
-        <f>RAWDATA!K33</f>
+        <f>RAWDATA!M33</f>
         <v>0</v>
       </c>
       <c r="J35" s="17" t="str">
         <f>UPPER(Notenliste!I33)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K35" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6746,7 +7001,7 @@
       </c>
       <c r="N35" s="19" t="str">
         <f>UPPER(Notenliste!K33)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6774,20 +7029,20 @@
         <v>0</v>
       </c>
       <c r="G36" s="18">
-        <f>RAWDATA!I34</f>
+        <f>RAWDATA!K34</f>
         <v>0</v>
       </c>
       <c r="H36" s="19">
-        <f>RAWDATA!J34</f>
+        <f>RAWDATA!L34</f>
         <v>0</v>
       </c>
       <c r="I36" s="19">
-        <f>RAWDATA!K34</f>
+        <f>RAWDATA!M34</f>
         <v>0</v>
       </c>
       <c r="J36" s="17" t="str">
         <f>UPPER(Notenliste!I34)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K36" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6803,7 +7058,7 @@
       </c>
       <c r="N36" s="19" t="str">
         <f>UPPER(Notenliste!K34)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6831,20 +7086,20 @@
         <v>0</v>
       </c>
       <c r="G37" s="18">
-        <f>RAWDATA!I35</f>
+        <f>RAWDATA!K35</f>
         <v>0</v>
       </c>
       <c r="H37" s="19">
-        <f>RAWDATA!J35</f>
+        <f>RAWDATA!L35</f>
         <v>0</v>
       </c>
       <c r="I37" s="19">
-        <f>RAWDATA!K35</f>
+        <f>RAWDATA!M35</f>
         <v>0</v>
       </c>
       <c r="J37" s="17" t="str">
         <f>UPPER(Notenliste!I35)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K37" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6860,7 +7115,7 @@
       </c>
       <c r="N37" s="19" t="str">
         <f>UPPER(Notenliste!K35)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6888,20 +7143,20 @@
         <v>0</v>
       </c>
       <c r="G38" s="18">
-        <f>RAWDATA!I36</f>
+        <f>RAWDATA!K36</f>
         <v>0</v>
       </c>
       <c r="H38" s="19">
-        <f>RAWDATA!J36</f>
+        <f>RAWDATA!L36</f>
         <v>0</v>
       </c>
       <c r="I38" s="19">
-        <f>RAWDATA!K36</f>
+        <f>RAWDATA!M36</f>
         <v>0</v>
       </c>
       <c r="J38" s="17" t="str">
         <f>UPPER(Notenliste!I36)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="K38" s="17" t="str">
         <f t="shared" si="0"/>
@@ -6917,7 +7172,7 @@
       </c>
       <c r="N38" s="19" t="str">
         <f>UPPER(Notenliste!K36)</f>
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
@@ -6943,86 +7198,86 @@
       <c r="N39" s="57"/>
     </row>
     <row r="40" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="72" t="s">
+      <c r="A40" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="72"/>
-      <c r="C40" s="72"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="72"/>
-      <c r="F40" s="72"/>
-      <c r="G40" s="72"/>
-      <c r="H40" s="72"/>
-      <c r="I40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="K40" s="72"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="72"/>
-      <c r="N40" s="72"/>
+      <c r="B40" s="73"/>
+      <c r="C40" s="73"/>
+      <c r="D40" s="73"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="73"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="73"/>
     </row>
     <row r="41" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="72"/>
-      <c r="B41" s="72"/>
-      <c r="C41" s="72"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="72"/>
-      <c r="F41" s="72"/>
-      <c r="G41" s="72"/>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="72"/>
-      <c r="K41" s="72"/>
-      <c r="L41" s="72"/>
-      <c r="M41" s="72"/>
-      <c r="N41" s="72"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="73"/>
+      <c r="C41" s="73"/>
+      <c r="D41" s="73"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="73"/>
+      <c r="J41" s="73"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="73"/>
+      <c r="M41" s="73"/>
+      <c r="N41" s="73"/>
     </row>
     <row r="42" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="72"/>
-      <c r="B42" s="72"/>
-      <c r="C42" s="72"/>
-      <c r="D42" s="72"/>
-      <c r="E42" s="72"/>
-      <c r="F42" s="72"/>
-      <c r="G42" s="72"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="72"/>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
-      <c r="M42" s="72"/>
-      <c r="N42" s="72"/>
+      <c r="A42" s="73"/>
+      <c r="B42" s="73"/>
+      <c r="C42" s="73"/>
+      <c r="D42" s="73"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
+      <c r="I42" s="73"/>
+      <c r="J42" s="73"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="73"/>
+      <c r="M42" s="73"/>
+      <c r="N42" s="73"/>
     </row>
     <row r="43" spans="1:15" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="72"/>
-      <c r="B43" s="72"/>
-      <c r="C43" s="72"/>
-      <c r="D43" s="72"/>
-      <c r="E43" s="72"/>
-      <c r="F43" s="72"/>
-      <c r="G43" s="72"/>
-      <c r="H43" s="72"/>
-      <c r="I43" s="72"/>
-      <c r="J43" s="72"/>
-      <c r="K43" s="72"/>
-      <c r="L43" s="72"/>
-      <c r="M43" s="72"/>
-      <c r="N43" s="72"/>
+      <c r="A43" s="73"/>
+      <c r="B43" s="73"/>
+      <c r="C43" s="73"/>
+      <c r="D43" s="73"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="73"/>
+      <c r="I43" s="73"/>
+      <c r="J43" s="73"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="73"/>
+      <c r="M43" s="73"/>
+      <c r="N43" s="73"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A44" s="72"/>
-      <c r="B44" s="72"/>
-      <c r="C44" s="72"/>
-      <c r="D44" s="72"/>
-      <c r="E44" s="72"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="72"/>
-      <c r="H44" s="72"/>
-      <c r="I44" s="72"/>
-      <c r="J44" s="72"/>
-      <c r="K44" s="72"/>
-      <c r="L44" s="72"/>
-      <c r="M44" s="72"/>
-      <c r="N44" s="72"/>
+      <c r="A44" s="73"/>
+      <c r="B44" s="73"/>
+      <c r="C44" s="73"/>
+      <c r="D44" s="73"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
+      <c r="I44" s="73"/>
+      <c r="J44" s="73"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="73"/>
+      <c r="M44" s="73"/>
+      <c r="N44" s="73"/>
       <c r="O44" s="58"/>
     </row>
   </sheetData>
@@ -7072,105 +7327,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="str">
+      <c r="A1" s="76" t="str">
         <f>Notenliste!B44&amp;Notenliste!B45</f>
         <v>course.namecourse.alternative</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
     </row>
     <row r="2" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75"/>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="76"/>
+      <c r="N2" s="76"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="76"/>
+      <c r="Q2" s="76"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="76"/>
+      <c r="X2" s="76"/>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="76" t="str">
+      <c r="A3" s="77" t="str">
         <f>"Dozent/in: "&amp;Notenliste!B41</f>
         <v>Dozent/in: course.teacher_name</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
       <c r="F3" s="42"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
-      <c r="P3" s="77"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="77"/>
-      <c r="X3" s="77"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
+      <c r="P3" s="78"/>
+      <c r="Q3" s="78"/>
+      <c r="R3" s="78"/>
+      <c r="S3" s="78"/>
+      <c r="T3" s="78"/>
+      <c r="U3" s="78"/>
+      <c r="V3" s="78"/>
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
     </row>
     <row r="4" spans="1:24" s="16" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="79" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="79" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="E4" s="81" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="43"/>
@@ -7189,22 +7444,22 @@
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
       <c r="U4" s="45"/>
-      <c r="V4" s="82" t="s">
+      <c r="V4" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="W4" s="73" t="s">
+      <c r="W4" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="X4" s="73" t="s">
+      <c r="X4" s="74" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:24" s="16" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="81"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="82"/>
       <c r="F5" s="46"/>
       <c r="G5" s="44">
         <v>1</v>
@@ -7249,9 +7504,9 @@
         <v>14</v>
       </c>
       <c r="U5" s="47"/>
-      <c r="V5" s="83"/>
-      <c r="W5" s="74"/>
-      <c r="X5" s="74"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="75"/>
+      <c r="X5" s="75"/>
     </row>
     <row r="6" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="17">

</xml_diff>